<commit_message>
implement more skills; add some animation; state-skill framework has been set up; bug fix.
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="510" windowWidth="9705" windowHeight="3000" tabRatio="423"/>
+    <workbookView xWindow="-75" yWindow="510" windowWidth="9705" windowHeight="3000" tabRatio="423" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="装备性能表" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="金钱经验表" sheetId="5" r:id="rId4"/>
     <sheet name="游戏公式" sheetId="7" r:id="rId5"/>
     <sheet name="套装表" sheetId="6" r:id="rId6"/>
+    <sheet name="技能-状态列表" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="3">金钱经验表!$A$1:$AK$28</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="406">
   <si>
     <t>武器等级</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1496,6 +1497,157 @@
     <t>最大HP增加倍数</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>技能编号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能名称</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能效果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能种类</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能动画</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现类</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>锁定技</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使角色的攻击随机值总是取最大值</t>
+  </si>
+  <si>
+    <t>重生</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色死亡时有30%机会满血复活</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>疾风</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发技</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次攻击会提升5%攻击速度,持续5秒，可叠加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>反击</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>致死</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色攻击时若攻击、防御、力量、敏捷均大于对方，有10%几率致死</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>假死</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>当一次攻击可以杀死自己时，有50%几率避免此次攻击</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不屈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击提升百分比为失去生命百分比的50%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>虚弱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击时50%几率造成虚弱，持续5秒，对方物理伤害和攻击减少20%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>威慑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色力量大于对方时，对方物理伤害减少10%；角色敏捷大于对方时，对方防御减少10%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>激昂</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色攻击速度提升20%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>顽强</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命恢复速度提升百分比为失去生命百分比的200%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>坚守</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御提升百分比为失去生命百分比的25%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂暴</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>嗜血</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击速度和物理伤害提升百分比为失去生命百分比的25%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御力减少50%；暴击技巧提升1000%；暴击威力提升100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰冻</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次攻击会造成冷冻效果；对方攻速减少20%，持续5秒，不可叠加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次受到攻击有20%几率进行一次反击，不能触发效果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1510,7 +1662,7 @@
     <numFmt numFmtId="181" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="182" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1639,6 +1791,39 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4E3F2A"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -2692,7 +2877,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="675">
+  <cellXfs count="680">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4716,6 +4901,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="7" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5031,7 +5231,7 @@
   </sheetPr>
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -36714,4 +36914,340 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" ht="18.75">
+      <c r="B4" s="675" t="s">
+        <v>368</v>
+      </c>
+      <c r="C4" s="675" t="s">
+        <v>369</v>
+      </c>
+      <c r="D4" s="675" t="s">
+        <v>373</v>
+      </c>
+      <c r="E4" s="675" t="s">
+        <v>371</v>
+      </c>
+      <c r="F4" s="675" t="s">
+        <v>370</v>
+      </c>
+      <c r="G4" s="675" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="676">
+        <v>3</v>
+      </c>
+      <c r="C5" s="676" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5" s="676"/>
+      <c r="E5" s="676" t="s">
+        <v>380</v>
+      </c>
+      <c r="F5" s="676" t="s">
+        <v>381</v>
+      </c>
+      <c r="G5" s="676"/>
+    </row>
+    <row r="6" spans="2:7" s="679" customFormat="1">
+      <c r="B6" s="678">
+        <v>4</v>
+      </c>
+      <c r="C6" s="678" t="s">
+        <v>382</v>
+      </c>
+      <c r="D6" s="678"/>
+      <c r="E6" s="678" t="s">
+        <v>380</v>
+      </c>
+      <c r="F6" s="678" t="s">
+        <v>405</v>
+      </c>
+      <c r="G6" s="678"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="676">
+        <v>5</v>
+      </c>
+      <c r="C7" s="676" t="s">
+        <v>383</v>
+      </c>
+      <c r="D7" s="676"/>
+      <c r="E7" s="676" t="s">
+        <v>380</v>
+      </c>
+      <c r="F7" s="676" t="s">
+        <v>384</v>
+      </c>
+      <c r="G7" s="676"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="676">
+        <v>6</v>
+      </c>
+      <c r="C8" s="676" t="s">
+        <v>385</v>
+      </c>
+      <c r="D8" s="676"/>
+      <c r="E8" s="676" t="s">
+        <v>380</v>
+      </c>
+      <c r="F8" s="676" t="s">
+        <v>386</v>
+      </c>
+      <c r="G8" s="676"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="676">
+        <v>8</v>
+      </c>
+      <c r="C9" s="676" t="s">
+        <v>389</v>
+      </c>
+      <c r="D9" s="676"/>
+      <c r="E9" s="676" t="s">
+        <v>380</v>
+      </c>
+      <c r="F9" s="676" t="s">
+        <v>390</v>
+      </c>
+      <c r="G9" s="676"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="676">
+        <v>1</v>
+      </c>
+      <c r="C10" s="676" t="s">
+        <v>374</v>
+      </c>
+      <c r="D10" s="676"/>
+      <c r="E10" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F10" s="677" t="s">
+        <v>376</v>
+      </c>
+      <c r="G10" s="676"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="676">
+        <v>2</v>
+      </c>
+      <c r="C11" s="676" t="s">
+        <v>377</v>
+      </c>
+      <c r="D11" s="676"/>
+      <c r="E11" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F11" s="676" t="s">
+        <v>378</v>
+      </c>
+      <c r="G11" s="676"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="676">
+        <v>7</v>
+      </c>
+      <c r="C12" s="676" t="s">
+        <v>387</v>
+      </c>
+      <c r="D12" s="676"/>
+      <c r="E12" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F12" s="676" t="s">
+        <v>388</v>
+      </c>
+      <c r="G12" s="676"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="676">
+        <v>9</v>
+      </c>
+      <c r="C13" s="676" t="s">
+        <v>391</v>
+      </c>
+      <c r="D13" s="676"/>
+      <c r="E13" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F13" s="676" t="s">
+        <v>392</v>
+      </c>
+      <c r="G13" s="676"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="676">
+        <v>10</v>
+      </c>
+      <c r="C14" s="676" t="s">
+        <v>393</v>
+      </c>
+      <c r="D14" s="676"/>
+      <c r="E14" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F14" s="676" t="s">
+        <v>394</v>
+      </c>
+      <c r="G14" s="676"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="676">
+        <v>11</v>
+      </c>
+      <c r="C15" s="676" t="s">
+        <v>395</v>
+      </c>
+      <c r="D15" s="676"/>
+      <c r="E15" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F15" s="676" t="s">
+        <v>396</v>
+      </c>
+      <c r="G15" s="676"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="676">
+        <v>12</v>
+      </c>
+      <c r="C16" s="676" t="s">
+        <v>397</v>
+      </c>
+      <c r="D16" s="676"/>
+      <c r="E16" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F16" s="676" t="s">
+        <v>398</v>
+      </c>
+      <c r="G16" s="676"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="676">
+        <v>13</v>
+      </c>
+      <c r="C17" s="676" t="s">
+        <v>400</v>
+      </c>
+      <c r="D17" s="676"/>
+      <c r="E17" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F17" s="676" t="s">
+        <v>401</v>
+      </c>
+      <c r="G17" s="676"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="676">
+        <v>14</v>
+      </c>
+      <c r="C18" s="676" t="s">
+        <v>399</v>
+      </c>
+      <c r="D18" s="676"/>
+      <c r="E18" s="676" t="s">
+        <v>375</v>
+      </c>
+      <c r="F18" s="676" t="s">
+        <v>402</v>
+      </c>
+      <c r="G18" s="676"/>
+    </row>
+    <row r="19" spans="2:7" s="679" customFormat="1">
+      <c r="B19" s="678">
+        <v>15</v>
+      </c>
+      <c r="C19" s="678" t="s">
+        <v>403</v>
+      </c>
+      <c r="D19" s="678"/>
+      <c r="E19" s="678" t="s">
+        <v>380</v>
+      </c>
+      <c r="F19" s="678" t="s">
+        <v>404</v>
+      </c>
+      <c r="G19" s="678"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="676"/>
+      <c r="C20" s="676"/>
+      <c r="D20" s="676"/>
+      <c r="E20" s="676"/>
+      <c r="F20" s="676"/>
+      <c r="G20" s="676"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="676"/>
+      <c r="C21" s="676"/>
+      <c r="D21" s="676"/>
+      <c r="E21" s="676"/>
+      <c r="F21" s="676"/>
+      <c r="G21" s="676"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="676"/>
+      <c r="C22" s="676"/>
+      <c r="D22" s="676"/>
+      <c r="E22" s="676"/>
+      <c r="F22" s="676"/>
+      <c r="G22" s="676"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="676"/>
+      <c r="C23" s="676"/>
+      <c r="D23" s="676"/>
+      <c r="E23" s="676"/>
+      <c r="F23" s="676"/>
+      <c r="G23" s="676"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="676"/>
+      <c r="C24" s="676"/>
+      <c r="D24" s="676"/>
+      <c r="E24" s="676"/>
+      <c r="F24" s="676"/>
+      <c r="G24" s="676"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="676"/>
+      <c r="C25" s="676"/>
+      <c r="D25" s="676"/>
+      <c r="E25" s="676"/>
+      <c r="F25" s="676"/>
+      <c r="G25" s="676"/>
+    </row>
+  </sheetData>
+  <sortState ref="B5:G14">
+    <sortCondition ref="E5"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add a few skill icons; implement add/delete skills; fix some bugs;
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="448">
   <si>
     <t>武器等级</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1533,14 +1533,6 @@
     <t>使角色的攻击随机值总是取最大值</t>
   </si>
   <si>
-    <t>重生</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色死亡时有30%机会满血复活</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>疾风</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1549,10 +1541,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>角色每次攻击会提升5%攻击速度,持续5秒，可叠加</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>反击</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1561,18 +1549,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>角色攻击时若攻击、防御、力量、敏捷均大于对方，有10%几率致死</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>假死</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>当一次攻击可以杀死自己时，有50%几率避免此次攻击</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>不屈</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1593,10 +1573,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>角色力量大于对方时，对方物理伤害减少10%；角色敏捷大于对方时，对方防御减少10%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>激昂</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1609,18 +1585,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>生命恢复速度提升百分比为失去生命百分比的200%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>坚守</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>防御提升百分比为失去生命百分比的25%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>狂暴</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1633,19 +1601,224 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>防御力减少50%；暴击技巧提升1000%；暴击威力提升100%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>冰冻</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>角色每次攻击会造成冷冻效果；对方攻速减少20%，持续5秒，不可叠加</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色每次受到攻击有20%几率进行一次反击，不能触发效果</t>
+    <t>角色攻击时若攻击、防御、力量、敏捷、物理伤害均大于对方，有15%几率致死</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>当一次攻击可以杀死自己时，有50%几率避免此次攻击造成的伤害</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>疾风II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发技</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>疾风III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>反转</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>若角色力量小于对方则物理伤害、生命恢复增加百分比为两者力量差百分比的200%；
+若角色敏捷小于对方则攻击速度、防御力增加百分比为两者敏捷差百分比的200%。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不屈II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击提升百分比为失去生命百分比的100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不屈III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击提升百分比为失去生命百分比的200%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>激昂II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色攻击速度提升40%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>顽强II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命恢复速度提升百分比为失去生命百分比的150%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命恢复速度提升百分比为失去生命百分比的300%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>顽强III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命恢复速度提升百分比为失去生命百分比的600%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>坚守II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>坚守III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>反击II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>反击III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>威慑II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色力量大于对方时，对方防御减少20%；
+角色敏捷大于对方时，对方物理伤害减少20%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>威慑III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色力量大于对方时，攻击速度和防御减少30%；
+角色敏捷大于对方时，物理伤害和生命恢复减少30%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色力量大于对方时，闪避技巧、攻击速度和防御减少40%；
+角色敏捷大于对方时，命中技巧、物理伤害和生命恢复减少40%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂暴II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御力减少20%；暴击技巧提升1000%；暴击威力提升100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御力减少40%；攻速提升50%；暴击技巧提升1000%；暴击威力提升100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂暴III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御力减少60%；闪避技巧提升100%；攻速提升100%；暴击技巧提升1000%；暴击威力提升100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂暴IV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御力减少80%；
+命中技巧提升100%；闪避技巧提升100%；攻速提升100%；暴击技巧提升1000%；暴击威力提升100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰冻II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰冻III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少40%，持续7秒，不可叠加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次攻击被闪避时攻速提升20%，命中提升100%，持续10秒，不可叠加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次受到攻击有30%几率进行一次反击，不能触发效果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次受到攻击有60%几率进行一次反击，不能触发效果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次受到攻击有100%几率进行一次反击，不能触发效果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次攻击被闪避时攻速提升40%，命中提升200%，持续15秒，不可叠加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次攻击被闪避时攻速提升80%，命中提升300%，持续30秒，不可叠加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使角色的攻击随机值总是取最大值，且总是暴击，且对方闪避有50%几率失效</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使角色的攻击随机值总是取最大值且至少有50%几率暴击</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色攻击速度提升100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御提升百分比为失去生命百分比的100%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御提升百分比为失去生命百分比的50%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御提升百分比为失去生命百分比的200%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少20%，持续5秒，不可叠加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少80%，持续15秒，不可叠加</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1662,7 +1835,7 @@
     <numFmt numFmtId="181" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="182" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1793,22 +1966,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4E3F2A"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -1820,6 +1977,62 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -2877,7 +3090,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="680">
+  <cellXfs count="687">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4903,19 +5116,40 @@
     <xf numFmtId="178" fontId="7" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -36918,10 +37152,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:G25"/>
+  <dimension ref="A4:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -36930,7 +37164,7 @@
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -36954,293 +37188,625 @@
         <v>372</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="676">
+    <row r="5" spans="2:7" ht="14.25">
+      <c r="B5" s="680">
+        <v>1</v>
+      </c>
+      <c r="C5" s="680" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5" s="680"/>
+      <c r="E5" s="680" t="s">
+        <v>378</v>
+      </c>
+      <c r="F5" s="680" t="s">
+        <v>434</v>
+      </c>
+      <c r="G5" s="680"/>
+    </row>
+    <row r="6" spans="2:7" ht="14.25">
+      <c r="B6" s="680">
+        <v>2</v>
+      </c>
+      <c r="C6" s="680" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6" s="680"/>
+      <c r="E6" s="680" t="s">
+        <v>398</v>
+      </c>
+      <c r="F6" s="680" t="s">
+        <v>438</v>
+      </c>
+      <c r="G6" s="680"/>
+    </row>
+    <row r="7" spans="2:7" ht="14.25">
+      <c r="B7" s="680">
         <v>3</v>
       </c>
-      <c r="C5" s="676" t="s">
+      <c r="C7" s="680" t="s">
+        <v>399</v>
+      </c>
+      <c r="D7" s="680"/>
+      <c r="E7" s="680" t="s">
+        <v>398</v>
+      </c>
+      <c r="F7" s="680" t="s">
+        <v>439</v>
+      </c>
+      <c r="G7" s="680"/>
+    </row>
+    <row r="8" spans="2:7" s="677" customFormat="1" ht="14.25">
+      <c r="B8" s="681">
+        <v>4</v>
+      </c>
+      <c r="C8" s="681" t="s">
         <v>379</v>
       </c>
-      <c r="D5" s="676"/>
-      <c r="E5" s="676" t="s">
+      <c r="D8" s="681"/>
+      <c r="E8" s="681" t="s">
+        <v>378</v>
+      </c>
+      <c r="F8" s="681" t="s">
+        <v>435</v>
+      </c>
+      <c r="G8" s="681"/>
+    </row>
+    <row r="9" spans="2:7" s="679" customFormat="1" ht="14.25">
+      <c r="B9" s="680">
+        <v>5</v>
+      </c>
+      <c r="C9" s="682" t="s">
+        <v>417</v>
+      </c>
+      <c r="D9" s="682"/>
+      <c r="E9" s="682" t="s">
+        <v>378</v>
+      </c>
+      <c r="F9" s="682" t="s">
+        <v>436</v>
+      </c>
+      <c r="G9" s="682"/>
+    </row>
+    <row r="10" spans="2:7" s="679" customFormat="1" ht="14.25">
+      <c r="B10" s="680">
+        <v>6</v>
+      </c>
+      <c r="C10" s="682" t="s">
+        <v>418</v>
+      </c>
+      <c r="D10" s="682"/>
+      <c r="E10" s="682" t="s">
+        <v>378</v>
+      </c>
+      <c r="F10" s="682" t="s">
+        <v>437</v>
+      </c>
+      <c r="G10" s="682"/>
+    </row>
+    <row r="11" spans="2:7" ht="14.25">
+      <c r="B11" s="680">
+        <v>7</v>
+      </c>
+      <c r="C11" s="680" t="s">
         <v>380</v>
       </c>
-      <c r="F5" s="676" t="s">
+      <c r="D11" s="680"/>
+      <c r="E11" s="680" t="s">
+        <v>378</v>
+      </c>
+      <c r="F11" s="680" t="s">
+        <v>395</v>
+      </c>
+      <c r="G11" s="680"/>
+    </row>
+    <row r="12" spans="2:7" ht="14.25">
+      <c r="B12" s="680">
+        <v>8</v>
+      </c>
+      <c r="C12" s="680" t="s">
         <v>381</v>
       </c>
-      <c r="G5" s="676"/>
-    </row>
-    <row r="6" spans="2:7" s="679" customFormat="1">
-      <c r="B6" s="678">
-        <v>4</v>
-      </c>
-      <c r="C6" s="678" t="s">
+      <c r="D12" s="680"/>
+      <c r="E12" s="680" t="s">
+        <v>378</v>
+      </c>
+      <c r="F12" s="680" t="s">
+        <v>396</v>
+      </c>
+      <c r="G12" s="680"/>
+    </row>
+    <row r="13" spans="2:7" ht="14.25">
+      <c r="B13" s="680">
+        <v>9</v>
+      </c>
+      <c r="C13" s="680" t="s">
+        <v>384</v>
+      </c>
+      <c r="D13" s="680"/>
+      <c r="E13" s="680" t="s">
+        <v>378</v>
+      </c>
+      <c r="F13" s="680" t="s">
+        <v>385</v>
+      </c>
+      <c r="G13" s="680"/>
+    </row>
+    <row r="14" spans="2:7" s="686" customFormat="1" ht="14.25">
+      <c r="B14" s="680">
+        <v>10</v>
+      </c>
+      <c r="C14" s="685" t="s">
+        <v>374</v>
+      </c>
+      <c r="D14" s="685"/>
+      <c r="E14" s="685" t="s">
+        <v>375</v>
+      </c>
+      <c r="F14" s="685" t="s">
+        <v>376</v>
+      </c>
+      <c r="G14" s="685"/>
+    </row>
+    <row r="15" spans="2:7" s="686" customFormat="1" ht="14.25">
+      <c r="B15" s="680">
+        <v>11</v>
+      </c>
+      <c r="C15" s="685" t="s">
+        <v>400</v>
+      </c>
+      <c r="D15" s="685"/>
+      <c r="E15" s="685" t="s">
+        <v>375</v>
+      </c>
+      <c r="F15" s="685" t="s">
+        <v>441</v>
+      </c>
+      <c r="G15" s="685"/>
+    </row>
+    <row r="16" spans="2:7" s="686" customFormat="1" ht="14.25">
+      <c r="B16" s="680">
+        <v>12</v>
+      </c>
+      <c r="C16" s="685" t="s">
+        <v>401</v>
+      </c>
+      <c r="D16" s="685"/>
+      <c r="E16" s="685" t="s">
+        <v>375</v>
+      </c>
+      <c r="F16" s="685" t="s">
+        <v>440</v>
+      </c>
+      <c r="G16" s="685"/>
+    </row>
+    <row r="17" spans="1:10" s="678" customFormat="1" ht="28.5">
+      <c r="A17" s="679"/>
+      <c r="B17" s="680">
+        <v>13</v>
+      </c>
+      <c r="C17" s="682" t="s">
+        <v>402</v>
+      </c>
+      <c r="D17" s="682"/>
+      <c r="E17" s="682" t="s">
+        <v>375</v>
+      </c>
+      <c r="F17" s="683" t="s">
+        <v>403</v>
+      </c>
+      <c r="G17" s="682"/>
+      <c r="H17" s="679"/>
+      <c r="I17" s="679"/>
+      <c r="J17" s="679"/>
+    </row>
+    <row r="18" spans="1:10" ht="14.25">
+      <c r="B18" s="680">
+        <v>14</v>
+      </c>
+      <c r="C18" s="680" t="s">
         <v>382</v>
       </c>
-      <c r="D6" s="678"/>
-      <c r="E6" s="678" t="s">
-        <v>380</v>
-      </c>
-      <c r="F6" s="678" t="s">
+      <c r="D18" s="680"/>
+      <c r="E18" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F18" s="680" t="s">
+        <v>383</v>
+      </c>
+      <c r="G18" s="680"/>
+    </row>
+    <row r="19" spans="1:10" ht="14.25">
+      <c r="B19" s="680">
+        <v>15</v>
+      </c>
+      <c r="C19" s="680" t="s">
+        <v>404</v>
+      </c>
+      <c r="D19" s="680"/>
+      <c r="E19" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F19" s="680" t="s">
         <v>405</v>
       </c>
-      <c r="G6" s="678"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="676">
-        <v>5</v>
-      </c>
-      <c r="C7" s="676" t="s">
-        <v>383</v>
-      </c>
-      <c r="D7" s="676"/>
-      <c r="E7" s="676" t="s">
-        <v>380</v>
-      </c>
-      <c r="F7" s="676" t="s">
-        <v>384</v>
-      </c>
-      <c r="G7" s="676"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="676">
-        <v>6</v>
-      </c>
-      <c r="C8" s="676" t="s">
-        <v>385</v>
-      </c>
-      <c r="D8" s="676"/>
-      <c r="E8" s="676" t="s">
-        <v>380</v>
-      </c>
-      <c r="F8" s="676" t="s">
+      <c r="G19" s="680"/>
+    </row>
+    <row r="20" spans="1:10" ht="14.25">
+      <c r="B20" s="680">
+        <v>16</v>
+      </c>
+      <c r="C20" s="680" t="s">
+        <v>406</v>
+      </c>
+      <c r="D20" s="680"/>
+      <c r="E20" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F20" s="680" t="s">
+        <v>407</v>
+      </c>
+      <c r="G20" s="680"/>
+    </row>
+    <row r="21" spans="1:10" ht="28.5">
+      <c r="B21" s="680">
+        <v>17</v>
+      </c>
+      <c r="C21" s="680" t="s">
         <v>386</v>
       </c>
-      <c r="G8" s="676"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="676">
-        <v>8</v>
-      </c>
-      <c r="C9" s="676" t="s">
+      <c r="D21" s="680"/>
+      <c r="E21" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F21" s="684" t="s">
+        <v>420</v>
+      </c>
+      <c r="G21" s="680"/>
+    </row>
+    <row r="22" spans="1:10" ht="28.5">
+      <c r="B22" s="680">
+        <v>18</v>
+      </c>
+      <c r="C22" s="680" t="s">
+        <v>419</v>
+      </c>
+      <c r="D22" s="680"/>
+      <c r="E22" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F22" s="684" t="s">
+        <v>422</v>
+      </c>
+      <c r="G22" s="680"/>
+    </row>
+    <row r="23" spans="1:10" ht="28.5">
+      <c r="B23" s="680">
+        <v>19</v>
+      </c>
+      <c r="C23" s="680" t="s">
+        <v>421</v>
+      </c>
+      <c r="D23" s="680"/>
+      <c r="E23" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F23" s="684" t="s">
+        <v>423</v>
+      </c>
+      <c r="G23" s="680"/>
+    </row>
+    <row r="24" spans="1:10" ht="14.25">
+      <c r="B24" s="680">
+        <v>20</v>
+      </c>
+      <c r="C24" s="680" t="s">
+        <v>387</v>
+      </c>
+      <c r="D24" s="680"/>
+      <c r="E24" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F24" s="680" t="s">
+        <v>388</v>
+      </c>
+      <c r="G24" s="680"/>
+    </row>
+    <row r="25" spans="1:10" ht="14.25">
+      <c r="B25" s="680">
+        <v>21</v>
+      </c>
+      <c r="C25" s="680" t="s">
+        <v>408</v>
+      </c>
+      <c r="D25" s="680"/>
+      <c r="E25" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F25" s="680" t="s">
+        <v>409</v>
+      </c>
+      <c r="G25" s="680"/>
+    </row>
+    <row r="26" spans="1:10" ht="14.25">
+      <c r="B26" s="680">
+        <v>22</v>
+      </c>
+      <c r="C26" s="680" t="s">
+        <v>408</v>
+      </c>
+      <c r="D26" s="680"/>
+      <c r="E26" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F26" s="680" t="s">
+        <v>442</v>
+      </c>
+      <c r="G26" s="680"/>
+    </row>
+    <row r="27" spans="1:10" ht="14.25">
+      <c r="B27" s="680">
+        <v>23</v>
+      </c>
+      <c r="C27" s="680" t="s">
         <v>389</v>
       </c>
-      <c r="D9" s="676"/>
-      <c r="E9" s="676" t="s">
-        <v>380</v>
-      </c>
-      <c r="F9" s="676" t="s">
+      <c r="D27" s="680"/>
+      <c r="E27" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F27" s="680" t="s">
+        <v>411</v>
+      </c>
+      <c r="G27" s="680"/>
+    </row>
+    <row r="28" spans="1:10" ht="14.25">
+      <c r="B28" s="680">
+        <v>24</v>
+      </c>
+      <c r="C28" s="680" t="s">
+        <v>410</v>
+      </c>
+      <c r="D28" s="680"/>
+      <c r="E28" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F28" s="680" t="s">
+        <v>412</v>
+      </c>
+      <c r="G28" s="680"/>
+    </row>
+    <row r="29" spans="1:10" ht="14.25">
+      <c r="B29" s="680">
+        <v>25</v>
+      </c>
+      <c r="C29" s="680" t="s">
+        <v>413</v>
+      </c>
+      <c r="D29" s="680"/>
+      <c r="E29" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F29" s="680" t="s">
+        <v>414</v>
+      </c>
+      <c r="G29" s="680"/>
+    </row>
+    <row r="30" spans="1:10" s="677" customFormat="1" ht="14.25">
+      <c r="B30" s="681">
+        <v>26</v>
+      </c>
+      <c r="C30" s="681" t="s">
         <v>390</v>
       </c>
-      <c r="G9" s="676"/>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="676">
-        <v>1</v>
-      </c>
-      <c r="C10" s="676" t="s">
-        <v>374</v>
-      </c>
-      <c r="D10" s="676"/>
-      <c r="E10" s="676" t="s">
+      <c r="D30" s="681"/>
+      <c r="E30" s="681" t="s">
         <v>375</v>
       </c>
-      <c r="F10" s="677" t="s">
-        <v>376</v>
-      </c>
-      <c r="G10" s="676"/>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="676">
-        <v>2</v>
-      </c>
-      <c r="C11" s="676" t="s">
-        <v>377</v>
-      </c>
-      <c r="D11" s="676"/>
-      <c r="E11" s="676" t="s">
+      <c r="F30" s="681" t="s">
+        <v>444</v>
+      </c>
+      <c r="G30" s="681"/>
+    </row>
+    <row r="31" spans="1:10" s="679" customFormat="1" ht="14.25">
+      <c r="B31" s="680">
+        <v>27</v>
+      </c>
+      <c r="C31" s="682" t="s">
+        <v>415</v>
+      </c>
+      <c r="D31" s="682"/>
+      <c r="E31" s="682" t="s">
         <v>375</v>
       </c>
-      <c r="F11" s="676" t="s">
+      <c r="F31" s="682" t="s">
+        <v>443</v>
+      </c>
+      <c r="G31" s="682"/>
+    </row>
+    <row r="32" spans="1:10" s="679" customFormat="1" ht="14.25">
+      <c r="B32" s="680">
+        <v>28</v>
+      </c>
+      <c r="C32" s="682" t="s">
+        <v>416</v>
+      </c>
+      <c r="D32" s="682"/>
+      <c r="E32" s="682" t="s">
+        <v>375</v>
+      </c>
+      <c r="F32" s="682" t="s">
+        <v>445</v>
+      </c>
+      <c r="G32" s="682"/>
+    </row>
+    <row r="33" spans="2:7" ht="14.25">
+      <c r="B33" s="680">
+        <v>29</v>
+      </c>
+      <c r="C33" s="680" t="s">
+        <v>392</v>
+      </c>
+      <c r="D33" s="680"/>
+      <c r="E33" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F33" s="680" t="s">
+        <v>393</v>
+      </c>
+      <c r="G33" s="680"/>
+    </row>
+    <row r="34" spans="2:7" ht="14.25">
+      <c r="B34" s="680">
+        <v>30</v>
+      </c>
+      <c r="C34" s="680" t="s">
+        <v>391</v>
+      </c>
+      <c r="D34" s="680"/>
+      <c r="E34" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F34" s="680" t="s">
+        <v>425</v>
+      </c>
+      <c r="G34" s="680"/>
+    </row>
+    <row r="35" spans="2:7" ht="14.25">
+      <c r="B35" s="680">
+        <v>31</v>
+      </c>
+      <c r="C35" s="680" t="s">
+        <v>424</v>
+      </c>
+      <c r="D35" s="680"/>
+      <c r="E35" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F35" s="680" t="s">
+        <v>426</v>
+      </c>
+      <c r="G35" s="680"/>
+    </row>
+    <row r="36" spans="2:7" ht="14.25">
+      <c r="B36" s="680">
+        <v>32</v>
+      </c>
+      <c r="C36" s="680" t="s">
+        <v>427</v>
+      </c>
+      <c r="D36" s="680"/>
+      <c r="E36" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F36" s="680" t="s">
+        <v>428</v>
+      </c>
+      <c r="G36" s="680"/>
+    </row>
+    <row r="37" spans="2:7" ht="28.5">
+      <c r="B37" s="680">
+        <v>33</v>
+      </c>
+      <c r="C37" s="680" t="s">
+        <v>429</v>
+      </c>
+      <c r="D37" s="680"/>
+      <c r="E37" s="680" t="s">
+        <v>375</v>
+      </c>
+      <c r="F37" s="684" t="s">
+        <v>430</v>
+      </c>
+      <c r="G37" s="680"/>
+    </row>
+    <row r="38" spans="2:7" s="677" customFormat="1" ht="14.25">
+      <c r="B38" s="681">
+        <v>34</v>
+      </c>
+      <c r="C38" s="681" t="s">
+        <v>394</v>
+      </c>
+      <c r="D38" s="681"/>
+      <c r="E38" s="681" t="s">
         <v>378</v>
       </c>
-      <c r="G11" s="676"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="676">
-        <v>7</v>
-      </c>
-      <c r="C12" s="676" t="s">
-        <v>387</v>
-      </c>
-      <c r="D12" s="676"/>
-      <c r="E12" s="676" t="s">
-        <v>375</v>
-      </c>
-      <c r="F12" s="676" t="s">
-        <v>388</v>
-      </c>
-      <c r="G12" s="676"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="676">
-        <v>9</v>
-      </c>
-      <c r="C13" s="676" t="s">
-        <v>391</v>
-      </c>
-      <c r="D13" s="676"/>
-      <c r="E13" s="676" t="s">
-        <v>375</v>
-      </c>
-      <c r="F13" s="676" t="s">
-        <v>392</v>
-      </c>
-      <c r="G13" s="676"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="676">
-        <v>10</v>
-      </c>
-      <c r="C14" s="676" t="s">
-        <v>393</v>
-      </c>
-      <c r="D14" s="676"/>
-      <c r="E14" s="676" t="s">
-        <v>375</v>
-      </c>
-      <c r="F14" s="676" t="s">
-        <v>394</v>
-      </c>
-      <c r="G14" s="676"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="676">
-        <v>11</v>
-      </c>
-      <c r="C15" s="676" t="s">
-        <v>395</v>
-      </c>
-      <c r="D15" s="676"/>
-      <c r="E15" s="676" t="s">
-        <v>375</v>
-      </c>
-      <c r="F15" s="676" t="s">
-        <v>396</v>
-      </c>
-      <c r="G15" s="676"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="676">
-        <v>12</v>
-      </c>
-      <c r="C16" s="676" t="s">
-        <v>397</v>
-      </c>
-      <c r="D16" s="676"/>
-      <c r="E16" s="676" t="s">
-        <v>375</v>
-      </c>
-      <c r="F16" s="676" t="s">
-        <v>398</v>
-      </c>
-      <c r="G16" s="676"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="676">
-        <v>13</v>
-      </c>
-      <c r="C17" s="676" t="s">
-        <v>400</v>
-      </c>
-      <c r="D17" s="676"/>
-      <c r="E17" s="676" t="s">
-        <v>375</v>
-      </c>
-      <c r="F17" s="676" t="s">
-        <v>401</v>
-      </c>
-      <c r="G17" s="676"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="676">
-        <v>14</v>
-      </c>
-      <c r="C18" s="676" t="s">
-        <v>399</v>
-      </c>
-      <c r="D18" s="676"/>
-      <c r="E18" s="676" t="s">
-        <v>375</v>
-      </c>
-      <c r="F18" s="676" t="s">
-        <v>402</v>
-      </c>
-      <c r="G18" s="676"/>
-    </row>
-    <row r="19" spans="2:7" s="679" customFormat="1">
-      <c r="B19" s="678">
-        <v>15</v>
-      </c>
-      <c r="C19" s="678" t="s">
-        <v>403</v>
-      </c>
-      <c r="D19" s="678"/>
-      <c r="E19" s="678" t="s">
-        <v>380</v>
-      </c>
-      <c r="F19" s="678" t="s">
-        <v>404</v>
-      </c>
-      <c r="G19" s="678"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="676"/>
-      <c r="C20" s="676"/>
-      <c r="D20" s="676"/>
-      <c r="E20" s="676"/>
-      <c r="F20" s="676"/>
-      <c r="G20" s="676"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="676"/>
-      <c r="C21" s="676"/>
-      <c r="D21" s="676"/>
-      <c r="E21" s="676"/>
-      <c r="F21" s="676"/>
-      <c r="G21" s="676"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="676"/>
-      <c r="C22" s="676"/>
-      <c r="D22" s="676"/>
-      <c r="E22" s="676"/>
-      <c r="F22" s="676"/>
-      <c r="G22" s="676"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="676"/>
-      <c r="C23" s="676"/>
-      <c r="D23" s="676"/>
-      <c r="E23" s="676"/>
-      <c r="F23" s="676"/>
-      <c r="G23" s="676"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="676"/>
-      <c r="C24" s="676"/>
-      <c r="D24" s="676"/>
-      <c r="E24" s="676"/>
-      <c r="F24" s="676"/>
-      <c r="G24" s="676"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="676"/>
-      <c r="C25" s="676"/>
-      <c r="D25" s="676"/>
-      <c r="E25" s="676"/>
-      <c r="F25" s="676"/>
-      <c r="G25" s="676"/>
+      <c r="F38" s="681" t="s">
+        <v>446</v>
+      </c>
+      <c r="G38" s="681"/>
+    </row>
+    <row r="39" spans="2:7" s="679" customFormat="1" ht="14.25">
+      <c r="B39" s="680">
+        <v>35</v>
+      </c>
+      <c r="C39" s="682" t="s">
+        <v>431</v>
+      </c>
+      <c r="D39" s="682"/>
+      <c r="E39" s="682" t="s">
+        <v>378</v>
+      </c>
+      <c r="F39" s="682" t="s">
+        <v>433</v>
+      </c>
+      <c r="G39" s="682"/>
+    </row>
+    <row r="40" spans="2:7" s="679" customFormat="1" ht="14.25">
+      <c r="B40" s="680">
+        <v>36</v>
+      </c>
+      <c r="C40" s="682" t="s">
+        <v>432</v>
+      </c>
+      <c r="D40" s="682"/>
+      <c r="E40" s="682" t="s">
+        <v>378</v>
+      </c>
+      <c r="F40" s="682" t="s">
+        <v>447</v>
+      </c>
+      <c r="G40" s="682"/>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="676"/>
+      <c r="C41" s="676"/>
+      <c r="D41" s="676"/>
+      <c r="E41" s="676"/>
+      <c r="F41" s="676"/>
+      <c r="G41" s="676"/>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="676"/>
+      <c r="C42" s="676"/>
+      <c r="D42" s="676"/>
+      <c r="E42" s="676"/>
+      <c r="F42" s="676"/>
+      <c r="G42" s="676"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="676"/>
+      <c r="C43" s="676"/>
+      <c r="D43" s="676"/>
+      <c r="E43" s="676"/>
+      <c r="F43" s="676"/>
+      <c r="G43" s="676"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="676"/>
+      <c r="C44" s="676"/>
+      <c r="D44" s="676"/>
+      <c r="E44" s="676"/>
+      <c r="F44" s="676"/>
+      <c r="G44" s="676"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="676"/>
+      <c r="C45" s="676"/>
+      <c r="D45" s="676"/>
+      <c r="E45" s="676"/>
+      <c r="F45" s="676"/>
+      <c r="G45" s="676"/>
     </row>
   </sheetData>
   <sortState ref="B5:G14">

</xml_diff>

<commit_message>
skill shop finish, consult integrate skills. add some skills
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -21,14 +21,14 @@
   </definedNames>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="pm" day="1485848847" val="694"/>
+      <pm:revision xmlns:pm="pm" day="1486346637" val="694"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="466">
   <si>
     <t>武器等级</t>
   </si>
@@ -1152,13 +1152,25 @@
     <t>技能动画</t>
   </si>
   <si>
-    <t>疾风</t>
+    <t>level</t>
+  </si>
+  <si>
+    <t>par1</t>
+  </si>
+  <si>
+    <t>par2</t>
+  </si>
+  <si>
+    <t>par3</t>
+  </si>
+  <si>
+    <t>疾风I</t>
   </si>
   <si>
     <t>触发技</t>
   </si>
   <si>
-    <t>角色每次攻击被闪避时攻速提升20%，命中提升100%，持续10秒，不可叠加</t>
+    <t>角色每次攻击被闪避时攻速提升20%，命中提升100%，持续5秒，不可叠加</t>
   </si>
   <si>
     <t>疾风II</t>
@@ -1167,16 +1179,16 @@
     <t>触发技</t>
   </si>
   <si>
-    <t>角色每次攻击被闪避时攻速提升40%，命中提升200%，持续15秒，不可叠加</t>
+    <t>角色每次攻击被闪避时攻速提升40%，命中提升200%，持续10秒，不可叠加</t>
   </si>
   <si>
     <t>疾风III</t>
   </si>
   <si>
-    <t>角色每次攻击被闪避时攻速提升80%，命中提升300%，持续30秒，不可叠加</t>
-  </si>
-  <si>
-    <t>反击</t>
+    <t>角色每次攻击被闪避时攻速提升80%，命中提升300%，持续20秒，不可叠加</t>
+  </si>
+  <si>
+    <t>反击I</t>
   </si>
   <si>
     <t>角色每次受到攻击有30%几率进行一次反击，不能触发效果</t>
@@ -1312,7 +1324,7 @@
     <t>生命恢复速度提升百分比为失去生命百分比的600%</t>
   </si>
   <si>
-    <t>坚守</t>
+    <t>坚守I</t>
   </si>
   <si>
     <t>防御提升百分比为失去生命百分比的50%</t>
@@ -1361,7 +1373,7 @@
 命中技巧提升100%；闪避技巧提升100%；攻速提升100%；暴击技巧提升1000%；暴击威力提升100%</t>
   </si>
   <si>
-    <t>冰冻</t>
+    <t>冰冻I</t>
   </si>
   <si>
     <t>角色每次攻击命中会造成冷冻效果；对方攻速减少20%，持续5秒，不可叠加</t>
@@ -1383,6 +1395,42 @@
   </si>
   <si>
     <t>角色受到暴击之后立即发动下一次攻击</t>
+  </si>
+  <si>
+    <t>北斗</t>
+  </si>
+  <si>
+    <t>攻速提升百分比为失去生命百分比的50%</t>
+  </si>
+  <si>
+    <t>七星</t>
+  </si>
+  <si>
+    <t>角色每连续攻击七次会恢复当前生命值相当的生命</t>
+  </si>
+  <si>
+    <t>铜头</t>
+  </si>
+  <si>
+    <t>角色不会受到暴击伤害</t>
+  </si>
+  <si>
+    <t>铁壁</t>
+  </si>
+  <si>
+    <t>角色每次攻击必定造成暴击</t>
+  </si>
+  <si>
+    <t>降龙</t>
+  </si>
+  <si>
+    <t>战斗期间敌人基础防御力减少90%</t>
+  </si>
+  <si>
+    <t>伏虎</t>
+  </si>
+  <si>
+    <t>战斗期间敌人基础攻击力减少90%</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1458,7 @@
     <numFmt numFmtId="3" formatCode="#,##0"/>
     <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -1533,6 +1581,12 @@
       <b/>
       <color rgb="FF0000FF"/>
       <sz val="18"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="302">
@@ -5176,7 +5230,7 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="743">
+  <cellXfs count="764">
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="1" hidden="0"/>
     </xf>
@@ -8137,6 +8191,89 @@
     </xf>
     <xf numFmtId="171" fontId="6" fillId="46" borderId="45" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="1" hidden="0"/>
     </xf>
   </cellXfs>
@@ -39823,23 +39960,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:J45"/>
+  <dimension ref="A4:IV47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A19" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A25" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.50"/>
   <cols>
-    <col min="2" max="2" width="11.872727" customWidth="1"/>
-    <col min="3" max="3" width="13.000000" customWidth="1"/>
-    <col min="4" max="4" width="10.000000"/>
-    <col min="5" max="5" width="13.000000" customWidth="1"/>
-    <col min="6" max="6" width="90.500000" customWidth="1"/>
-    <col min="7" max="7" width="13.000000" customWidth="1"/>
+    <col min="1" max="1" width="8.681818" style="756"/>
+    <col min="2" max="2" width="11.872727" customWidth="1" style="756"/>
+    <col min="3" max="3" width="13.000000" customWidth="1" style="756"/>
+    <col min="4" max="4" width="10.000000" style="756"/>
+    <col min="5" max="5" width="13.000000" customWidth="1" style="756"/>
+    <col min="6" max="6" width="90.500000" customWidth="1" style="756"/>
+    <col min="7" max="7" width="13.000000" customWidth="1" style="756"/>
+    <col min="8" max="256" width="8.681818" style="756"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:11">
       <c r="B4" s="520" t="s">
         <v>368</v>
       </c>
@@ -39858,116 +39997,878 @@
       <c r="G4" s="520" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="524" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="524" t="s">
+      <c r="H4" s="756" t="s">
         <v>374</v>
       </c>
-      <c r="D5" s="524"/>
-      <c r="E5" s="524" t="s">
+      <c r="I4" s="756" t="s">
         <v>375</v>
       </c>
-      <c r="F5" s="524" t="s">
+      <c r="J4" s="756" t="s">
         <v>376</v>
       </c>
-      <c r="G5" s="524"/>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="524" t="n">
+      <c r="K4" s="756" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:256" s="761" customFormat="1">
+      <c r="A5" s="762"/>
+      <c r="B5" s="525" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="525" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5" s="525"/>
+      <c r="E5" s="525" t="s">
+        <v>379</v>
+      </c>
+      <c r="F5" s="525" t="s">
+        <v>380</v>
+      </c>
+      <c r="G5" s="525"/>
+      <c r="H5" s="762"/>
+      <c r="I5" s="762"/>
+      <c r="J5" s="762"/>
+      <c r="K5" s="762"/>
+      <c r="L5" s="762"/>
+      <c r="M5" s="762"/>
+      <c r="N5" s="762"/>
+      <c r="O5" s="762"/>
+      <c r="P5" s="762"/>
+      <c r="Q5" s="762"/>
+      <c r="R5" s="762"/>
+      <c r="S5" s="762"/>
+      <c r="T5" s="762"/>
+      <c r="U5" s="762"/>
+      <c r="V5" s="762"/>
+      <c r="W5" s="762"/>
+      <c r="X5" s="762"/>
+      <c r="Y5" s="762"/>
+      <c r="Z5" s="762"/>
+      <c r="AA5" s="762"/>
+      <c r="AB5" s="762"/>
+      <c r="AC5" s="762"/>
+      <c r="AD5" s="762"/>
+      <c r="AE5" s="762"/>
+      <c r="AF5" s="762"/>
+      <c r="AG5" s="762"/>
+      <c r="AH5" s="762"/>
+      <c r="AI5" s="762"/>
+      <c r="AJ5" s="762"/>
+      <c r="AK5" s="762"/>
+      <c r="AL5" s="762"/>
+      <c r="AM5" s="762"/>
+      <c r="AN5" s="762"/>
+      <c r="AO5" s="762"/>
+      <c r="AP5" s="762"/>
+      <c r="AQ5" s="762"/>
+      <c r="AR5" s="762"/>
+      <c r="AS5" s="762"/>
+      <c r="AT5" s="762"/>
+      <c r="AU5" s="762"/>
+      <c r="AV5" s="762"/>
+      <c r="AW5" s="762"/>
+      <c r="AX5" s="762"/>
+      <c r="AY5" s="762"/>
+      <c r="AZ5" s="762"/>
+      <c r="BA5" s="762"/>
+      <c r="BB5" s="762"/>
+      <c r="BC5" s="762"/>
+      <c r="BD5" s="762"/>
+      <c r="BE5" s="762"/>
+      <c r="BF5" s="762"/>
+      <c r="BG5" s="762"/>
+      <c r="BH5" s="762"/>
+      <c r="BI5" s="762"/>
+      <c r="BJ5" s="762"/>
+      <c r="BK5" s="762"/>
+      <c r="BL5" s="762"/>
+      <c r="BM5" s="762"/>
+      <c r="BN5" s="762"/>
+      <c r="BO5" s="762"/>
+      <c r="BP5" s="762"/>
+      <c r="BQ5" s="762"/>
+      <c r="BR5" s="762"/>
+      <c r="BS5" s="762"/>
+      <c r="BT5" s="762"/>
+      <c r="BU5" s="762"/>
+      <c r="BV5" s="762"/>
+      <c r="BW5" s="762"/>
+      <c r="BX5" s="762"/>
+      <c r="BY5" s="762"/>
+      <c r="BZ5" s="762"/>
+      <c r="CA5" s="762"/>
+      <c r="CB5" s="762"/>
+      <c r="CC5" s="762"/>
+      <c r="CD5" s="762"/>
+      <c r="CE5" s="762"/>
+      <c r="CF5" s="762"/>
+      <c r="CG5" s="762"/>
+      <c r="CH5" s="762"/>
+      <c r="CI5" s="762"/>
+      <c r="CJ5" s="762"/>
+      <c r="CK5" s="762"/>
+      <c r="CL5" s="762"/>
+      <c r="CM5" s="762"/>
+      <c r="CN5" s="762"/>
+      <c r="CO5" s="762"/>
+      <c r="CP5" s="762"/>
+      <c r="CQ5" s="762"/>
+      <c r="CR5" s="762"/>
+      <c r="CS5" s="762"/>
+      <c r="CT5" s="762"/>
+      <c r="CU5" s="762"/>
+      <c r="CV5" s="762"/>
+      <c r="CW5" s="762"/>
+      <c r="CX5" s="762"/>
+      <c r="CY5" s="762"/>
+      <c r="CZ5" s="762"/>
+      <c r="DA5" s="762"/>
+      <c r="DB5" s="762"/>
+      <c r="DC5" s="762"/>
+      <c r="DD5" s="762"/>
+      <c r="DE5" s="762"/>
+      <c r="DF5" s="762"/>
+      <c r="DG5" s="762"/>
+      <c r="DH5" s="762"/>
+      <c r="DI5" s="762"/>
+      <c r="DJ5" s="762"/>
+      <c r="DK5" s="762"/>
+      <c r="DL5" s="762"/>
+      <c r="DM5" s="762"/>
+      <c r="DN5" s="762"/>
+      <c r="DO5" s="762"/>
+      <c r="DP5" s="762"/>
+      <c r="DQ5" s="762"/>
+      <c r="DR5" s="762"/>
+      <c r="DS5" s="762"/>
+      <c r="DT5" s="762"/>
+      <c r="DU5" s="762"/>
+      <c r="DV5" s="762"/>
+      <c r="DW5" s="762"/>
+      <c r="DX5" s="762"/>
+      <c r="DY5" s="762"/>
+      <c r="DZ5" s="762"/>
+      <c r="EA5" s="762"/>
+      <c r="EB5" s="762"/>
+      <c r="EC5" s="762"/>
+      <c r="ED5" s="762"/>
+      <c r="EE5" s="762"/>
+      <c r="EF5" s="762"/>
+      <c r="EG5" s="762"/>
+      <c r="EH5" s="762"/>
+      <c r="EI5" s="762"/>
+      <c r="EJ5" s="762"/>
+      <c r="EK5" s="762"/>
+      <c r="EL5" s="762"/>
+      <c r="EM5" s="762"/>
+      <c r="EN5" s="762"/>
+      <c r="EO5" s="762"/>
+      <c r="EP5" s="762"/>
+      <c r="EQ5" s="762"/>
+      <c r="ER5" s="762"/>
+      <c r="ES5" s="762"/>
+      <c r="ET5" s="762"/>
+      <c r="EU5" s="762"/>
+      <c r="EV5" s="762"/>
+      <c r="EW5" s="762"/>
+      <c r="EX5" s="762"/>
+      <c r="EY5" s="762"/>
+      <c r="EZ5" s="762"/>
+      <c r="FA5" s="762"/>
+      <c r="FB5" s="762"/>
+      <c r="FC5" s="762"/>
+      <c r="FD5" s="762"/>
+      <c r="FE5" s="762"/>
+      <c r="FF5" s="762"/>
+      <c r="FG5" s="762"/>
+      <c r="FH5" s="762"/>
+      <c r="FI5" s="762"/>
+      <c r="FJ5" s="762"/>
+      <c r="FK5" s="762"/>
+      <c r="FL5" s="762"/>
+      <c r="FM5" s="762"/>
+      <c r="FN5" s="762"/>
+      <c r="FO5" s="762"/>
+      <c r="FP5" s="762"/>
+      <c r="FQ5" s="762"/>
+      <c r="FR5" s="762"/>
+      <c r="FS5" s="762"/>
+      <c r="FT5" s="762"/>
+      <c r="FU5" s="762"/>
+      <c r="FV5" s="762"/>
+      <c r="FW5" s="762"/>
+      <c r="FX5" s="762"/>
+      <c r="FY5" s="762"/>
+      <c r="FZ5" s="762"/>
+      <c r="GA5" s="762"/>
+      <c r="GB5" s="762"/>
+      <c r="GC5" s="762"/>
+      <c r="GD5" s="762"/>
+      <c r="GE5" s="762"/>
+      <c r="GF5" s="762"/>
+      <c r="GG5" s="762"/>
+      <c r="GH5" s="762"/>
+      <c r="GI5" s="762"/>
+      <c r="GJ5" s="762"/>
+      <c r="GK5" s="762"/>
+      <c r="GL5" s="762"/>
+      <c r="GM5" s="762"/>
+      <c r="GN5" s="762"/>
+      <c r="GO5" s="762"/>
+      <c r="GP5" s="762"/>
+      <c r="GQ5" s="762"/>
+      <c r="GR5" s="762"/>
+      <c r="GS5" s="762"/>
+      <c r="GT5" s="762"/>
+      <c r="GU5" s="762"/>
+      <c r="GV5" s="762"/>
+      <c r="GW5" s="762"/>
+      <c r="GX5" s="762"/>
+      <c r="GY5" s="762"/>
+      <c r="GZ5" s="762"/>
+      <c r="HA5" s="762"/>
+      <c r="HB5" s="762"/>
+      <c r="HC5" s="762"/>
+      <c r="HD5" s="762"/>
+      <c r="HE5" s="762"/>
+      <c r="HF5" s="762"/>
+      <c r="HG5" s="762"/>
+      <c r="HH5" s="762"/>
+      <c r="HI5" s="762"/>
+      <c r="HJ5" s="762"/>
+      <c r="HK5" s="762"/>
+      <c r="HL5" s="762"/>
+      <c r="HM5" s="762"/>
+      <c r="HN5" s="762"/>
+      <c r="HO5" s="762"/>
+      <c r="HP5" s="762"/>
+      <c r="HQ5" s="762"/>
+      <c r="HR5" s="762"/>
+      <c r="HS5" s="762"/>
+      <c r="HT5" s="762"/>
+      <c r="HU5" s="762"/>
+      <c r="HV5" s="762"/>
+      <c r="HW5" s="762"/>
+      <c r="HX5" s="762"/>
+      <c r="HY5" s="762"/>
+      <c r="HZ5" s="762"/>
+      <c r="IA5" s="762"/>
+      <c r="IB5" s="762"/>
+      <c r="IC5" s="762"/>
+      <c r="ID5" s="762"/>
+      <c r="IE5" s="762"/>
+      <c r="IF5" s="762"/>
+      <c r="IG5" s="762"/>
+      <c r="IH5" s="762"/>
+      <c r="II5" s="762"/>
+      <c r="IJ5" s="762"/>
+      <c r="IK5" s="762"/>
+      <c r="IL5" s="762"/>
+      <c r="IM5" s="762"/>
+      <c r="IN5" s="762"/>
+      <c r="IO5" s="762"/>
+      <c r="IP5" s="762"/>
+      <c r="IQ5" s="762"/>
+      <c r="IR5" s="762"/>
+      <c r="IS5" s="762"/>
+      <c r="IT5" s="762"/>
+      <c r="IU5" s="762"/>
+      <c r="IV5" s="762"/>
+    </row>
+    <row r="6" spans="1:256" s="761" customFormat="1">
+      <c r="A6" s="762"/>
+      <c r="B6" s="525" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="524" t="s">
-        <v>377</v>
-      </c>
-      <c r="D6" s="524"/>
-      <c r="E6" s="524" t="s">
-        <v>378</v>
-      </c>
-      <c r="F6" s="524" t="s">
-        <v>379</v>
-      </c>
-      <c r="G6" s="524"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="524" t="n">
+      <c r="C6" s="525" t="s">
+        <v>381</v>
+      </c>
+      <c r="D6" s="525"/>
+      <c r="E6" s="525" t="s">
+        <v>382</v>
+      </c>
+      <c r="F6" s="525" t="s">
+        <v>383</v>
+      </c>
+      <c r="G6" s="525"/>
+      <c r="H6" s="762"/>
+      <c r="I6" s="762"/>
+      <c r="J6" s="762"/>
+      <c r="K6" s="762"/>
+      <c r="L6" s="762"/>
+      <c r="M6" s="762"/>
+      <c r="N6" s="762"/>
+      <c r="O6" s="762"/>
+      <c r="P6" s="762"/>
+      <c r="Q6" s="762"/>
+      <c r="R6" s="762"/>
+      <c r="S6" s="762"/>
+      <c r="T6" s="762"/>
+      <c r="U6" s="762"/>
+      <c r="V6" s="762"/>
+      <c r="W6" s="762"/>
+      <c r="X6" s="762"/>
+      <c r="Y6" s="762"/>
+      <c r="Z6" s="762"/>
+      <c r="AA6" s="762"/>
+      <c r="AB6" s="762"/>
+      <c r="AC6" s="762"/>
+      <c r="AD6" s="762"/>
+      <c r="AE6" s="762"/>
+      <c r="AF6" s="762"/>
+      <c r="AG6" s="762"/>
+      <c r="AH6" s="762"/>
+      <c r="AI6" s="762"/>
+      <c r="AJ6" s="762"/>
+      <c r="AK6" s="762"/>
+      <c r="AL6" s="762"/>
+      <c r="AM6" s="762"/>
+      <c r="AN6" s="762"/>
+      <c r="AO6" s="762"/>
+      <c r="AP6" s="762"/>
+      <c r="AQ6" s="762"/>
+      <c r="AR6" s="762"/>
+      <c r="AS6" s="762"/>
+      <c r="AT6" s="762"/>
+      <c r="AU6" s="762"/>
+      <c r="AV6" s="762"/>
+      <c r="AW6" s="762"/>
+      <c r="AX6" s="762"/>
+      <c r="AY6" s="762"/>
+      <c r="AZ6" s="762"/>
+      <c r="BA6" s="762"/>
+      <c r="BB6" s="762"/>
+      <c r="BC6" s="762"/>
+      <c r="BD6" s="762"/>
+      <c r="BE6" s="762"/>
+      <c r="BF6" s="762"/>
+      <c r="BG6" s="762"/>
+      <c r="BH6" s="762"/>
+      <c r="BI6" s="762"/>
+      <c r="BJ6" s="762"/>
+      <c r="BK6" s="762"/>
+      <c r="BL6" s="762"/>
+      <c r="BM6" s="762"/>
+      <c r="BN6" s="762"/>
+      <c r="BO6" s="762"/>
+      <c r="BP6" s="762"/>
+      <c r="BQ6" s="762"/>
+      <c r="BR6" s="762"/>
+      <c r="BS6" s="762"/>
+      <c r="BT6" s="762"/>
+      <c r="BU6" s="762"/>
+      <c r="BV6" s="762"/>
+      <c r="BW6" s="762"/>
+      <c r="BX6" s="762"/>
+      <c r="BY6" s="762"/>
+      <c r="BZ6" s="762"/>
+      <c r="CA6" s="762"/>
+      <c r="CB6" s="762"/>
+      <c r="CC6" s="762"/>
+      <c r="CD6" s="762"/>
+      <c r="CE6" s="762"/>
+      <c r="CF6" s="762"/>
+      <c r="CG6" s="762"/>
+      <c r="CH6" s="762"/>
+      <c r="CI6" s="762"/>
+      <c r="CJ6" s="762"/>
+      <c r="CK6" s="762"/>
+      <c r="CL6" s="762"/>
+      <c r="CM6" s="762"/>
+      <c r="CN6" s="762"/>
+      <c r="CO6" s="762"/>
+      <c r="CP6" s="762"/>
+      <c r="CQ6" s="762"/>
+      <c r="CR6" s="762"/>
+      <c r="CS6" s="762"/>
+      <c r="CT6" s="762"/>
+      <c r="CU6" s="762"/>
+      <c r="CV6" s="762"/>
+      <c r="CW6" s="762"/>
+      <c r="CX6" s="762"/>
+      <c r="CY6" s="762"/>
+      <c r="CZ6" s="762"/>
+      <c r="DA6" s="762"/>
+      <c r="DB6" s="762"/>
+      <c r="DC6" s="762"/>
+      <c r="DD6" s="762"/>
+      <c r="DE6" s="762"/>
+      <c r="DF6" s="762"/>
+      <c r="DG6" s="762"/>
+      <c r="DH6" s="762"/>
+      <c r="DI6" s="762"/>
+      <c r="DJ6" s="762"/>
+      <c r="DK6" s="762"/>
+      <c r="DL6" s="762"/>
+      <c r="DM6" s="762"/>
+      <c r="DN6" s="762"/>
+      <c r="DO6" s="762"/>
+      <c r="DP6" s="762"/>
+      <c r="DQ6" s="762"/>
+      <c r="DR6" s="762"/>
+      <c r="DS6" s="762"/>
+      <c r="DT6" s="762"/>
+      <c r="DU6" s="762"/>
+      <c r="DV6" s="762"/>
+      <c r="DW6" s="762"/>
+      <c r="DX6" s="762"/>
+      <c r="DY6" s="762"/>
+      <c r="DZ6" s="762"/>
+      <c r="EA6" s="762"/>
+      <c r="EB6" s="762"/>
+      <c r="EC6" s="762"/>
+      <c r="ED6" s="762"/>
+      <c r="EE6" s="762"/>
+      <c r="EF6" s="762"/>
+      <c r="EG6" s="762"/>
+      <c r="EH6" s="762"/>
+      <c r="EI6" s="762"/>
+      <c r="EJ6" s="762"/>
+      <c r="EK6" s="762"/>
+      <c r="EL6" s="762"/>
+      <c r="EM6" s="762"/>
+      <c r="EN6" s="762"/>
+      <c r="EO6" s="762"/>
+      <c r="EP6" s="762"/>
+      <c r="EQ6" s="762"/>
+      <c r="ER6" s="762"/>
+      <c r="ES6" s="762"/>
+      <c r="ET6" s="762"/>
+      <c r="EU6" s="762"/>
+      <c r="EV6" s="762"/>
+      <c r="EW6" s="762"/>
+      <c r="EX6" s="762"/>
+      <c r="EY6" s="762"/>
+      <c r="EZ6" s="762"/>
+      <c r="FA6" s="762"/>
+      <c r="FB6" s="762"/>
+      <c r="FC6" s="762"/>
+      <c r="FD6" s="762"/>
+      <c r="FE6" s="762"/>
+      <c r="FF6" s="762"/>
+      <c r="FG6" s="762"/>
+      <c r="FH6" s="762"/>
+      <c r="FI6" s="762"/>
+      <c r="FJ6" s="762"/>
+      <c r="FK6" s="762"/>
+      <c r="FL6" s="762"/>
+      <c r="FM6" s="762"/>
+      <c r="FN6" s="762"/>
+      <c r="FO6" s="762"/>
+      <c r="FP6" s="762"/>
+      <c r="FQ6" s="762"/>
+      <c r="FR6" s="762"/>
+      <c r="FS6" s="762"/>
+      <c r="FT6" s="762"/>
+      <c r="FU6" s="762"/>
+      <c r="FV6" s="762"/>
+      <c r="FW6" s="762"/>
+      <c r="FX6" s="762"/>
+      <c r="FY6" s="762"/>
+      <c r="FZ6" s="762"/>
+      <c r="GA6" s="762"/>
+      <c r="GB6" s="762"/>
+      <c r="GC6" s="762"/>
+      <c r="GD6" s="762"/>
+      <c r="GE6" s="762"/>
+      <c r="GF6" s="762"/>
+      <c r="GG6" s="762"/>
+      <c r="GH6" s="762"/>
+      <c r="GI6" s="762"/>
+      <c r="GJ6" s="762"/>
+      <c r="GK6" s="762"/>
+      <c r="GL6" s="762"/>
+      <c r="GM6" s="762"/>
+      <c r="GN6" s="762"/>
+      <c r="GO6" s="762"/>
+      <c r="GP6" s="762"/>
+      <c r="GQ6" s="762"/>
+      <c r="GR6" s="762"/>
+      <c r="GS6" s="762"/>
+      <c r="GT6" s="762"/>
+      <c r="GU6" s="762"/>
+      <c r="GV6" s="762"/>
+      <c r="GW6" s="762"/>
+      <c r="GX6" s="762"/>
+      <c r="GY6" s="762"/>
+      <c r="GZ6" s="762"/>
+      <c r="HA6" s="762"/>
+      <c r="HB6" s="762"/>
+      <c r="HC6" s="762"/>
+      <c r="HD6" s="762"/>
+      <c r="HE6" s="762"/>
+      <c r="HF6" s="762"/>
+      <c r="HG6" s="762"/>
+      <c r="HH6" s="762"/>
+      <c r="HI6" s="762"/>
+      <c r="HJ6" s="762"/>
+      <c r="HK6" s="762"/>
+      <c r="HL6" s="762"/>
+      <c r="HM6" s="762"/>
+      <c r="HN6" s="762"/>
+      <c r="HO6" s="762"/>
+      <c r="HP6" s="762"/>
+      <c r="HQ6" s="762"/>
+      <c r="HR6" s="762"/>
+      <c r="HS6" s="762"/>
+      <c r="HT6" s="762"/>
+      <c r="HU6" s="762"/>
+      <c r="HV6" s="762"/>
+      <c r="HW6" s="762"/>
+      <c r="HX6" s="762"/>
+      <c r="HY6" s="762"/>
+      <c r="HZ6" s="762"/>
+      <c r="IA6" s="762"/>
+      <c r="IB6" s="762"/>
+      <c r="IC6" s="762"/>
+      <c r="ID6" s="762"/>
+      <c r="IE6" s="762"/>
+      <c r="IF6" s="762"/>
+      <c r="IG6" s="762"/>
+      <c r="IH6" s="762"/>
+      <c r="II6" s="762"/>
+      <c r="IJ6" s="762"/>
+      <c r="IK6" s="762"/>
+      <c r="IL6" s="762"/>
+      <c r="IM6" s="762"/>
+      <c r="IN6" s="762"/>
+      <c r="IO6" s="762"/>
+      <c r="IP6" s="762"/>
+      <c r="IQ6" s="762"/>
+      <c r="IR6" s="762"/>
+      <c r="IS6" s="762"/>
+      <c r="IT6" s="762"/>
+      <c r="IU6" s="762"/>
+      <c r="IV6" s="762"/>
+    </row>
+    <row r="7" spans="1:256" s="761" customFormat="1">
+      <c r="A7" s="762"/>
+      <c r="B7" s="525" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="524" t="s">
-        <v>380</v>
-      </c>
-      <c r="D7" s="524"/>
-      <c r="E7" s="524" t="s">
-        <v>378</v>
-      </c>
-      <c r="F7" s="524" t="s">
-        <v>381</v>
-      </c>
-      <c r="G7" s="524"/>
-    </row>
-    <row r="8" spans="2:7" s="522" customFormat="1">
+      <c r="C7" s="525" t="s">
+        <v>384</v>
+      </c>
+      <c r="D7" s="525"/>
+      <c r="E7" s="525" t="s">
+        <v>382</v>
+      </c>
+      <c r="F7" s="525" t="s">
+        <v>385</v>
+      </c>
+      <c r="G7" s="525"/>
+      <c r="H7" s="762"/>
+      <c r="I7" s="762"/>
+      <c r="J7" s="762"/>
+      <c r="K7" s="762"/>
+      <c r="L7" s="762"/>
+      <c r="M7" s="762"/>
+      <c r="N7" s="762"/>
+      <c r="O7" s="762"/>
+      <c r="P7" s="762"/>
+      <c r="Q7" s="762"/>
+      <c r="R7" s="762"/>
+      <c r="S7" s="762"/>
+      <c r="T7" s="762"/>
+      <c r="U7" s="762"/>
+      <c r="V7" s="762"/>
+      <c r="W7" s="762"/>
+      <c r="X7" s="762"/>
+      <c r="Y7" s="762"/>
+      <c r="Z7" s="762"/>
+      <c r="AA7" s="762"/>
+      <c r="AB7" s="762"/>
+      <c r="AC7" s="762"/>
+      <c r="AD7" s="762"/>
+      <c r="AE7" s="762"/>
+      <c r="AF7" s="762"/>
+      <c r="AG7" s="762"/>
+      <c r="AH7" s="762"/>
+      <c r="AI7" s="762"/>
+      <c r="AJ7" s="762"/>
+      <c r="AK7" s="762"/>
+      <c r="AL7" s="762"/>
+      <c r="AM7" s="762"/>
+      <c r="AN7" s="762"/>
+      <c r="AO7" s="762"/>
+      <c r="AP7" s="762"/>
+      <c r="AQ7" s="762"/>
+      <c r="AR7" s="762"/>
+      <c r="AS7" s="762"/>
+      <c r="AT7" s="762"/>
+      <c r="AU7" s="762"/>
+      <c r="AV7" s="762"/>
+      <c r="AW7" s="762"/>
+      <c r="AX7" s="762"/>
+      <c r="AY7" s="762"/>
+      <c r="AZ7" s="762"/>
+      <c r="BA7" s="762"/>
+      <c r="BB7" s="762"/>
+      <c r="BC7" s="762"/>
+      <c r="BD7" s="762"/>
+      <c r="BE7" s="762"/>
+      <c r="BF7" s="762"/>
+      <c r="BG7" s="762"/>
+      <c r="BH7" s="762"/>
+      <c r="BI7" s="762"/>
+      <c r="BJ7" s="762"/>
+      <c r="BK7" s="762"/>
+      <c r="BL7" s="762"/>
+      <c r="BM7" s="762"/>
+      <c r="BN7" s="762"/>
+      <c r="BO7" s="762"/>
+      <c r="BP7" s="762"/>
+      <c r="BQ7" s="762"/>
+      <c r="BR7" s="762"/>
+      <c r="BS7" s="762"/>
+      <c r="BT7" s="762"/>
+      <c r="BU7" s="762"/>
+      <c r="BV7" s="762"/>
+      <c r="BW7" s="762"/>
+      <c r="BX7" s="762"/>
+      <c r="BY7" s="762"/>
+      <c r="BZ7" s="762"/>
+      <c r="CA7" s="762"/>
+      <c r="CB7" s="762"/>
+      <c r="CC7" s="762"/>
+      <c r="CD7" s="762"/>
+      <c r="CE7" s="762"/>
+      <c r="CF7" s="762"/>
+      <c r="CG7" s="762"/>
+      <c r="CH7" s="762"/>
+      <c r="CI7" s="762"/>
+      <c r="CJ7" s="762"/>
+      <c r="CK7" s="762"/>
+      <c r="CL7" s="762"/>
+      <c r="CM7" s="762"/>
+      <c r="CN7" s="762"/>
+      <c r="CO7" s="762"/>
+      <c r="CP7" s="762"/>
+      <c r="CQ7" s="762"/>
+      <c r="CR7" s="762"/>
+      <c r="CS7" s="762"/>
+      <c r="CT7" s="762"/>
+      <c r="CU7" s="762"/>
+      <c r="CV7" s="762"/>
+      <c r="CW7" s="762"/>
+      <c r="CX7" s="762"/>
+      <c r="CY7" s="762"/>
+      <c r="CZ7" s="762"/>
+      <c r="DA7" s="762"/>
+      <c r="DB7" s="762"/>
+      <c r="DC7" s="762"/>
+      <c r="DD7" s="762"/>
+      <c r="DE7" s="762"/>
+      <c r="DF7" s="762"/>
+      <c r="DG7" s="762"/>
+      <c r="DH7" s="762"/>
+      <c r="DI7" s="762"/>
+      <c r="DJ7" s="762"/>
+      <c r="DK7" s="762"/>
+      <c r="DL7" s="762"/>
+      <c r="DM7" s="762"/>
+      <c r="DN7" s="762"/>
+      <c r="DO7" s="762"/>
+      <c r="DP7" s="762"/>
+      <c r="DQ7" s="762"/>
+      <c r="DR7" s="762"/>
+      <c r="DS7" s="762"/>
+      <c r="DT7" s="762"/>
+      <c r="DU7" s="762"/>
+      <c r="DV7" s="762"/>
+      <c r="DW7" s="762"/>
+      <c r="DX7" s="762"/>
+      <c r="DY7" s="762"/>
+      <c r="DZ7" s="762"/>
+      <c r="EA7" s="762"/>
+      <c r="EB7" s="762"/>
+      <c r="EC7" s="762"/>
+      <c r="ED7" s="762"/>
+      <c r="EE7" s="762"/>
+      <c r="EF7" s="762"/>
+      <c r="EG7" s="762"/>
+      <c r="EH7" s="762"/>
+      <c r="EI7" s="762"/>
+      <c r="EJ7" s="762"/>
+      <c r="EK7" s="762"/>
+      <c r="EL7" s="762"/>
+      <c r="EM7" s="762"/>
+      <c r="EN7" s="762"/>
+      <c r="EO7" s="762"/>
+      <c r="EP7" s="762"/>
+      <c r="EQ7" s="762"/>
+      <c r="ER7" s="762"/>
+      <c r="ES7" s="762"/>
+      <c r="ET7" s="762"/>
+      <c r="EU7" s="762"/>
+      <c r="EV7" s="762"/>
+      <c r="EW7" s="762"/>
+      <c r="EX7" s="762"/>
+      <c r="EY7" s="762"/>
+      <c r="EZ7" s="762"/>
+      <c r="FA7" s="762"/>
+      <c r="FB7" s="762"/>
+      <c r="FC7" s="762"/>
+      <c r="FD7" s="762"/>
+      <c r="FE7" s="762"/>
+      <c r="FF7" s="762"/>
+      <c r="FG7" s="762"/>
+      <c r="FH7" s="762"/>
+      <c r="FI7" s="762"/>
+      <c r="FJ7" s="762"/>
+      <c r="FK7" s="762"/>
+      <c r="FL7" s="762"/>
+      <c r="FM7" s="762"/>
+      <c r="FN7" s="762"/>
+      <c r="FO7" s="762"/>
+      <c r="FP7" s="762"/>
+      <c r="FQ7" s="762"/>
+      <c r="FR7" s="762"/>
+      <c r="FS7" s="762"/>
+      <c r="FT7" s="762"/>
+      <c r="FU7" s="762"/>
+      <c r="FV7" s="762"/>
+      <c r="FW7" s="762"/>
+      <c r="FX7" s="762"/>
+      <c r="FY7" s="762"/>
+      <c r="FZ7" s="762"/>
+      <c r="GA7" s="762"/>
+      <c r="GB7" s="762"/>
+      <c r="GC7" s="762"/>
+      <c r="GD7" s="762"/>
+      <c r="GE7" s="762"/>
+      <c r="GF7" s="762"/>
+      <c r="GG7" s="762"/>
+      <c r="GH7" s="762"/>
+      <c r="GI7" s="762"/>
+      <c r="GJ7" s="762"/>
+      <c r="GK7" s="762"/>
+      <c r="GL7" s="762"/>
+      <c r="GM7" s="762"/>
+      <c r="GN7" s="762"/>
+      <c r="GO7" s="762"/>
+      <c r="GP7" s="762"/>
+      <c r="GQ7" s="762"/>
+      <c r="GR7" s="762"/>
+      <c r="GS7" s="762"/>
+      <c r="GT7" s="762"/>
+      <c r="GU7" s="762"/>
+      <c r="GV7" s="762"/>
+      <c r="GW7" s="762"/>
+      <c r="GX7" s="762"/>
+      <c r="GY7" s="762"/>
+      <c r="GZ7" s="762"/>
+      <c r="HA7" s="762"/>
+      <c r="HB7" s="762"/>
+      <c r="HC7" s="762"/>
+      <c r="HD7" s="762"/>
+      <c r="HE7" s="762"/>
+      <c r="HF7" s="762"/>
+      <c r="HG7" s="762"/>
+      <c r="HH7" s="762"/>
+      <c r="HI7" s="762"/>
+      <c r="HJ7" s="762"/>
+      <c r="HK7" s="762"/>
+      <c r="HL7" s="762"/>
+      <c r="HM7" s="762"/>
+      <c r="HN7" s="762"/>
+      <c r="HO7" s="762"/>
+      <c r="HP7" s="762"/>
+      <c r="HQ7" s="762"/>
+      <c r="HR7" s="762"/>
+      <c r="HS7" s="762"/>
+      <c r="HT7" s="762"/>
+      <c r="HU7" s="762"/>
+      <c r="HV7" s="762"/>
+      <c r="HW7" s="762"/>
+      <c r="HX7" s="762"/>
+      <c r="HY7" s="762"/>
+      <c r="HZ7" s="762"/>
+      <c r="IA7" s="762"/>
+      <c r="IB7" s="762"/>
+      <c r="IC7" s="762"/>
+      <c r="ID7" s="762"/>
+      <c r="IE7" s="762"/>
+      <c r="IF7" s="762"/>
+      <c r="IG7" s="762"/>
+      <c r="IH7" s="762"/>
+      <c r="II7" s="762"/>
+      <c r="IJ7" s="762"/>
+      <c r="IK7" s="762"/>
+      <c r="IL7" s="762"/>
+      <c r="IM7" s="762"/>
+      <c r="IN7" s="762"/>
+      <c r="IO7" s="762"/>
+      <c r="IP7" s="762"/>
+      <c r="IQ7" s="762"/>
+      <c r="IR7" s="762"/>
+      <c r="IS7" s="762"/>
+      <c r="IT7" s="762"/>
+      <c r="IU7" s="762"/>
+      <c r="IV7" s="762"/>
+    </row>
+    <row r="8" spans="2:8" s="757" customFormat="1">
       <c r="B8" s="525" t="n">
         <v>4</v>
       </c>
       <c r="C8" s="525" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="D8" s="525"/>
       <c r="E8" s="525" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F8" s="525" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="G8" s="525"/>
     </row>
-    <row r="9" spans="2:7" s="10" customFormat="1">
-      <c r="B9" s="524" t="n">
+    <row r="9" spans="1:256" s="763" customFormat="1">
+      <c r="B9" s="525" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="524" t="s">
-        <v>384</v>
-      </c>
-      <c r="D9" s="524"/>
-      <c r="E9" s="524" t="s">
-        <v>375</v>
-      </c>
-      <c r="F9" s="524" t="s">
-        <v>385</v>
-      </c>
-      <c r="G9" s="524"/>
-    </row>
-    <row r="10" spans="2:7" s="10" customFormat="1">
-      <c r="B10" s="524" t="n">
+      <c r="C9" s="525" t="s">
+        <v>388</v>
+      </c>
+      <c r="D9" s="525"/>
+      <c r="E9" s="525" t="s">
+        <v>379</v>
+      </c>
+      <c r="F9" s="525" t="s">
+        <v>389</v>
+      </c>
+      <c r="G9" s="525"/>
+    </row>
+    <row r="10" spans="1:256" s="763" customFormat="1">
+      <c r="B10" s="525" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="524" t="s">
-        <v>386</v>
-      </c>
-      <c r="D10" s="524"/>
-      <c r="E10" s="524" t="s">
-        <v>375</v>
-      </c>
-      <c r="F10" s="524" t="s">
-        <v>387</v>
-      </c>
-      <c r="G10" s="524"/>
+      <c r="C10" s="525" t="s">
+        <v>390</v>
+      </c>
+      <c r="D10" s="525"/>
+      <c r="E10" s="525" t="s">
+        <v>379</v>
+      </c>
+      <c r="F10" s="525" t="s">
+        <v>391</v>
+      </c>
+      <c r="G10" s="525"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="524" t="n">
         <v>7</v>
       </c>
       <c r="C11" s="524" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D11" s="524"/>
       <c r="E11" s="524" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F11" s="524" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="G11" s="524"/>
     </row>
@@ -39976,14 +40877,14 @@
         <v>8</v>
       </c>
       <c r="C12" s="524" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D12" s="524"/>
       <c r="E12" s="524" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F12" s="524" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="G12" s="524"/>
     </row>
@@ -39992,98 +40893,98 @@
         <v>9</v>
       </c>
       <c r="C13" s="524" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="D13" s="524"/>
       <c r="E13" s="524" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F13" s="524" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="G13" s="524"/>
     </row>
-    <row r="14" spans="2:7" s="528" customFormat="1">
+    <row r="14" spans="2:7" s="759" customFormat="1">
       <c r="B14" s="524" t="n">
         <v>10</v>
       </c>
       <c r="C14" s="527" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="D14" s="527"/>
       <c r="E14" s="527" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F14" s="527" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="G14" s="527"/>
     </row>
-    <row r="15" spans="2:7" s="528" customFormat="1">
+    <row r="15" spans="2:7" s="759" customFormat="1">
       <c r="B15" s="524" t="n">
         <v>11</v>
       </c>
       <c r="C15" s="527" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="D15" s="527"/>
       <c r="E15" s="527" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F15" s="527" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="G15" s="527"/>
     </row>
-    <row r="16" spans="2:7" s="528" customFormat="1">
+    <row r="16" spans="2:7" s="759" customFormat="1">
       <c r="B16" s="524" t="n">
         <v>12</v>
       </c>
       <c r="C16" s="527" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="D16" s="527"/>
       <c r="E16" s="527" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F16" s="527" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="G16" s="527"/>
     </row>
-    <row r="17" spans="1:10" s="523" customFormat="1">
-      <c r="A17" s="10"/>
+    <row r="17" spans="1:10" s="760" customFormat="1">
+      <c r="A17" s="758"/>
       <c r="B17" s="524" t="n">
         <v>13</v>
       </c>
       <c r="C17" s="524" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D17" s="524"/>
       <c r="E17" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F17" s="526" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="G17" s="524"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="H17" s="758"/>
+      <c r="I17" s="758"/>
+      <c r="J17" s="758"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="524" t="n">
         <v>14</v>
       </c>
       <c r="C18" s="524" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="D18" s="524"/>
       <c r="E18" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F18" s="524" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="G18" s="524"/>
     </row>
@@ -40092,14 +40993,14 @@
         <v>15</v>
       </c>
       <c r="C19" s="524" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D19" s="524"/>
       <c r="E19" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F19" s="524" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="G19" s="524"/>
     </row>
@@ -40108,14 +41009,14 @@
         <v>16</v>
       </c>
       <c r="C20" s="524" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="D20" s="524"/>
       <c r="E20" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F20" s="524" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="G20" s="524"/>
     </row>
@@ -40124,14 +41025,14 @@
         <v>17</v>
       </c>
       <c r="C21" s="524" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="D21" s="524"/>
       <c r="E21" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F21" s="526" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="G21" s="524"/>
     </row>
@@ -40140,14 +41041,14 @@
         <v>18</v>
       </c>
       <c r="C22" s="524" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="D22" s="524"/>
       <c r="E22" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F22" s="526" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G22" s="524"/>
     </row>
@@ -40156,14 +41057,14 @@
         <v>19</v>
       </c>
       <c r="C23" s="524" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="D23" s="524"/>
       <c r="E23" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F23" s="526" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="G23" s="524"/>
     </row>
@@ -40172,14 +41073,14 @@
         <v>20</v>
       </c>
       <c r="C24" s="524" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="D24" s="524"/>
       <c r="E24" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F24" s="524" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="G24" s="524"/>
     </row>
@@ -40188,14 +41089,14 @@
         <v>21</v>
       </c>
       <c r="C25" s="524" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="D25" s="524"/>
       <c r="E25" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F25" s="524" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="G25" s="524"/>
     </row>
@@ -40204,14 +41105,14 @@
         <v>22</v>
       </c>
       <c r="C26" s="524" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="D26" s="524"/>
       <c r="E26" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F26" s="524" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="G26" s="524"/>
     </row>
@@ -40220,14 +41121,14 @@
         <v>23</v>
       </c>
       <c r="C27" s="524" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D27" s="524"/>
       <c r="E27" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F27" s="524" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="G27" s="524"/>
     </row>
@@ -40236,14 +41137,14 @@
         <v>24</v>
       </c>
       <c r="C28" s="524" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D28" s="524"/>
       <c r="E28" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F28" s="524" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="G28" s="524"/>
     </row>
@@ -40252,78 +41153,78 @@
         <v>25</v>
       </c>
       <c r="C29" s="524" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D29" s="524"/>
       <c r="E29" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F29" s="524" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="G29" s="524"/>
     </row>
-    <row r="30" spans="2:7" s="522" customFormat="1">
+    <row r="30" spans="1:256" s="757" customFormat="1">
       <c r="B30" s="525" t="n">
         <v>26</v>
       </c>
       <c r="C30" s="525" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D30" s="525"/>
       <c r="E30" s="525" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F30" s="525" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="G30" s="525"/>
     </row>
-    <row r="31" spans="2:7" s="10" customFormat="1">
-      <c r="B31" s="524" t="n">
+    <row r="31" spans="1:256" s="763" customFormat="1">
+      <c r="B31" s="525" t="n">
         <v>27</v>
       </c>
-      <c r="C31" s="524" t="s">
-        <v>428</v>
-      </c>
-      <c r="D31" s="524"/>
-      <c r="E31" s="524" t="s">
-        <v>395</v>
-      </c>
-      <c r="F31" s="524" t="s">
-        <v>429</v>
-      </c>
-      <c r="G31" s="524"/>
-    </row>
-    <row r="32" spans="2:7" s="10" customFormat="1">
-      <c r="B32" s="524" t="n">
+      <c r="C31" s="525" t="s">
+        <v>432</v>
+      </c>
+      <c r="D31" s="525"/>
+      <c r="E31" s="525" t="s">
+        <v>399</v>
+      </c>
+      <c r="F31" s="525" t="s">
+        <v>433</v>
+      </c>
+      <c r="G31" s="525"/>
+    </row>
+    <row r="32" spans="1:256" s="763" customFormat="1">
+      <c r="B32" s="525" t="n">
         <v>28</v>
       </c>
-      <c r="C32" s="524" t="s">
-        <v>430</v>
-      </c>
-      <c r="D32" s="524"/>
-      <c r="E32" s="524" t="s">
-        <v>395</v>
-      </c>
-      <c r="F32" s="524" t="s">
-        <v>431</v>
-      </c>
-      <c r="G32" s="524"/>
+      <c r="C32" s="525" t="s">
+        <v>434</v>
+      </c>
+      <c r="D32" s="525"/>
+      <c r="E32" s="525" t="s">
+        <v>399</v>
+      </c>
+      <c r="F32" s="525" t="s">
+        <v>435</v>
+      </c>
+      <c r="G32" s="525"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="524" t="n">
         <v>29</v>
       </c>
       <c r="C33" s="524" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D33" s="524"/>
       <c r="E33" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F33" s="524" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="G33" s="524"/>
     </row>
@@ -40332,14 +41233,14 @@
         <v>30</v>
       </c>
       <c r="C34" s="524" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="D34" s="524"/>
       <c r="E34" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F34" s="524" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="G34" s="524"/>
     </row>
@@ -40348,14 +41249,14 @@
         <v>31</v>
       </c>
       <c r="C35" s="524" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D35" s="524"/>
       <c r="E35" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F35" s="524" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="G35" s="524"/>
     </row>
@@ -40364,14 +41265,14 @@
         <v>32</v>
       </c>
       <c r="C36" s="524" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="D36" s="524"/>
       <c r="E36" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F36" s="524" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="G36" s="524"/>
     </row>
@@ -40380,112 +41281,172 @@
         <v>33</v>
       </c>
       <c r="C37" s="524" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D37" s="524"/>
       <c r="E37" s="524" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F37" s="526" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="G37" s="524"/>
     </row>
-    <row r="38" spans="2:7" s="522" customFormat="1">
+    <row r="38" spans="1:256" s="757" customFormat="1">
       <c r="B38" s="525" t="n">
         <v>34</v>
       </c>
       <c r="C38" s="525" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="D38" s="525"/>
       <c r="E38" s="525" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F38" s="525" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="G38" s="525"/>
     </row>
-    <row r="39" spans="2:7" s="10" customFormat="1">
-      <c r="B39" s="524" t="n">
+    <row r="39" spans="1:256" s="763" customFormat="1">
+      <c r="B39" s="525" t="n">
         <v>35</v>
       </c>
-      <c r="C39" s="524" t="s">
-        <v>444</v>
-      </c>
-      <c r="D39" s="524"/>
-      <c r="E39" s="524" t="s">
-        <v>375</v>
-      </c>
-      <c r="F39" s="524" t="s">
-        <v>445</v>
-      </c>
-      <c r="G39" s="524"/>
-    </row>
-    <row r="40" spans="2:7" s="10" customFormat="1">
-      <c r="B40" s="524" t="n">
+      <c r="C39" s="525" t="s">
+        <v>448</v>
+      </c>
+      <c r="D39" s="525"/>
+      <c r="E39" s="525" t="s">
+        <v>379</v>
+      </c>
+      <c r="F39" s="525" t="s">
+        <v>449</v>
+      </c>
+      <c r="G39" s="525"/>
+    </row>
+    <row r="40" spans="1:256" s="763" customFormat="1">
+      <c r="B40" s="525" t="n">
         <v>36</v>
       </c>
-      <c r="C40" s="524" t="s">
-        <v>446</v>
-      </c>
-      <c r="D40" s="524"/>
-      <c r="E40" s="524" t="s">
-        <v>375</v>
-      </c>
-      <c r="F40" s="524" t="s">
-        <v>447</v>
-      </c>
-      <c r="G40" s="524"/>
+      <c r="C40" s="525" t="s">
+        <v>450</v>
+      </c>
+      <c r="D40" s="525"/>
+      <c r="E40" s="525" t="s">
+        <v>379</v>
+      </c>
+      <c r="F40" s="525" t="s">
+        <v>451</v>
+      </c>
+      <c r="G40" s="525"/>
     </row>
     <row r="41" spans="2:7">
       <c r="B41" s="521" t="n">
         <v>37</v>
       </c>
       <c r="C41" s="521" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D41" s="521"/>
       <c r="E41" s="521" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F41" s="521" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="G41" s="521"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="521"/>
-      <c r="C42" s="521"/>
+      <c r="B42" s="521" t="n">
+        <v>38</v>
+      </c>
+      <c r="C42" s="521" t="s">
+        <v>454</v>
+      </c>
       <c r="D42" s="521"/>
-      <c r="E42" s="521"/>
-      <c r="F42" s="521"/>
+      <c r="E42" s="521" t="s">
+        <v>399</v>
+      </c>
+      <c r="F42" s="521" t="s">
+        <v>455</v>
+      </c>
       <c r="G42" s="521"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="521"/>
-      <c r="C43" s="521"/>
+      <c r="B43" s="521" t="n">
+        <v>39</v>
+      </c>
+      <c r="C43" s="521" t="s">
+        <v>456</v>
+      </c>
       <c r="D43" s="521"/>
-      <c r="E43" s="521"/>
-      <c r="F43" s="521"/>
+      <c r="E43" s="521" t="s">
+        <v>379</v>
+      </c>
+      <c r="F43" s="521" t="s">
+        <v>457</v>
+      </c>
       <c r="G43" s="521"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="521"/>
-      <c r="C44" s="521"/>
+      <c r="B44" s="521" t="n">
+        <v>40</v>
+      </c>
+      <c r="C44" s="521" t="s">
+        <v>458</v>
+      </c>
       <c r="D44" s="521"/>
-      <c r="E44" s="521"/>
-      <c r="F44" s="521"/>
+      <c r="E44" s="521" t="s">
+        <v>399</v>
+      </c>
+      <c r="F44" s="521" t="s">
+        <v>459</v>
+      </c>
       <c r="G44" s="521"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="521"/>
-      <c r="C45" s="521"/>
+      <c r="B45" s="521" t="n">
+        <v>41</v>
+      </c>
+      <c r="C45" s="521" t="s">
+        <v>460</v>
+      </c>
       <c r="D45" s="521"/>
-      <c r="E45" s="521"/>
-      <c r="F45" s="521"/>
+      <c r="E45" s="521" t="s">
+        <v>399</v>
+      </c>
+      <c r="F45" s="521" t="s">
+        <v>461</v>
+      </c>
       <c r="G45" s="521"/>
+    </row>
+    <row r="46" spans="2:6" s="743" customFormat="1">
+      <c r="B46" s="743" t="n">
+        <v>42</v>
+      </c>
+      <c r="C46" s="743" t="s">
+        <v>462</v>
+      </c>
+      <c r="E46" s="743" t="s">
+        <v>399</v>
+      </c>
+      <c r="F46" s="743" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" s="743" customFormat="1">
+      <c r="B47" s="743" t="n">
+        <v>43</v>
+      </c>
+      <c r="C47" s="743" t="s">
+        <v>464</v>
+      </c>
+      <c r="E47" s="743" t="s">
+        <v>399</v>
+      </c>
+      <c r="F47" s="743" t="s">
+        <v>465</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>

</xml_diff>

<commit_message>
fix some bugs. test to level-12, test to layer 5
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="shashibici"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="6" xWindow="240" yWindow="60" windowWidth="9705" windowHeight="3000" tabRatio="305"/>
+    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="9705" windowHeight="3000" tabRatio="305"/>
   </bookViews>
   <sheets>
     <sheet name="装备性能表" sheetId="1" r:id="rId4"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="pm" day="1486346637" val="694"/>
+      <pm:revision xmlns:pm="pm" day="1486363645" val="694"/>
     </ext>
   </extLst>
 </workbook>
@@ -5230,7 +5230,7 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="764">
+  <cellXfs count="765">
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="1" hidden="0"/>
     </xf>
@@ -8274,6 +8274,10 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="1" hidden="0"/>
     </xf>
   </cellXfs>
@@ -18068,8 +18072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView view="normal" topLeftCell="C1" zoomScale="55" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" view="normal" zoomScale="55" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="11" defaultColWidth="12.627273" defaultRowHeight="14.50"/>
@@ -18397,7 +18401,7 @@
         <v>105</v>
       </c>
       <c r="D9" s="140" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="150" t="n">
         <v>9</v>
@@ -18436,7 +18440,7 @@
         <v>108</v>
       </c>
       <c r="D10" s="140" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="150" t="n">
         <v>26</v>
@@ -18520,7 +18524,7 @@
         <v>27</v>
       </c>
       <c r="F12" s="50" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G12" s="156" t="n">
         <v>76</v>
@@ -39962,8 +39966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:IV47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A25" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView view="normal" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.50"/>
@@ -41340,21 +41344,271 @@
       </c>
       <c r="G40" s="525"/>
     </row>
-    <row r="41" spans="2:7">
-      <c r="B41" s="521" t="n">
+    <row r="41" spans="1:256" s="761" customFormat="1">
+      <c r="A41" s="762"/>
+      <c r="B41" s="764" t="n">
         <v>37</v>
       </c>
-      <c r="C41" s="521" t="s">
+      <c r="C41" s="764" t="s">
         <v>452</v>
       </c>
-      <c r="D41" s="521"/>
-      <c r="E41" s="521" t="s">
+      <c r="D41" s="764"/>
+      <c r="E41" s="764" t="s">
         <v>379</v>
       </c>
-      <c r="F41" s="521" t="s">
+      <c r="F41" s="764" t="s">
         <v>453</v>
       </c>
-      <c r="G41" s="521"/>
+      <c r="G41" s="764"/>
+      <c r="H41" s="762"/>
+      <c r="I41" s="762"/>
+      <c r="J41" s="762"/>
+      <c r="K41" s="762"/>
+      <c r="L41" s="762"/>
+      <c r="M41" s="762"/>
+      <c r="N41" s="762"/>
+      <c r="O41" s="762"/>
+      <c r="P41" s="762"/>
+      <c r="Q41" s="762"/>
+      <c r="R41" s="762"/>
+      <c r="S41" s="762"/>
+      <c r="T41" s="762"/>
+      <c r="U41" s="762"/>
+      <c r="V41" s="762"/>
+      <c r="W41" s="762"/>
+      <c r="X41" s="762"/>
+      <c r="Y41" s="762"/>
+      <c r="Z41" s="762"/>
+      <c r="AA41" s="762"/>
+      <c r="AB41" s="762"/>
+      <c r="AC41" s="762"/>
+      <c r="AD41" s="762"/>
+      <c r="AE41" s="762"/>
+      <c r="AF41" s="762"/>
+      <c r="AG41" s="762"/>
+      <c r="AH41" s="762"/>
+      <c r="AI41" s="762"/>
+      <c r="AJ41" s="762"/>
+      <c r="AK41" s="762"/>
+      <c r="AL41" s="762"/>
+      <c r="AM41" s="762"/>
+      <c r="AN41" s="762"/>
+      <c r="AO41" s="762"/>
+      <c r="AP41" s="762"/>
+      <c r="AQ41" s="762"/>
+      <c r="AR41" s="762"/>
+      <c r="AS41" s="762"/>
+      <c r="AT41" s="762"/>
+      <c r="AU41" s="762"/>
+      <c r="AV41" s="762"/>
+      <c r="AW41" s="762"/>
+      <c r="AX41" s="762"/>
+      <c r="AY41" s="762"/>
+      <c r="AZ41" s="762"/>
+      <c r="BA41" s="762"/>
+      <c r="BB41" s="762"/>
+      <c r="BC41" s="762"/>
+      <c r="BD41" s="762"/>
+      <c r="BE41" s="762"/>
+      <c r="BF41" s="762"/>
+      <c r="BG41" s="762"/>
+      <c r="BH41" s="762"/>
+      <c r="BI41" s="762"/>
+      <c r="BJ41" s="762"/>
+      <c r="BK41" s="762"/>
+      <c r="BL41" s="762"/>
+      <c r="BM41" s="762"/>
+      <c r="BN41" s="762"/>
+      <c r="BO41" s="762"/>
+      <c r="BP41" s="762"/>
+      <c r="BQ41" s="762"/>
+      <c r="BR41" s="762"/>
+      <c r="BS41" s="762"/>
+      <c r="BT41" s="762"/>
+      <c r="BU41" s="762"/>
+      <c r="BV41" s="762"/>
+      <c r="BW41" s="762"/>
+      <c r="BX41" s="762"/>
+      <c r="BY41" s="762"/>
+      <c r="BZ41" s="762"/>
+      <c r="CA41" s="762"/>
+      <c r="CB41" s="762"/>
+      <c r="CC41" s="762"/>
+      <c r="CD41" s="762"/>
+      <c r="CE41" s="762"/>
+      <c r="CF41" s="762"/>
+      <c r="CG41" s="762"/>
+      <c r="CH41" s="762"/>
+      <c r="CI41" s="762"/>
+      <c r="CJ41" s="762"/>
+      <c r="CK41" s="762"/>
+      <c r="CL41" s="762"/>
+      <c r="CM41" s="762"/>
+      <c r="CN41" s="762"/>
+      <c r="CO41" s="762"/>
+      <c r="CP41" s="762"/>
+      <c r="CQ41" s="762"/>
+      <c r="CR41" s="762"/>
+      <c r="CS41" s="762"/>
+      <c r="CT41" s="762"/>
+      <c r="CU41" s="762"/>
+      <c r="CV41" s="762"/>
+      <c r="CW41" s="762"/>
+      <c r="CX41" s="762"/>
+      <c r="CY41" s="762"/>
+      <c r="CZ41" s="762"/>
+      <c r="DA41" s="762"/>
+      <c r="DB41" s="762"/>
+      <c r="DC41" s="762"/>
+      <c r="DD41" s="762"/>
+      <c r="DE41" s="762"/>
+      <c r="DF41" s="762"/>
+      <c r="DG41" s="762"/>
+      <c r="DH41" s="762"/>
+      <c r="DI41" s="762"/>
+      <c r="DJ41" s="762"/>
+      <c r="DK41" s="762"/>
+      <c r="DL41" s="762"/>
+      <c r="DM41" s="762"/>
+      <c r="DN41" s="762"/>
+      <c r="DO41" s="762"/>
+      <c r="DP41" s="762"/>
+      <c r="DQ41" s="762"/>
+      <c r="DR41" s="762"/>
+      <c r="DS41" s="762"/>
+      <c r="DT41" s="762"/>
+      <c r="DU41" s="762"/>
+      <c r="DV41" s="762"/>
+      <c r="DW41" s="762"/>
+      <c r="DX41" s="762"/>
+      <c r="DY41" s="762"/>
+      <c r="DZ41" s="762"/>
+      <c r="EA41" s="762"/>
+      <c r="EB41" s="762"/>
+      <c r="EC41" s="762"/>
+      <c r="ED41" s="762"/>
+      <c r="EE41" s="762"/>
+      <c r="EF41" s="762"/>
+      <c r="EG41" s="762"/>
+      <c r="EH41" s="762"/>
+      <c r="EI41" s="762"/>
+      <c r="EJ41" s="762"/>
+      <c r="EK41" s="762"/>
+      <c r="EL41" s="762"/>
+      <c r="EM41" s="762"/>
+      <c r="EN41" s="762"/>
+      <c r="EO41" s="762"/>
+      <c r="EP41" s="762"/>
+      <c r="EQ41" s="762"/>
+      <c r="ER41" s="762"/>
+      <c r="ES41" s="762"/>
+      <c r="ET41" s="762"/>
+      <c r="EU41" s="762"/>
+      <c r="EV41" s="762"/>
+      <c r="EW41" s="762"/>
+      <c r="EX41" s="762"/>
+      <c r="EY41" s="762"/>
+      <c r="EZ41" s="762"/>
+      <c r="FA41" s="762"/>
+      <c r="FB41" s="762"/>
+      <c r="FC41" s="762"/>
+      <c r="FD41" s="762"/>
+      <c r="FE41" s="762"/>
+      <c r="FF41" s="762"/>
+      <c r="FG41" s="762"/>
+      <c r="FH41" s="762"/>
+      <c r="FI41" s="762"/>
+      <c r="FJ41" s="762"/>
+      <c r="FK41" s="762"/>
+      <c r="FL41" s="762"/>
+      <c r="FM41" s="762"/>
+      <c r="FN41" s="762"/>
+      <c r="FO41" s="762"/>
+      <c r="FP41" s="762"/>
+      <c r="FQ41" s="762"/>
+      <c r="FR41" s="762"/>
+      <c r="FS41" s="762"/>
+      <c r="FT41" s="762"/>
+      <c r="FU41" s="762"/>
+      <c r="FV41" s="762"/>
+      <c r="FW41" s="762"/>
+      <c r="FX41" s="762"/>
+      <c r="FY41" s="762"/>
+      <c r="FZ41" s="762"/>
+      <c r="GA41" s="762"/>
+      <c r="GB41" s="762"/>
+      <c r="GC41" s="762"/>
+      <c r="GD41" s="762"/>
+      <c r="GE41" s="762"/>
+      <c r="GF41" s="762"/>
+      <c r="GG41" s="762"/>
+      <c r="GH41" s="762"/>
+      <c r="GI41" s="762"/>
+      <c r="GJ41" s="762"/>
+      <c r="GK41" s="762"/>
+      <c r="GL41" s="762"/>
+      <c r="GM41" s="762"/>
+      <c r="GN41" s="762"/>
+      <c r="GO41" s="762"/>
+      <c r="GP41" s="762"/>
+      <c r="GQ41" s="762"/>
+      <c r="GR41" s="762"/>
+      <c r="GS41" s="762"/>
+      <c r="GT41" s="762"/>
+      <c r="GU41" s="762"/>
+      <c r="GV41" s="762"/>
+      <c r="GW41" s="762"/>
+      <c r="GX41" s="762"/>
+      <c r="GY41" s="762"/>
+      <c r="GZ41" s="762"/>
+      <c r="HA41" s="762"/>
+      <c r="HB41" s="762"/>
+      <c r="HC41" s="762"/>
+      <c r="HD41" s="762"/>
+      <c r="HE41" s="762"/>
+      <c r="HF41" s="762"/>
+      <c r="HG41" s="762"/>
+      <c r="HH41" s="762"/>
+      <c r="HI41" s="762"/>
+      <c r="HJ41" s="762"/>
+      <c r="HK41" s="762"/>
+      <c r="HL41" s="762"/>
+      <c r="HM41" s="762"/>
+      <c r="HN41" s="762"/>
+      <c r="HO41" s="762"/>
+      <c r="HP41" s="762"/>
+      <c r="HQ41" s="762"/>
+      <c r="HR41" s="762"/>
+      <c r="HS41" s="762"/>
+      <c r="HT41" s="762"/>
+      <c r="HU41" s="762"/>
+      <c r="HV41" s="762"/>
+      <c r="HW41" s="762"/>
+      <c r="HX41" s="762"/>
+      <c r="HY41" s="762"/>
+      <c r="HZ41" s="762"/>
+      <c r="IA41" s="762"/>
+      <c r="IB41" s="762"/>
+      <c r="IC41" s="762"/>
+      <c r="ID41" s="762"/>
+      <c r="IE41" s="762"/>
+      <c r="IF41" s="762"/>
+      <c r="IG41" s="762"/>
+      <c r="IH41" s="762"/>
+      <c r="II41" s="762"/>
+      <c r="IJ41" s="762"/>
+      <c r="IK41" s="762"/>
+      <c r="IL41" s="762"/>
+      <c r="IM41" s="762"/>
+      <c r="IN41" s="762"/>
+      <c r="IO41" s="762"/>
+      <c r="IP41" s="762"/>
+      <c r="IQ41" s="762"/>
+      <c r="IR41" s="762"/>
+      <c r="IS41" s="762"/>
+      <c r="IT41" s="762"/>
+      <c r="IU41" s="762"/>
+      <c r="IV41" s="762"/>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" s="521" t="n">

</xml_diff>

<commit_message>
fix bugs, add skill display during battle
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -21,7 +21,7 @@
   </definedNames>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="pm" day="1486449374" val="694"/>
+      <pm:revision xmlns:pm="pm" day="1486475792" val="694"/>
     </ext>
   </extLst>
 </workbook>
@@ -39958,7 +39958,7 @@
   <dimension ref="A4:IV50"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A25" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.50"/>

</xml_diff>

<commit_message>
fix bugs. add new skills
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -21,14 +21,14 @@
   </definedNames>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="pm" day="1486475792" val="694"/>
+      <pm:revision xmlns:pm="pm" day="1486539213" val="694"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="474">
   <si>
     <t>武器等级</t>
   </si>
@@ -1449,6 +1449,12 @@
   </si>
   <si>
     <t>每次攻击必暴击，生命生命恢复+100%，生命最大值+100%，攻速减慢50%</t>
+  </si>
+  <si>
+    <t>必中</t>
+  </si>
+  <si>
+    <t>每次攻击必定命中</t>
   </si>
 </sst>
 </file>
@@ -5248,7 +5254,7 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="758">
+  <cellXfs count="759">
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="1" hidden="0"/>
     </xf>
@@ -8269,6 +8275,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="1" hidden="0"/>
     </xf>
   </cellXfs>
@@ -18064,7 +18073,7 @@
   <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView view="normal" zoomScale="55" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A10" sqref="A10:IV10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="11" defaultColWidth="12.627273" defaultRowHeight="14.50"/>
@@ -18476,7 +18485,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="155" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G11" s="48" t="n">
         <v>76</v>
@@ -39955,10 +39964,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:IV50"/>
+  <dimension ref="A4:IV51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A25" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A27" zoomScale="115" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.50"/>
@@ -41601,7 +41610,7 @@
       <c r="IU41" s="757"/>
       <c r="IV41" s="757"/>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:6">
       <c r="B42" s="521" t="n">
         <v>38</v>
       </c>
@@ -41615,7 +41624,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="43" spans="2:7">
+    <row r="43" spans="2:6">
       <c r="B43" s="521" t="n">
         <v>39</v>
       </c>
@@ -41629,21 +41638,273 @@
         <v>457</v>
       </c>
     </row>
-    <row r="44" spans="2:7">
-      <c r="B44" s="521" t="n">
+    <row r="44" spans="1:256" s="758" customFormat="1">
+      <c r="A44" s="757"/>
+      <c r="B44" s="757" t="n">
         <v>40</v>
       </c>
-      <c r="C44" s="521" t="s">
+      <c r="C44" s="757" t="s">
         <v>458</v>
       </c>
-      <c r="E44" s="521" t="s">
+      <c r="D44" s="757"/>
+      <c r="E44" s="757" t="s">
         <v>399</v>
       </c>
-      <c r="F44" s="521" t="s">
+      <c r="F44" s="757" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="45" spans="2:7">
+      <c r="G44" s="757"/>
+      <c r="H44" s="757"/>
+      <c r="I44" s="757"/>
+      <c r="J44" s="757"/>
+      <c r="K44" s="757"/>
+      <c r="L44" s="757"/>
+      <c r="M44" s="757"/>
+      <c r="N44" s="757"/>
+      <c r="O44" s="757"/>
+      <c r="P44" s="757"/>
+      <c r="Q44" s="757"/>
+      <c r="R44" s="757"/>
+      <c r="S44" s="757"/>
+      <c r="T44" s="757"/>
+      <c r="U44" s="757"/>
+      <c r="V44" s="757"/>
+      <c r="W44" s="757"/>
+      <c r="X44" s="757"/>
+      <c r="Y44" s="757"/>
+      <c r="Z44" s="757"/>
+      <c r="AA44" s="757"/>
+      <c r="AB44" s="757"/>
+      <c r="AC44" s="757"/>
+      <c r="AD44" s="757"/>
+      <c r="AE44" s="757"/>
+      <c r="AF44" s="757"/>
+      <c r="AG44" s="757"/>
+      <c r="AH44" s="757"/>
+      <c r="AI44" s="757"/>
+      <c r="AJ44" s="757"/>
+      <c r="AK44" s="757"/>
+      <c r="AL44" s="757"/>
+      <c r="AM44" s="757"/>
+      <c r="AN44" s="757"/>
+      <c r="AO44" s="757"/>
+      <c r="AP44" s="757"/>
+      <c r="AQ44" s="757"/>
+      <c r="AR44" s="757"/>
+      <c r="AS44" s="757"/>
+      <c r="AT44" s="757"/>
+      <c r="AU44" s="757"/>
+      <c r="AV44" s="757"/>
+      <c r="AW44" s="757"/>
+      <c r="AX44" s="757"/>
+      <c r="AY44" s="757"/>
+      <c r="AZ44" s="757"/>
+      <c r="BA44" s="757"/>
+      <c r="BB44" s="757"/>
+      <c r="BC44" s="757"/>
+      <c r="BD44" s="757"/>
+      <c r="BE44" s="757"/>
+      <c r="BF44" s="757"/>
+      <c r="BG44" s="757"/>
+      <c r="BH44" s="757"/>
+      <c r="BI44" s="757"/>
+      <c r="BJ44" s="757"/>
+      <c r="BK44" s="757"/>
+      <c r="BL44" s="757"/>
+      <c r="BM44" s="757"/>
+      <c r="BN44" s="757"/>
+      <c r="BO44" s="757"/>
+      <c r="BP44" s="757"/>
+      <c r="BQ44" s="757"/>
+      <c r="BR44" s="757"/>
+      <c r="BS44" s="757"/>
+      <c r="BT44" s="757"/>
+      <c r="BU44" s="757"/>
+      <c r="BV44" s="757"/>
+      <c r="BW44" s="757"/>
+      <c r="BX44" s="757"/>
+      <c r="BY44" s="757"/>
+      <c r="BZ44" s="757"/>
+      <c r="CA44" s="757"/>
+      <c r="CB44" s="757"/>
+      <c r="CC44" s="757"/>
+      <c r="CD44" s="757"/>
+      <c r="CE44" s="757"/>
+      <c r="CF44" s="757"/>
+      <c r="CG44" s="757"/>
+      <c r="CH44" s="757"/>
+      <c r="CI44" s="757"/>
+      <c r="CJ44" s="757"/>
+      <c r="CK44" s="757"/>
+      <c r="CL44" s="757"/>
+      <c r="CM44" s="757"/>
+      <c r="CN44" s="757"/>
+      <c r="CO44" s="757"/>
+      <c r="CP44" s="757"/>
+      <c r="CQ44" s="757"/>
+      <c r="CR44" s="757"/>
+      <c r="CS44" s="757"/>
+      <c r="CT44" s="757"/>
+      <c r="CU44" s="757"/>
+      <c r="CV44" s="757"/>
+      <c r="CW44" s="757"/>
+      <c r="CX44" s="757"/>
+      <c r="CY44" s="757"/>
+      <c r="CZ44" s="757"/>
+      <c r="DA44" s="757"/>
+      <c r="DB44" s="757"/>
+      <c r="DC44" s="757"/>
+      <c r="DD44" s="757"/>
+      <c r="DE44" s="757"/>
+      <c r="DF44" s="757"/>
+      <c r="DG44" s="757"/>
+      <c r="DH44" s="757"/>
+      <c r="DI44" s="757"/>
+      <c r="DJ44" s="757"/>
+      <c r="DK44" s="757"/>
+      <c r="DL44" s="757"/>
+      <c r="DM44" s="757"/>
+      <c r="DN44" s="757"/>
+      <c r="DO44" s="757"/>
+      <c r="DP44" s="757"/>
+      <c r="DQ44" s="757"/>
+      <c r="DR44" s="757"/>
+      <c r="DS44" s="757"/>
+      <c r="DT44" s="757"/>
+      <c r="DU44" s="757"/>
+      <c r="DV44" s="757"/>
+      <c r="DW44" s="757"/>
+      <c r="DX44" s="757"/>
+      <c r="DY44" s="757"/>
+      <c r="DZ44" s="757"/>
+      <c r="EA44" s="757"/>
+      <c r="EB44" s="757"/>
+      <c r="EC44" s="757"/>
+      <c r="ED44" s="757"/>
+      <c r="EE44" s="757"/>
+      <c r="EF44" s="757"/>
+      <c r="EG44" s="757"/>
+      <c r="EH44" s="757"/>
+      <c r="EI44" s="757"/>
+      <c r="EJ44" s="757"/>
+      <c r="EK44" s="757"/>
+      <c r="EL44" s="757"/>
+      <c r="EM44" s="757"/>
+      <c r="EN44" s="757"/>
+      <c r="EO44" s="757"/>
+      <c r="EP44" s="757"/>
+      <c r="EQ44" s="757"/>
+      <c r="ER44" s="757"/>
+      <c r="ES44" s="757"/>
+      <c r="ET44" s="757"/>
+      <c r="EU44" s="757"/>
+      <c r="EV44" s="757"/>
+      <c r="EW44" s="757"/>
+      <c r="EX44" s="757"/>
+      <c r="EY44" s="757"/>
+      <c r="EZ44" s="757"/>
+      <c r="FA44" s="757"/>
+      <c r="FB44" s="757"/>
+      <c r="FC44" s="757"/>
+      <c r="FD44" s="757"/>
+      <c r="FE44" s="757"/>
+      <c r="FF44" s="757"/>
+      <c r="FG44" s="757"/>
+      <c r="FH44" s="757"/>
+      <c r="FI44" s="757"/>
+      <c r="FJ44" s="757"/>
+      <c r="FK44" s="757"/>
+      <c r="FL44" s="757"/>
+      <c r="FM44" s="757"/>
+      <c r="FN44" s="757"/>
+      <c r="FO44" s="757"/>
+      <c r="FP44" s="757"/>
+      <c r="FQ44" s="757"/>
+      <c r="FR44" s="757"/>
+      <c r="FS44" s="757"/>
+      <c r="FT44" s="757"/>
+      <c r="FU44" s="757"/>
+      <c r="FV44" s="757"/>
+      <c r="FW44" s="757"/>
+      <c r="FX44" s="757"/>
+      <c r="FY44" s="757"/>
+      <c r="FZ44" s="757"/>
+      <c r="GA44" s="757"/>
+      <c r="GB44" s="757"/>
+      <c r="GC44" s="757"/>
+      <c r="GD44" s="757"/>
+      <c r="GE44" s="757"/>
+      <c r="GF44" s="757"/>
+      <c r="GG44" s="757"/>
+      <c r="GH44" s="757"/>
+      <c r="GI44" s="757"/>
+      <c r="GJ44" s="757"/>
+      <c r="GK44" s="757"/>
+      <c r="GL44" s="757"/>
+      <c r="GM44" s="757"/>
+      <c r="GN44" s="757"/>
+      <c r="GO44" s="757"/>
+      <c r="GP44" s="757"/>
+      <c r="GQ44" s="757"/>
+      <c r="GR44" s="757"/>
+      <c r="GS44" s="757"/>
+      <c r="GT44" s="757"/>
+      <c r="GU44" s="757"/>
+      <c r="GV44" s="757"/>
+      <c r="GW44" s="757"/>
+      <c r="GX44" s="757"/>
+      <c r="GY44" s="757"/>
+      <c r="GZ44" s="757"/>
+      <c r="HA44" s="757"/>
+      <c r="HB44" s="757"/>
+      <c r="HC44" s="757"/>
+      <c r="HD44" s="757"/>
+      <c r="HE44" s="757"/>
+      <c r="HF44" s="757"/>
+      <c r="HG44" s="757"/>
+      <c r="HH44" s="757"/>
+      <c r="HI44" s="757"/>
+      <c r="HJ44" s="757"/>
+      <c r="HK44" s="757"/>
+      <c r="HL44" s="757"/>
+      <c r="HM44" s="757"/>
+      <c r="HN44" s="757"/>
+      <c r="HO44" s="757"/>
+      <c r="HP44" s="757"/>
+      <c r="HQ44" s="757"/>
+      <c r="HR44" s="757"/>
+      <c r="HS44" s="757"/>
+      <c r="HT44" s="757"/>
+      <c r="HU44" s="757"/>
+      <c r="HV44" s="757"/>
+      <c r="HW44" s="757"/>
+      <c r="HX44" s="757"/>
+      <c r="HY44" s="757"/>
+      <c r="HZ44" s="757"/>
+      <c r="IA44" s="757"/>
+      <c r="IB44" s="757"/>
+      <c r="IC44" s="757"/>
+      <c r="ID44" s="757"/>
+      <c r="IE44" s="757"/>
+      <c r="IF44" s="757"/>
+      <c r="IG44" s="757"/>
+      <c r="IH44" s="757"/>
+      <c r="II44" s="757"/>
+      <c r="IJ44" s="757"/>
+      <c r="IK44" s="757"/>
+      <c r="IL44" s="757"/>
+      <c r="IM44" s="757"/>
+      <c r="IN44" s="757"/>
+      <c r="IO44" s="757"/>
+      <c r="IP44" s="757"/>
+      <c r="IQ44" s="757"/>
+      <c r="IR44" s="757"/>
+      <c r="IS44" s="757"/>
+      <c r="IT44" s="757"/>
+      <c r="IU44" s="757"/>
+      <c r="IV44" s="757"/>
+    </row>
+    <row r="45" spans="2:6">
       <c r="B45" s="521" t="n">
         <v>41</v>
       </c>
@@ -41685,46 +41946,816 @@
         <v>465</v>
       </c>
     </row>
-    <row r="48" spans="2:6">
-      <c r="B48" s="521" t="n">
+    <row r="48" spans="1:256" s="758" customFormat="1">
+      <c r="A48" s="757"/>
+      <c r="B48" s="757" t="n">
         <v>44</v>
       </c>
-      <c r="C48" s="521" t="s">
+      <c r="C48" s="757" t="s">
         <v>466</v>
       </c>
-      <c r="E48" s="521" t="s">
+      <c r="D48" s="757"/>
+      <c r="E48" s="757" t="s">
         <v>399</v>
       </c>
-      <c r="F48" s="521" t="s">
+      <c r="F48" s="757" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="49" spans="2:6">
-      <c r="B49" s="521" t="n">
+      <c r="G48" s="757"/>
+      <c r="H48" s="757"/>
+      <c r="I48" s="757"/>
+      <c r="J48" s="757"/>
+      <c r="K48" s="757"/>
+      <c r="L48" s="757"/>
+      <c r="M48" s="757"/>
+      <c r="N48" s="757"/>
+      <c r="O48" s="757"/>
+      <c r="P48" s="757"/>
+      <c r="Q48" s="757"/>
+      <c r="R48" s="757"/>
+      <c r="S48" s="757"/>
+      <c r="T48" s="757"/>
+      <c r="U48" s="757"/>
+      <c r="V48" s="757"/>
+      <c r="W48" s="757"/>
+      <c r="X48" s="757"/>
+      <c r="Y48" s="757"/>
+      <c r="Z48" s="757"/>
+      <c r="AA48" s="757"/>
+      <c r="AB48" s="757"/>
+      <c r="AC48" s="757"/>
+      <c r="AD48" s="757"/>
+      <c r="AE48" s="757"/>
+      <c r="AF48" s="757"/>
+      <c r="AG48" s="757"/>
+      <c r="AH48" s="757"/>
+      <c r="AI48" s="757"/>
+      <c r="AJ48" s="757"/>
+      <c r="AK48" s="757"/>
+      <c r="AL48" s="757"/>
+      <c r="AM48" s="757"/>
+      <c r="AN48" s="757"/>
+      <c r="AO48" s="757"/>
+      <c r="AP48" s="757"/>
+      <c r="AQ48" s="757"/>
+      <c r="AR48" s="757"/>
+      <c r="AS48" s="757"/>
+      <c r="AT48" s="757"/>
+      <c r="AU48" s="757"/>
+      <c r="AV48" s="757"/>
+      <c r="AW48" s="757"/>
+      <c r="AX48" s="757"/>
+      <c r="AY48" s="757"/>
+      <c r="AZ48" s="757"/>
+      <c r="BA48" s="757"/>
+      <c r="BB48" s="757"/>
+      <c r="BC48" s="757"/>
+      <c r="BD48" s="757"/>
+      <c r="BE48" s="757"/>
+      <c r="BF48" s="757"/>
+      <c r="BG48" s="757"/>
+      <c r="BH48" s="757"/>
+      <c r="BI48" s="757"/>
+      <c r="BJ48" s="757"/>
+      <c r="BK48" s="757"/>
+      <c r="BL48" s="757"/>
+      <c r="BM48" s="757"/>
+      <c r="BN48" s="757"/>
+      <c r="BO48" s="757"/>
+      <c r="BP48" s="757"/>
+      <c r="BQ48" s="757"/>
+      <c r="BR48" s="757"/>
+      <c r="BS48" s="757"/>
+      <c r="BT48" s="757"/>
+      <c r="BU48" s="757"/>
+      <c r="BV48" s="757"/>
+      <c r="BW48" s="757"/>
+      <c r="BX48" s="757"/>
+      <c r="BY48" s="757"/>
+      <c r="BZ48" s="757"/>
+      <c r="CA48" s="757"/>
+      <c r="CB48" s="757"/>
+      <c r="CC48" s="757"/>
+      <c r="CD48" s="757"/>
+      <c r="CE48" s="757"/>
+      <c r="CF48" s="757"/>
+      <c r="CG48" s="757"/>
+      <c r="CH48" s="757"/>
+      <c r="CI48" s="757"/>
+      <c r="CJ48" s="757"/>
+      <c r="CK48" s="757"/>
+      <c r="CL48" s="757"/>
+      <c r="CM48" s="757"/>
+      <c r="CN48" s="757"/>
+      <c r="CO48" s="757"/>
+      <c r="CP48" s="757"/>
+      <c r="CQ48" s="757"/>
+      <c r="CR48" s="757"/>
+      <c r="CS48" s="757"/>
+      <c r="CT48" s="757"/>
+      <c r="CU48" s="757"/>
+      <c r="CV48" s="757"/>
+      <c r="CW48" s="757"/>
+      <c r="CX48" s="757"/>
+      <c r="CY48" s="757"/>
+      <c r="CZ48" s="757"/>
+      <c r="DA48" s="757"/>
+      <c r="DB48" s="757"/>
+      <c r="DC48" s="757"/>
+      <c r="DD48" s="757"/>
+      <c r="DE48" s="757"/>
+      <c r="DF48" s="757"/>
+      <c r="DG48" s="757"/>
+      <c r="DH48" s="757"/>
+      <c r="DI48" s="757"/>
+      <c r="DJ48" s="757"/>
+      <c r="DK48" s="757"/>
+      <c r="DL48" s="757"/>
+      <c r="DM48" s="757"/>
+      <c r="DN48" s="757"/>
+      <c r="DO48" s="757"/>
+      <c r="DP48" s="757"/>
+      <c r="DQ48" s="757"/>
+      <c r="DR48" s="757"/>
+      <c r="DS48" s="757"/>
+      <c r="DT48" s="757"/>
+      <c r="DU48" s="757"/>
+      <c r="DV48" s="757"/>
+      <c r="DW48" s="757"/>
+      <c r="DX48" s="757"/>
+      <c r="DY48" s="757"/>
+      <c r="DZ48" s="757"/>
+      <c r="EA48" s="757"/>
+      <c r="EB48" s="757"/>
+      <c r="EC48" s="757"/>
+      <c r="ED48" s="757"/>
+      <c r="EE48" s="757"/>
+      <c r="EF48" s="757"/>
+      <c r="EG48" s="757"/>
+      <c r="EH48" s="757"/>
+      <c r="EI48" s="757"/>
+      <c r="EJ48" s="757"/>
+      <c r="EK48" s="757"/>
+      <c r="EL48" s="757"/>
+      <c r="EM48" s="757"/>
+      <c r="EN48" s="757"/>
+      <c r="EO48" s="757"/>
+      <c r="EP48" s="757"/>
+      <c r="EQ48" s="757"/>
+      <c r="ER48" s="757"/>
+      <c r="ES48" s="757"/>
+      <c r="ET48" s="757"/>
+      <c r="EU48" s="757"/>
+      <c r="EV48" s="757"/>
+      <c r="EW48" s="757"/>
+      <c r="EX48" s="757"/>
+      <c r="EY48" s="757"/>
+      <c r="EZ48" s="757"/>
+      <c r="FA48" s="757"/>
+      <c r="FB48" s="757"/>
+      <c r="FC48" s="757"/>
+      <c r="FD48" s="757"/>
+      <c r="FE48" s="757"/>
+      <c r="FF48" s="757"/>
+      <c r="FG48" s="757"/>
+      <c r="FH48" s="757"/>
+      <c r="FI48" s="757"/>
+      <c r="FJ48" s="757"/>
+      <c r="FK48" s="757"/>
+      <c r="FL48" s="757"/>
+      <c r="FM48" s="757"/>
+      <c r="FN48" s="757"/>
+      <c r="FO48" s="757"/>
+      <c r="FP48" s="757"/>
+      <c r="FQ48" s="757"/>
+      <c r="FR48" s="757"/>
+      <c r="FS48" s="757"/>
+      <c r="FT48" s="757"/>
+      <c r="FU48" s="757"/>
+      <c r="FV48" s="757"/>
+      <c r="FW48" s="757"/>
+      <c r="FX48" s="757"/>
+      <c r="FY48" s="757"/>
+      <c r="FZ48" s="757"/>
+      <c r="GA48" s="757"/>
+      <c r="GB48" s="757"/>
+      <c r="GC48" s="757"/>
+      <c r="GD48" s="757"/>
+      <c r="GE48" s="757"/>
+      <c r="GF48" s="757"/>
+      <c r="GG48" s="757"/>
+      <c r="GH48" s="757"/>
+      <c r="GI48" s="757"/>
+      <c r="GJ48" s="757"/>
+      <c r="GK48" s="757"/>
+      <c r="GL48" s="757"/>
+      <c r="GM48" s="757"/>
+      <c r="GN48" s="757"/>
+      <c r="GO48" s="757"/>
+      <c r="GP48" s="757"/>
+      <c r="GQ48" s="757"/>
+      <c r="GR48" s="757"/>
+      <c r="GS48" s="757"/>
+      <c r="GT48" s="757"/>
+      <c r="GU48" s="757"/>
+      <c r="GV48" s="757"/>
+      <c r="GW48" s="757"/>
+      <c r="GX48" s="757"/>
+      <c r="GY48" s="757"/>
+      <c r="GZ48" s="757"/>
+      <c r="HA48" s="757"/>
+      <c r="HB48" s="757"/>
+      <c r="HC48" s="757"/>
+      <c r="HD48" s="757"/>
+      <c r="HE48" s="757"/>
+      <c r="HF48" s="757"/>
+      <c r="HG48" s="757"/>
+      <c r="HH48" s="757"/>
+      <c r="HI48" s="757"/>
+      <c r="HJ48" s="757"/>
+      <c r="HK48" s="757"/>
+      <c r="HL48" s="757"/>
+      <c r="HM48" s="757"/>
+      <c r="HN48" s="757"/>
+      <c r="HO48" s="757"/>
+      <c r="HP48" s="757"/>
+      <c r="HQ48" s="757"/>
+      <c r="HR48" s="757"/>
+      <c r="HS48" s="757"/>
+      <c r="HT48" s="757"/>
+      <c r="HU48" s="757"/>
+      <c r="HV48" s="757"/>
+      <c r="HW48" s="757"/>
+      <c r="HX48" s="757"/>
+      <c r="HY48" s="757"/>
+      <c r="HZ48" s="757"/>
+      <c r="IA48" s="757"/>
+      <c r="IB48" s="757"/>
+      <c r="IC48" s="757"/>
+      <c r="ID48" s="757"/>
+      <c r="IE48" s="757"/>
+      <c r="IF48" s="757"/>
+      <c r="IG48" s="757"/>
+      <c r="IH48" s="757"/>
+      <c r="II48" s="757"/>
+      <c r="IJ48" s="757"/>
+      <c r="IK48" s="757"/>
+      <c r="IL48" s="757"/>
+      <c r="IM48" s="757"/>
+      <c r="IN48" s="757"/>
+      <c r="IO48" s="757"/>
+      <c r="IP48" s="757"/>
+      <c r="IQ48" s="757"/>
+      <c r="IR48" s="757"/>
+      <c r="IS48" s="757"/>
+      <c r="IT48" s="757"/>
+      <c r="IU48" s="757"/>
+      <c r="IV48" s="757"/>
+    </row>
+    <row r="49" spans="1:256" s="758" customFormat="1">
+      <c r="A49" s="757"/>
+      <c r="B49" s="757" t="n">
         <v>45</v>
       </c>
-      <c r="C49" s="521" t="s">
+      <c r="C49" s="757" t="s">
         <v>468</v>
       </c>
-      <c r="E49" s="521" t="s">
+      <c r="D49" s="757"/>
+      <c r="E49" s="757" t="s">
         <v>399</v>
       </c>
-      <c r="F49" s="521" t="s">
+      <c r="F49" s="757" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="50" spans="2:6">
-      <c r="B50" s="521" t="n">
+      <c r="G49" s="757"/>
+      <c r="H49" s="757"/>
+      <c r="I49" s="757"/>
+      <c r="J49" s="757"/>
+      <c r="K49" s="757"/>
+      <c r="L49" s="757"/>
+      <c r="M49" s="757"/>
+      <c r="N49" s="757"/>
+      <c r="O49" s="757"/>
+      <c r="P49" s="757"/>
+      <c r="Q49" s="757"/>
+      <c r="R49" s="757"/>
+      <c r="S49" s="757"/>
+      <c r="T49" s="757"/>
+      <c r="U49" s="757"/>
+      <c r="V49" s="757"/>
+      <c r="W49" s="757"/>
+      <c r="X49" s="757"/>
+      <c r="Y49" s="757"/>
+      <c r="Z49" s="757"/>
+      <c r="AA49" s="757"/>
+      <c r="AB49" s="757"/>
+      <c r="AC49" s="757"/>
+      <c r="AD49" s="757"/>
+      <c r="AE49" s="757"/>
+      <c r="AF49" s="757"/>
+      <c r="AG49" s="757"/>
+      <c r="AH49" s="757"/>
+      <c r="AI49" s="757"/>
+      <c r="AJ49" s="757"/>
+      <c r="AK49" s="757"/>
+      <c r="AL49" s="757"/>
+      <c r="AM49" s="757"/>
+      <c r="AN49" s="757"/>
+      <c r="AO49" s="757"/>
+      <c r="AP49" s="757"/>
+      <c r="AQ49" s="757"/>
+      <c r="AR49" s="757"/>
+      <c r="AS49" s="757"/>
+      <c r="AT49" s="757"/>
+      <c r="AU49" s="757"/>
+      <c r="AV49" s="757"/>
+      <c r="AW49" s="757"/>
+      <c r="AX49" s="757"/>
+      <c r="AY49" s="757"/>
+      <c r="AZ49" s="757"/>
+      <c r="BA49" s="757"/>
+      <c r="BB49" s="757"/>
+      <c r="BC49" s="757"/>
+      <c r="BD49" s="757"/>
+      <c r="BE49" s="757"/>
+      <c r="BF49" s="757"/>
+      <c r="BG49" s="757"/>
+      <c r="BH49" s="757"/>
+      <c r="BI49" s="757"/>
+      <c r="BJ49" s="757"/>
+      <c r="BK49" s="757"/>
+      <c r="BL49" s="757"/>
+      <c r="BM49" s="757"/>
+      <c r="BN49" s="757"/>
+      <c r="BO49" s="757"/>
+      <c r="BP49" s="757"/>
+      <c r="BQ49" s="757"/>
+      <c r="BR49" s="757"/>
+      <c r="BS49" s="757"/>
+      <c r="BT49" s="757"/>
+      <c r="BU49" s="757"/>
+      <c r="BV49" s="757"/>
+      <c r="BW49" s="757"/>
+      <c r="BX49" s="757"/>
+      <c r="BY49" s="757"/>
+      <c r="BZ49" s="757"/>
+      <c r="CA49" s="757"/>
+      <c r="CB49" s="757"/>
+      <c r="CC49" s="757"/>
+      <c r="CD49" s="757"/>
+      <c r="CE49" s="757"/>
+      <c r="CF49" s="757"/>
+      <c r="CG49" s="757"/>
+      <c r="CH49" s="757"/>
+      <c r="CI49" s="757"/>
+      <c r="CJ49" s="757"/>
+      <c r="CK49" s="757"/>
+      <c r="CL49" s="757"/>
+      <c r="CM49" s="757"/>
+      <c r="CN49" s="757"/>
+      <c r="CO49" s="757"/>
+      <c r="CP49" s="757"/>
+      <c r="CQ49" s="757"/>
+      <c r="CR49" s="757"/>
+      <c r="CS49" s="757"/>
+      <c r="CT49" s="757"/>
+      <c r="CU49" s="757"/>
+      <c r="CV49" s="757"/>
+      <c r="CW49" s="757"/>
+      <c r="CX49" s="757"/>
+      <c r="CY49" s="757"/>
+      <c r="CZ49" s="757"/>
+      <c r="DA49" s="757"/>
+      <c r="DB49" s="757"/>
+      <c r="DC49" s="757"/>
+      <c r="DD49" s="757"/>
+      <c r="DE49" s="757"/>
+      <c r="DF49" s="757"/>
+      <c r="DG49" s="757"/>
+      <c r="DH49" s="757"/>
+      <c r="DI49" s="757"/>
+      <c r="DJ49" s="757"/>
+      <c r="DK49" s="757"/>
+      <c r="DL49" s="757"/>
+      <c r="DM49" s="757"/>
+      <c r="DN49" s="757"/>
+      <c r="DO49" s="757"/>
+      <c r="DP49" s="757"/>
+      <c r="DQ49" s="757"/>
+      <c r="DR49" s="757"/>
+      <c r="DS49" s="757"/>
+      <c r="DT49" s="757"/>
+      <c r="DU49" s="757"/>
+      <c r="DV49" s="757"/>
+      <c r="DW49" s="757"/>
+      <c r="DX49" s="757"/>
+      <c r="DY49" s="757"/>
+      <c r="DZ49" s="757"/>
+      <c r="EA49" s="757"/>
+      <c r="EB49" s="757"/>
+      <c r="EC49" s="757"/>
+      <c r="ED49" s="757"/>
+      <c r="EE49" s="757"/>
+      <c r="EF49" s="757"/>
+      <c r="EG49" s="757"/>
+      <c r="EH49" s="757"/>
+      <c r="EI49" s="757"/>
+      <c r="EJ49" s="757"/>
+      <c r="EK49" s="757"/>
+      <c r="EL49" s="757"/>
+      <c r="EM49" s="757"/>
+      <c r="EN49" s="757"/>
+      <c r="EO49" s="757"/>
+      <c r="EP49" s="757"/>
+      <c r="EQ49" s="757"/>
+      <c r="ER49" s="757"/>
+      <c r="ES49" s="757"/>
+      <c r="ET49" s="757"/>
+      <c r="EU49" s="757"/>
+      <c r="EV49" s="757"/>
+      <c r="EW49" s="757"/>
+      <c r="EX49" s="757"/>
+      <c r="EY49" s="757"/>
+      <c r="EZ49" s="757"/>
+      <c r="FA49" s="757"/>
+      <c r="FB49" s="757"/>
+      <c r="FC49" s="757"/>
+      <c r="FD49" s="757"/>
+      <c r="FE49" s="757"/>
+      <c r="FF49" s="757"/>
+      <c r="FG49" s="757"/>
+      <c r="FH49" s="757"/>
+      <c r="FI49" s="757"/>
+      <c r="FJ49" s="757"/>
+      <c r="FK49" s="757"/>
+      <c r="FL49" s="757"/>
+      <c r="FM49" s="757"/>
+      <c r="FN49" s="757"/>
+      <c r="FO49" s="757"/>
+      <c r="FP49" s="757"/>
+      <c r="FQ49" s="757"/>
+      <c r="FR49" s="757"/>
+      <c r="FS49" s="757"/>
+      <c r="FT49" s="757"/>
+      <c r="FU49" s="757"/>
+      <c r="FV49" s="757"/>
+      <c r="FW49" s="757"/>
+      <c r="FX49" s="757"/>
+      <c r="FY49" s="757"/>
+      <c r="FZ49" s="757"/>
+      <c r="GA49" s="757"/>
+      <c r="GB49" s="757"/>
+      <c r="GC49" s="757"/>
+      <c r="GD49" s="757"/>
+      <c r="GE49" s="757"/>
+      <c r="GF49" s="757"/>
+      <c r="GG49" s="757"/>
+      <c r="GH49" s="757"/>
+      <c r="GI49" s="757"/>
+      <c r="GJ49" s="757"/>
+      <c r="GK49" s="757"/>
+      <c r="GL49" s="757"/>
+      <c r="GM49" s="757"/>
+      <c r="GN49" s="757"/>
+      <c r="GO49" s="757"/>
+      <c r="GP49" s="757"/>
+      <c r="GQ49" s="757"/>
+      <c r="GR49" s="757"/>
+      <c r="GS49" s="757"/>
+      <c r="GT49" s="757"/>
+      <c r="GU49" s="757"/>
+      <c r="GV49" s="757"/>
+      <c r="GW49" s="757"/>
+      <c r="GX49" s="757"/>
+      <c r="GY49" s="757"/>
+      <c r="GZ49" s="757"/>
+      <c r="HA49" s="757"/>
+      <c r="HB49" s="757"/>
+      <c r="HC49" s="757"/>
+      <c r="HD49" s="757"/>
+      <c r="HE49" s="757"/>
+      <c r="HF49" s="757"/>
+      <c r="HG49" s="757"/>
+      <c r="HH49" s="757"/>
+      <c r="HI49" s="757"/>
+      <c r="HJ49" s="757"/>
+      <c r="HK49" s="757"/>
+      <c r="HL49" s="757"/>
+      <c r="HM49" s="757"/>
+      <c r="HN49" s="757"/>
+      <c r="HO49" s="757"/>
+      <c r="HP49" s="757"/>
+      <c r="HQ49" s="757"/>
+      <c r="HR49" s="757"/>
+      <c r="HS49" s="757"/>
+      <c r="HT49" s="757"/>
+      <c r="HU49" s="757"/>
+      <c r="HV49" s="757"/>
+      <c r="HW49" s="757"/>
+      <c r="HX49" s="757"/>
+      <c r="HY49" s="757"/>
+      <c r="HZ49" s="757"/>
+      <c r="IA49" s="757"/>
+      <c r="IB49" s="757"/>
+      <c r="IC49" s="757"/>
+      <c r="ID49" s="757"/>
+      <c r="IE49" s="757"/>
+      <c r="IF49" s="757"/>
+      <c r="IG49" s="757"/>
+      <c r="IH49" s="757"/>
+      <c r="II49" s="757"/>
+      <c r="IJ49" s="757"/>
+      <c r="IK49" s="757"/>
+      <c r="IL49" s="757"/>
+      <c r="IM49" s="757"/>
+      <c r="IN49" s="757"/>
+      <c r="IO49" s="757"/>
+      <c r="IP49" s="757"/>
+      <c r="IQ49" s="757"/>
+      <c r="IR49" s="757"/>
+      <c r="IS49" s="757"/>
+      <c r="IT49" s="757"/>
+      <c r="IU49" s="757"/>
+      <c r="IV49" s="757"/>
+    </row>
+    <row r="50" spans="1:256" s="758" customFormat="1">
+      <c r="A50" s="757"/>
+      <c r="B50" s="757" t="n">
         <v>46</v>
       </c>
-      <c r="C50" s="521" t="s">
+      <c r="C50" s="757" t="s">
         <v>470</v>
       </c>
-      <c r="E50" s="521" t="s">
+      <c r="D50" s="757"/>
+      <c r="E50" s="757" t="s">
         <v>399</v>
       </c>
-      <c r="F50" s="521" t="s">
+      <c r="F50" s="757" t="s">
         <v>471</v>
+      </c>
+      <c r="G50" s="757"/>
+      <c r="H50" s="757"/>
+      <c r="I50" s="757"/>
+      <c r="J50" s="757"/>
+      <c r="K50" s="757"/>
+      <c r="L50" s="757"/>
+      <c r="M50" s="757"/>
+      <c r="N50" s="757"/>
+      <c r="O50" s="757"/>
+      <c r="P50" s="757"/>
+      <c r="Q50" s="757"/>
+      <c r="R50" s="757"/>
+      <c r="S50" s="757"/>
+      <c r="T50" s="757"/>
+      <c r="U50" s="757"/>
+      <c r="V50" s="757"/>
+      <c r="W50" s="757"/>
+      <c r="X50" s="757"/>
+      <c r="Y50" s="757"/>
+      <c r="Z50" s="757"/>
+      <c r="AA50" s="757"/>
+      <c r="AB50" s="757"/>
+      <c r="AC50" s="757"/>
+      <c r="AD50" s="757"/>
+      <c r="AE50" s="757"/>
+      <c r="AF50" s="757"/>
+      <c r="AG50" s="757"/>
+      <c r="AH50" s="757"/>
+      <c r="AI50" s="757"/>
+      <c r="AJ50" s="757"/>
+      <c r="AK50" s="757"/>
+      <c r="AL50" s="757"/>
+      <c r="AM50" s="757"/>
+      <c r="AN50" s="757"/>
+      <c r="AO50" s="757"/>
+      <c r="AP50" s="757"/>
+      <c r="AQ50" s="757"/>
+      <c r="AR50" s="757"/>
+      <c r="AS50" s="757"/>
+      <c r="AT50" s="757"/>
+      <c r="AU50" s="757"/>
+      <c r="AV50" s="757"/>
+      <c r="AW50" s="757"/>
+      <c r="AX50" s="757"/>
+      <c r="AY50" s="757"/>
+      <c r="AZ50" s="757"/>
+      <c r="BA50" s="757"/>
+      <c r="BB50" s="757"/>
+      <c r="BC50" s="757"/>
+      <c r="BD50" s="757"/>
+      <c r="BE50" s="757"/>
+      <c r="BF50" s="757"/>
+      <c r="BG50" s="757"/>
+      <c r="BH50" s="757"/>
+      <c r="BI50" s="757"/>
+      <c r="BJ50" s="757"/>
+      <c r="BK50" s="757"/>
+      <c r="BL50" s="757"/>
+      <c r="BM50" s="757"/>
+      <c r="BN50" s="757"/>
+      <c r="BO50" s="757"/>
+      <c r="BP50" s="757"/>
+      <c r="BQ50" s="757"/>
+      <c r="BR50" s="757"/>
+      <c r="BS50" s="757"/>
+      <c r="BT50" s="757"/>
+      <c r="BU50" s="757"/>
+      <c r="BV50" s="757"/>
+      <c r="BW50" s="757"/>
+      <c r="BX50" s="757"/>
+      <c r="BY50" s="757"/>
+      <c r="BZ50" s="757"/>
+      <c r="CA50" s="757"/>
+      <c r="CB50" s="757"/>
+      <c r="CC50" s="757"/>
+      <c r="CD50" s="757"/>
+      <c r="CE50" s="757"/>
+      <c r="CF50" s="757"/>
+      <c r="CG50" s="757"/>
+      <c r="CH50" s="757"/>
+      <c r="CI50" s="757"/>
+      <c r="CJ50" s="757"/>
+      <c r="CK50" s="757"/>
+      <c r="CL50" s="757"/>
+      <c r="CM50" s="757"/>
+      <c r="CN50" s="757"/>
+      <c r="CO50" s="757"/>
+      <c r="CP50" s="757"/>
+      <c r="CQ50" s="757"/>
+      <c r="CR50" s="757"/>
+      <c r="CS50" s="757"/>
+      <c r="CT50" s="757"/>
+      <c r="CU50" s="757"/>
+      <c r="CV50" s="757"/>
+      <c r="CW50" s="757"/>
+      <c r="CX50" s="757"/>
+      <c r="CY50" s="757"/>
+      <c r="CZ50" s="757"/>
+      <c r="DA50" s="757"/>
+      <c r="DB50" s="757"/>
+      <c r="DC50" s="757"/>
+      <c r="DD50" s="757"/>
+      <c r="DE50" s="757"/>
+      <c r="DF50" s="757"/>
+      <c r="DG50" s="757"/>
+      <c r="DH50" s="757"/>
+      <c r="DI50" s="757"/>
+      <c r="DJ50" s="757"/>
+      <c r="DK50" s="757"/>
+      <c r="DL50" s="757"/>
+      <c r="DM50" s="757"/>
+      <c r="DN50" s="757"/>
+      <c r="DO50" s="757"/>
+      <c r="DP50" s="757"/>
+      <c r="DQ50" s="757"/>
+      <c r="DR50" s="757"/>
+      <c r="DS50" s="757"/>
+      <c r="DT50" s="757"/>
+      <c r="DU50" s="757"/>
+      <c r="DV50" s="757"/>
+      <c r="DW50" s="757"/>
+      <c r="DX50" s="757"/>
+      <c r="DY50" s="757"/>
+      <c r="DZ50" s="757"/>
+      <c r="EA50" s="757"/>
+      <c r="EB50" s="757"/>
+      <c r="EC50" s="757"/>
+      <c r="ED50" s="757"/>
+      <c r="EE50" s="757"/>
+      <c r="EF50" s="757"/>
+      <c r="EG50" s="757"/>
+      <c r="EH50" s="757"/>
+      <c r="EI50" s="757"/>
+      <c r="EJ50" s="757"/>
+      <c r="EK50" s="757"/>
+      <c r="EL50" s="757"/>
+      <c r="EM50" s="757"/>
+      <c r="EN50" s="757"/>
+      <c r="EO50" s="757"/>
+      <c r="EP50" s="757"/>
+      <c r="EQ50" s="757"/>
+      <c r="ER50" s="757"/>
+      <c r="ES50" s="757"/>
+      <c r="ET50" s="757"/>
+      <c r="EU50" s="757"/>
+      <c r="EV50" s="757"/>
+      <c r="EW50" s="757"/>
+      <c r="EX50" s="757"/>
+      <c r="EY50" s="757"/>
+      <c r="EZ50" s="757"/>
+      <c r="FA50" s="757"/>
+      <c r="FB50" s="757"/>
+      <c r="FC50" s="757"/>
+      <c r="FD50" s="757"/>
+      <c r="FE50" s="757"/>
+      <c r="FF50" s="757"/>
+      <c r="FG50" s="757"/>
+      <c r="FH50" s="757"/>
+      <c r="FI50" s="757"/>
+      <c r="FJ50" s="757"/>
+      <c r="FK50" s="757"/>
+      <c r="FL50" s="757"/>
+      <c r="FM50" s="757"/>
+      <c r="FN50" s="757"/>
+      <c r="FO50" s="757"/>
+      <c r="FP50" s="757"/>
+      <c r="FQ50" s="757"/>
+      <c r="FR50" s="757"/>
+      <c r="FS50" s="757"/>
+      <c r="FT50" s="757"/>
+      <c r="FU50" s="757"/>
+      <c r="FV50" s="757"/>
+      <c r="FW50" s="757"/>
+      <c r="FX50" s="757"/>
+      <c r="FY50" s="757"/>
+      <c r="FZ50" s="757"/>
+      <c r="GA50" s="757"/>
+      <c r="GB50" s="757"/>
+      <c r="GC50" s="757"/>
+      <c r="GD50" s="757"/>
+      <c r="GE50" s="757"/>
+      <c r="GF50" s="757"/>
+      <c r="GG50" s="757"/>
+      <c r="GH50" s="757"/>
+      <c r="GI50" s="757"/>
+      <c r="GJ50" s="757"/>
+      <c r="GK50" s="757"/>
+      <c r="GL50" s="757"/>
+      <c r="GM50" s="757"/>
+      <c r="GN50" s="757"/>
+      <c r="GO50" s="757"/>
+      <c r="GP50" s="757"/>
+      <c r="GQ50" s="757"/>
+      <c r="GR50" s="757"/>
+      <c r="GS50" s="757"/>
+      <c r="GT50" s="757"/>
+      <c r="GU50" s="757"/>
+      <c r="GV50" s="757"/>
+      <c r="GW50" s="757"/>
+      <c r="GX50" s="757"/>
+      <c r="GY50" s="757"/>
+      <c r="GZ50" s="757"/>
+      <c r="HA50" s="757"/>
+      <c r="HB50" s="757"/>
+      <c r="HC50" s="757"/>
+      <c r="HD50" s="757"/>
+      <c r="HE50" s="757"/>
+      <c r="HF50" s="757"/>
+      <c r="HG50" s="757"/>
+      <c r="HH50" s="757"/>
+      <c r="HI50" s="757"/>
+      <c r="HJ50" s="757"/>
+      <c r="HK50" s="757"/>
+      <c r="HL50" s="757"/>
+      <c r="HM50" s="757"/>
+      <c r="HN50" s="757"/>
+      <c r="HO50" s="757"/>
+      <c r="HP50" s="757"/>
+      <c r="HQ50" s="757"/>
+      <c r="HR50" s="757"/>
+      <c r="HS50" s="757"/>
+      <c r="HT50" s="757"/>
+      <c r="HU50" s="757"/>
+      <c r="HV50" s="757"/>
+      <c r="HW50" s="757"/>
+      <c r="HX50" s="757"/>
+      <c r="HY50" s="757"/>
+      <c r="HZ50" s="757"/>
+      <c r="IA50" s="757"/>
+      <c r="IB50" s="757"/>
+      <c r="IC50" s="757"/>
+      <c r="ID50" s="757"/>
+      <c r="IE50" s="757"/>
+      <c r="IF50" s="757"/>
+      <c r="IG50" s="757"/>
+      <c r="IH50" s="757"/>
+      <c r="II50" s="757"/>
+      <c r="IJ50" s="757"/>
+      <c r="IK50" s="757"/>
+      <c r="IL50" s="757"/>
+      <c r="IM50" s="757"/>
+      <c r="IN50" s="757"/>
+      <c r="IO50" s="757"/>
+      <c r="IP50" s="757"/>
+      <c r="IQ50" s="757"/>
+      <c r="IR50" s="757"/>
+      <c r="IS50" s="757"/>
+      <c r="IT50" s="757"/>
+      <c r="IU50" s="757"/>
+      <c r="IV50" s="757"/>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="521" t="n">
+        <v>47</v>
+      </c>
+      <c r="C51" s="521" t="s">
+        <v>472</v>
+      </c>
+      <c r="E51" s="521" t="s">
+        <v>399</v>
+      </c>
+      <c r="F51" s="521" t="s">
+        <v>473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bugs. add some new skills
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -21,14 +21,14 @@
   </definedNames>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="pm" day="1486539213" val="694"/>
+      <pm:revision xmlns:pm="pm" day="1486614118" val="694"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="475">
   <si>
     <t>武器等级</t>
   </si>
@@ -1424,13 +1424,16 @@
     <t>降龙</t>
   </si>
   <si>
-    <t>战斗期间敌人基础防御力减少90%</t>
+    <t>特殊技</t>
+  </si>
+  <si>
+    <t>敌我双方所有触发技无效</t>
   </si>
   <si>
     <t>伏虎</t>
   </si>
   <si>
-    <t>战斗期间敌人基础攻击力减少90%</t>
+    <t>敌我双方所有锁定技无效</t>
   </si>
   <si>
     <t>巨化I</t>
@@ -39967,7 +39970,7 @@
   <dimension ref="A4:IV51"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A27" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.50"/>
@@ -41638,7 +41641,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="44" spans="1:256" s="758" customFormat="1">
+    <row r="44" spans="1:256" s="522" customFormat="1">
       <c r="A44" s="757"/>
       <c r="B44" s="757" t="n">
         <v>40</v>
@@ -41926,10 +41929,10 @@
         <v>462</v>
       </c>
       <c r="E46" s="521" t="s">
-        <v>399</v>
+        <v>463</v>
       </c>
       <c r="F46" s="521" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="47" spans="2:6" s="521" customFormat="1">
@@ -41937,29 +41940,29 @@
         <v>43</v>
       </c>
       <c r="C47" s="521" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E47" s="521" t="s">
-        <v>399</v>
+        <v>463</v>
       </c>
       <c r="F47" s="521" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="48" spans="1:256" s="758" customFormat="1">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="48" spans="1:256" s="522" customFormat="1">
       <c r="A48" s="757"/>
       <c r="B48" s="757" t="n">
         <v>44</v>
       </c>
       <c r="C48" s="757" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D48" s="757"/>
       <c r="E48" s="757" t="s">
         <v>399</v>
       </c>
       <c r="F48" s="757" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="G48" s="757"/>
       <c r="H48" s="757"/>
@@ -42212,20 +42215,20 @@
       <c r="IU48" s="757"/>
       <c r="IV48" s="757"/>
     </row>
-    <row r="49" spans="1:256" s="758" customFormat="1">
+    <row r="49" spans="1:256" s="522" customFormat="1">
       <c r="A49" s="757"/>
       <c r="B49" s="757" t="n">
         <v>45</v>
       </c>
       <c r="C49" s="757" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D49" s="757"/>
       <c r="E49" s="757" t="s">
         <v>399</v>
       </c>
       <c r="F49" s="757" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="G49" s="757"/>
       <c r="H49" s="757"/>
@@ -42478,20 +42481,20 @@
       <c r="IU49" s="757"/>
       <c r="IV49" s="757"/>
     </row>
-    <row r="50" spans="1:256" s="758" customFormat="1">
+    <row r="50" spans="1:256" s="522" customFormat="1">
       <c r="A50" s="757"/>
       <c r="B50" s="757" t="n">
         <v>46</v>
       </c>
       <c r="C50" s="757" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D50" s="757"/>
       <c r="E50" s="757" t="s">
         <v>399</v>
       </c>
       <c r="F50" s="757" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="G50" s="757"/>
       <c r="H50" s="757"/>
@@ -42744,19 +42747,271 @@
       <c r="IU50" s="757"/>
       <c r="IV50" s="757"/>
     </row>
-    <row r="51" spans="2:6">
-      <c r="B51" s="521" t="n">
+    <row r="51" spans="1:256" s="758" customFormat="1">
+      <c r="A51" s="757"/>
+      <c r="B51" s="757" t="n">
         <v>47</v>
       </c>
-      <c r="C51" s="521" t="s">
-        <v>472</v>
-      </c>
-      <c r="E51" s="521" t="s">
+      <c r="C51" s="757" t="s">
+        <v>473</v>
+      </c>
+      <c r="D51" s="757"/>
+      <c r="E51" s="757" t="s">
         <v>399</v>
       </c>
-      <c r="F51" s="521" t="s">
-        <v>473</v>
-      </c>
+      <c r="F51" s="757" t="s">
+        <v>474</v>
+      </c>
+      <c r="G51" s="757"/>
+      <c r="H51" s="757"/>
+      <c r="I51" s="757"/>
+      <c r="J51" s="757"/>
+      <c r="K51" s="757"/>
+      <c r="L51" s="757"/>
+      <c r="M51" s="757"/>
+      <c r="N51" s="757"/>
+      <c r="O51" s="757"/>
+      <c r="P51" s="757"/>
+      <c r="Q51" s="757"/>
+      <c r="R51" s="757"/>
+      <c r="S51" s="757"/>
+      <c r="T51" s="757"/>
+      <c r="U51" s="757"/>
+      <c r="V51" s="757"/>
+      <c r="W51" s="757"/>
+      <c r="X51" s="757"/>
+      <c r="Y51" s="757"/>
+      <c r="Z51" s="757"/>
+      <c r="AA51" s="757"/>
+      <c r="AB51" s="757"/>
+      <c r="AC51" s="757"/>
+      <c r="AD51" s="757"/>
+      <c r="AE51" s="757"/>
+      <c r="AF51" s="757"/>
+      <c r="AG51" s="757"/>
+      <c r="AH51" s="757"/>
+      <c r="AI51" s="757"/>
+      <c r="AJ51" s="757"/>
+      <c r="AK51" s="757"/>
+      <c r="AL51" s="757"/>
+      <c r="AM51" s="757"/>
+      <c r="AN51" s="757"/>
+      <c r="AO51" s="757"/>
+      <c r="AP51" s="757"/>
+      <c r="AQ51" s="757"/>
+      <c r="AR51" s="757"/>
+      <c r="AS51" s="757"/>
+      <c r="AT51" s="757"/>
+      <c r="AU51" s="757"/>
+      <c r="AV51" s="757"/>
+      <c r="AW51" s="757"/>
+      <c r="AX51" s="757"/>
+      <c r="AY51" s="757"/>
+      <c r="AZ51" s="757"/>
+      <c r="BA51" s="757"/>
+      <c r="BB51" s="757"/>
+      <c r="BC51" s="757"/>
+      <c r="BD51" s="757"/>
+      <c r="BE51" s="757"/>
+      <c r="BF51" s="757"/>
+      <c r="BG51" s="757"/>
+      <c r="BH51" s="757"/>
+      <c r="BI51" s="757"/>
+      <c r="BJ51" s="757"/>
+      <c r="BK51" s="757"/>
+      <c r="BL51" s="757"/>
+      <c r="BM51" s="757"/>
+      <c r="BN51" s="757"/>
+      <c r="BO51" s="757"/>
+      <c r="BP51" s="757"/>
+      <c r="BQ51" s="757"/>
+      <c r="BR51" s="757"/>
+      <c r="BS51" s="757"/>
+      <c r="BT51" s="757"/>
+      <c r="BU51" s="757"/>
+      <c r="BV51" s="757"/>
+      <c r="BW51" s="757"/>
+      <c r="BX51" s="757"/>
+      <c r="BY51" s="757"/>
+      <c r="BZ51" s="757"/>
+      <c r="CA51" s="757"/>
+      <c r="CB51" s="757"/>
+      <c r="CC51" s="757"/>
+      <c r="CD51" s="757"/>
+      <c r="CE51" s="757"/>
+      <c r="CF51" s="757"/>
+      <c r="CG51" s="757"/>
+      <c r="CH51" s="757"/>
+      <c r="CI51" s="757"/>
+      <c r="CJ51" s="757"/>
+      <c r="CK51" s="757"/>
+      <c r="CL51" s="757"/>
+      <c r="CM51" s="757"/>
+      <c r="CN51" s="757"/>
+      <c r="CO51" s="757"/>
+      <c r="CP51" s="757"/>
+      <c r="CQ51" s="757"/>
+      <c r="CR51" s="757"/>
+      <c r="CS51" s="757"/>
+      <c r="CT51" s="757"/>
+      <c r="CU51" s="757"/>
+      <c r="CV51" s="757"/>
+      <c r="CW51" s="757"/>
+      <c r="CX51" s="757"/>
+      <c r="CY51" s="757"/>
+      <c r="CZ51" s="757"/>
+      <c r="DA51" s="757"/>
+      <c r="DB51" s="757"/>
+      <c r="DC51" s="757"/>
+      <c r="DD51" s="757"/>
+      <c r="DE51" s="757"/>
+      <c r="DF51" s="757"/>
+      <c r="DG51" s="757"/>
+      <c r="DH51" s="757"/>
+      <c r="DI51" s="757"/>
+      <c r="DJ51" s="757"/>
+      <c r="DK51" s="757"/>
+      <c r="DL51" s="757"/>
+      <c r="DM51" s="757"/>
+      <c r="DN51" s="757"/>
+      <c r="DO51" s="757"/>
+      <c r="DP51" s="757"/>
+      <c r="DQ51" s="757"/>
+      <c r="DR51" s="757"/>
+      <c r="DS51" s="757"/>
+      <c r="DT51" s="757"/>
+      <c r="DU51" s="757"/>
+      <c r="DV51" s="757"/>
+      <c r="DW51" s="757"/>
+      <c r="DX51" s="757"/>
+      <c r="DY51" s="757"/>
+      <c r="DZ51" s="757"/>
+      <c r="EA51" s="757"/>
+      <c r="EB51" s="757"/>
+      <c r="EC51" s="757"/>
+      <c r="ED51" s="757"/>
+      <c r="EE51" s="757"/>
+      <c r="EF51" s="757"/>
+      <c r="EG51" s="757"/>
+      <c r="EH51" s="757"/>
+      <c r="EI51" s="757"/>
+      <c r="EJ51" s="757"/>
+      <c r="EK51" s="757"/>
+      <c r="EL51" s="757"/>
+      <c r="EM51" s="757"/>
+      <c r="EN51" s="757"/>
+      <c r="EO51" s="757"/>
+      <c r="EP51" s="757"/>
+      <c r="EQ51" s="757"/>
+      <c r="ER51" s="757"/>
+      <c r="ES51" s="757"/>
+      <c r="ET51" s="757"/>
+      <c r="EU51" s="757"/>
+      <c r="EV51" s="757"/>
+      <c r="EW51" s="757"/>
+      <c r="EX51" s="757"/>
+      <c r="EY51" s="757"/>
+      <c r="EZ51" s="757"/>
+      <c r="FA51" s="757"/>
+      <c r="FB51" s="757"/>
+      <c r="FC51" s="757"/>
+      <c r="FD51" s="757"/>
+      <c r="FE51" s="757"/>
+      <c r="FF51" s="757"/>
+      <c r="FG51" s="757"/>
+      <c r="FH51" s="757"/>
+      <c r="FI51" s="757"/>
+      <c r="FJ51" s="757"/>
+      <c r="FK51" s="757"/>
+      <c r="FL51" s="757"/>
+      <c r="FM51" s="757"/>
+      <c r="FN51" s="757"/>
+      <c r="FO51" s="757"/>
+      <c r="FP51" s="757"/>
+      <c r="FQ51" s="757"/>
+      <c r="FR51" s="757"/>
+      <c r="FS51" s="757"/>
+      <c r="FT51" s="757"/>
+      <c r="FU51" s="757"/>
+      <c r="FV51" s="757"/>
+      <c r="FW51" s="757"/>
+      <c r="FX51" s="757"/>
+      <c r="FY51" s="757"/>
+      <c r="FZ51" s="757"/>
+      <c r="GA51" s="757"/>
+      <c r="GB51" s="757"/>
+      <c r="GC51" s="757"/>
+      <c r="GD51" s="757"/>
+      <c r="GE51" s="757"/>
+      <c r="GF51" s="757"/>
+      <c r="GG51" s="757"/>
+      <c r="GH51" s="757"/>
+      <c r="GI51" s="757"/>
+      <c r="GJ51" s="757"/>
+      <c r="GK51" s="757"/>
+      <c r="GL51" s="757"/>
+      <c r="GM51" s="757"/>
+      <c r="GN51" s="757"/>
+      <c r="GO51" s="757"/>
+      <c r="GP51" s="757"/>
+      <c r="GQ51" s="757"/>
+      <c r="GR51" s="757"/>
+      <c r="GS51" s="757"/>
+      <c r="GT51" s="757"/>
+      <c r="GU51" s="757"/>
+      <c r="GV51" s="757"/>
+      <c r="GW51" s="757"/>
+      <c r="GX51" s="757"/>
+      <c r="GY51" s="757"/>
+      <c r="GZ51" s="757"/>
+      <c r="HA51" s="757"/>
+      <c r="HB51" s="757"/>
+      <c r="HC51" s="757"/>
+      <c r="HD51" s="757"/>
+      <c r="HE51" s="757"/>
+      <c r="HF51" s="757"/>
+      <c r="HG51" s="757"/>
+      <c r="HH51" s="757"/>
+      <c r="HI51" s="757"/>
+      <c r="HJ51" s="757"/>
+      <c r="HK51" s="757"/>
+      <c r="HL51" s="757"/>
+      <c r="HM51" s="757"/>
+      <c r="HN51" s="757"/>
+      <c r="HO51" s="757"/>
+      <c r="HP51" s="757"/>
+      <c r="HQ51" s="757"/>
+      <c r="HR51" s="757"/>
+      <c r="HS51" s="757"/>
+      <c r="HT51" s="757"/>
+      <c r="HU51" s="757"/>
+      <c r="HV51" s="757"/>
+      <c r="HW51" s="757"/>
+      <c r="HX51" s="757"/>
+      <c r="HY51" s="757"/>
+      <c r="HZ51" s="757"/>
+      <c r="IA51" s="757"/>
+      <c r="IB51" s="757"/>
+      <c r="IC51" s="757"/>
+      <c r="ID51" s="757"/>
+      <c r="IE51" s="757"/>
+      <c r="IF51" s="757"/>
+      <c r="IG51" s="757"/>
+      <c r="IH51" s="757"/>
+      <c r="II51" s="757"/>
+      <c r="IJ51" s="757"/>
+      <c r="IK51" s="757"/>
+      <c r="IL51" s="757"/>
+      <c r="IM51" s="757"/>
+      <c r="IN51" s="757"/>
+      <c r="IO51" s="757"/>
+      <c r="IP51" s="757"/>
+      <c r="IQ51" s="757"/>
+      <c r="IR51" s="757"/>
+      <c r="IS51" s="757"/>
+      <c r="IT51" s="757"/>
+      <c r="IU51" s="757"/>
+      <c r="IV51" s="757"/>
     </row>
   </sheetData>
   <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>

</xml_diff>

<commit_message>
fix bugs, add new skill
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -21,7 +21,7 @@
   </definedNames>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="pm" day="1486707921" val="694"/>
+      <pm:revision xmlns:pm="pm" day="1486889229" val="694"/>
     </ext>
   </extLst>
 </workbook>
@@ -1224,7 +1224,7 @@
     <t>攻击时50%几率造成虚弱，持续5秒，对方物理伤害和攻击减少20%</t>
   </si>
   <si>
-    <t>祝福</t>
+    <t>祝福I</t>
   </si>
   <si>
     <t>锁定技</t>
@@ -1248,8 +1248,8 @@
     <t>反转</t>
   </si>
   <si>
-    <t>若角色力量小于对方则物理伤害、生命恢复增加百分比为两者力量差百分比的200%；
-若角色敏捷小于对方则攻击速度、防御力增加百分比为两者敏捷差百分比的200%。</t>
+    <t>若角色力量小于对方则物理伤害、生命恢复增加百分比为两者力量差百分比的300%；
+若角色敏捷小于对方则攻击速度、防御力增加百分比为两者敏捷差百分比的300%。</t>
   </si>
   <si>
     <t>不屈</t>
@@ -1306,7 +1306,7 @@
     <t>角色攻击速度提升100%</t>
   </si>
   <si>
-    <t>顽强</t>
+    <t>顽强I</t>
   </si>
   <si>
     <t>生命恢复速度提升百分比为失去生命百分比的150%</t>
@@ -1345,7 +1345,7 @@
     <t>嗜血</t>
   </si>
   <si>
-    <t>攻击速度和物理伤害提升百分比为失去生命百分比的25%</t>
+    <t>攻击速度提升百分比为失去生命的100%，物理伤害提升百分比为失去生命百分比的50%</t>
   </si>
   <si>
     <t>狂暴</t>
@@ -1376,19 +1376,19 @@
     <t>冰冻I</t>
   </si>
   <si>
-    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少40%，持续5秒，不可叠加</t>
+    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少30%，持续5秒，不可叠加</t>
   </si>
   <si>
     <t>冰冻II</t>
   </si>
   <si>
-    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少60%，持续7秒，不可叠加</t>
+    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少50%，持续7秒，不可叠加</t>
   </si>
   <si>
     <t>冰冻III</t>
   </si>
   <si>
-    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少80%，持续15秒，不可叠加</t>
+    <t>角色每次攻击命中会造成冷冻效果；对方攻速减少70%，持续15秒，不可叠加</t>
   </si>
   <si>
     <t>复仇</t>
@@ -1439,19 +1439,19 @@
     <t>巨化I</t>
   </si>
   <si>
-    <t>每次攻击必暴击，攻速减慢20%</t>
+    <t>每次攻击必暴击，攻速减慢10%</t>
   </si>
   <si>
     <t>巨化II</t>
   </si>
   <si>
-    <t>每次攻击必暴击，生命生命恢复+100%，攻速减慢30%</t>
+    <t>每次攻击必暴击，生命生命恢复+100%，攻速减慢15%</t>
   </si>
   <si>
     <t>巨化III</t>
   </si>
   <si>
-    <t>每次攻击必暴击，生命生命恢复+100%，生命最大值+100%，攻速减慢40%</t>
+    <t>每次攻击必暴击，生命生命恢复+100%，生命最大值+100%，攻速减慢20%</t>
   </si>
   <si>
     <t>必中</t>
@@ -39969,8 +39969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:IV51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A9" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A19" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.50"/>
@@ -41123,7 +41123,7 @@
       </c>
       <c r="G26" s="524"/>
     </row>
-    <row r="27" spans="1:256" s="758" customFormat="1">
+    <row r="27" spans="1:256" s="522" customFormat="1">
       <c r="A27" s="757"/>
       <c r="B27" s="525" t="n">
         <v>23</v>
@@ -41389,7 +41389,7 @@
       <c r="IU27" s="757"/>
       <c r="IV27" s="757"/>
     </row>
-    <row r="28" spans="1:256" s="758" customFormat="1">
+    <row r="28" spans="1:256" s="522" customFormat="1">
       <c r="A28" s="757"/>
       <c r="B28" s="525" t="n">
         <v>24</v>
@@ -41655,7 +41655,7 @@
       <c r="IU28" s="757"/>
       <c r="IV28" s="757"/>
     </row>
-    <row r="29" spans="1:256" s="758" customFormat="1">
+    <row r="29" spans="1:256" s="522" customFormat="1">
       <c r="A29" s="757"/>
       <c r="B29" s="525" t="n">
         <v>25</v>
@@ -41969,21 +41969,271 @@
       </c>
       <c r="G32" s="525"/>
     </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="524" t="n">
+    <row r="33" spans="1:256" s="758" customFormat="1">
+      <c r="A33" s="757"/>
+      <c r="B33" s="525" t="n">
         <v>29</v>
       </c>
-      <c r="C33" s="524" t="s">
+      <c r="C33" s="525" t="s">
         <v>436</v>
       </c>
-      <c r="D33" s="524"/>
-      <c r="E33" s="524" t="s">
+      <c r="D33" s="525"/>
+      <c r="E33" s="525" t="s">
         <v>399</v>
       </c>
-      <c r="F33" s="524" t="s">
+      <c r="F33" s="525" t="s">
         <v>437</v>
       </c>
-      <c r="G33" s="524"/>
+      <c r="G33" s="525"/>
+      <c r="H33" s="757"/>
+      <c r="I33" s="757"/>
+      <c r="J33" s="757"/>
+      <c r="K33" s="757"/>
+      <c r="L33" s="757"/>
+      <c r="M33" s="757"/>
+      <c r="N33" s="757"/>
+      <c r="O33" s="757"/>
+      <c r="P33" s="757"/>
+      <c r="Q33" s="757"/>
+      <c r="R33" s="757"/>
+      <c r="S33" s="757"/>
+      <c r="T33" s="757"/>
+      <c r="U33" s="757"/>
+      <c r="V33" s="757"/>
+      <c r="W33" s="757"/>
+      <c r="X33" s="757"/>
+      <c r="Y33" s="757"/>
+      <c r="Z33" s="757"/>
+      <c r="AA33" s="757"/>
+      <c r="AB33" s="757"/>
+      <c r="AC33" s="757"/>
+      <c r="AD33" s="757"/>
+      <c r="AE33" s="757"/>
+      <c r="AF33" s="757"/>
+      <c r="AG33" s="757"/>
+      <c r="AH33" s="757"/>
+      <c r="AI33" s="757"/>
+      <c r="AJ33" s="757"/>
+      <c r="AK33" s="757"/>
+      <c r="AL33" s="757"/>
+      <c r="AM33" s="757"/>
+      <c r="AN33" s="757"/>
+      <c r="AO33" s="757"/>
+      <c r="AP33" s="757"/>
+      <c r="AQ33" s="757"/>
+      <c r="AR33" s="757"/>
+      <c r="AS33" s="757"/>
+      <c r="AT33" s="757"/>
+      <c r="AU33" s="757"/>
+      <c r="AV33" s="757"/>
+      <c r="AW33" s="757"/>
+      <c r="AX33" s="757"/>
+      <c r="AY33" s="757"/>
+      <c r="AZ33" s="757"/>
+      <c r="BA33" s="757"/>
+      <c r="BB33" s="757"/>
+      <c r="BC33" s="757"/>
+      <c r="BD33" s="757"/>
+      <c r="BE33" s="757"/>
+      <c r="BF33" s="757"/>
+      <c r="BG33" s="757"/>
+      <c r="BH33" s="757"/>
+      <c r="BI33" s="757"/>
+      <c r="BJ33" s="757"/>
+      <c r="BK33" s="757"/>
+      <c r="BL33" s="757"/>
+      <c r="BM33" s="757"/>
+      <c r="BN33" s="757"/>
+      <c r="BO33" s="757"/>
+      <c r="BP33" s="757"/>
+      <c r="BQ33" s="757"/>
+      <c r="BR33" s="757"/>
+      <c r="BS33" s="757"/>
+      <c r="BT33" s="757"/>
+      <c r="BU33" s="757"/>
+      <c r="BV33" s="757"/>
+      <c r="BW33" s="757"/>
+      <c r="BX33" s="757"/>
+      <c r="BY33" s="757"/>
+      <c r="BZ33" s="757"/>
+      <c r="CA33" s="757"/>
+      <c r="CB33" s="757"/>
+      <c r="CC33" s="757"/>
+      <c r="CD33" s="757"/>
+      <c r="CE33" s="757"/>
+      <c r="CF33" s="757"/>
+      <c r="CG33" s="757"/>
+      <c r="CH33" s="757"/>
+      <c r="CI33" s="757"/>
+      <c r="CJ33" s="757"/>
+      <c r="CK33" s="757"/>
+      <c r="CL33" s="757"/>
+      <c r="CM33" s="757"/>
+      <c r="CN33" s="757"/>
+      <c r="CO33" s="757"/>
+      <c r="CP33" s="757"/>
+      <c r="CQ33" s="757"/>
+      <c r="CR33" s="757"/>
+      <c r="CS33" s="757"/>
+      <c r="CT33" s="757"/>
+      <c r="CU33" s="757"/>
+      <c r="CV33" s="757"/>
+      <c r="CW33" s="757"/>
+      <c r="CX33" s="757"/>
+      <c r="CY33" s="757"/>
+      <c r="CZ33" s="757"/>
+      <c r="DA33" s="757"/>
+      <c r="DB33" s="757"/>
+      <c r="DC33" s="757"/>
+      <c r="DD33" s="757"/>
+      <c r="DE33" s="757"/>
+      <c r="DF33" s="757"/>
+      <c r="DG33" s="757"/>
+      <c r="DH33" s="757"/>
+      <c r="DI33" s="757"/>
+      <c r="DJ33" s="757"/>
+      <c r="DK33" s="757"/>
+      <c r="DL33" s="757"/>
+      <c r="DM33" s="757"/>
+      <c r="DN33" s="757"/>
+      <c r="DO33" s="757"/>
+      <c r="DP33" s="757"/>
+      <c r="DQ33" s="757"/>
+      <c r="DR33" s="757"/>
+      <c r="DS33" s="757"/>
+      <c r="DT33" s="757"/>
+      <c r="DU33" s="757"/>
+      <c r="DV33" s="757"/>
+      <c r="DW33" s="757"/>
+      <c r="DX33" s="757"/>
+      <c r="DY33" s="757"/>
+      <c r="DZ33" s="757"/>
+      <c r="EA33" s="757"/>
+      <c r="EB33" s="757"/>
+      <c r="EC33" s="757"/>
+      <c r="ED33" s="757"/>
+      <c r="EE33" s="757"/>
+      <c r="EF33" s="757"/>
+      <c r="EG33" s="757"/>
+      <c r="EH33" s="757"/>
+      <c r="EI33" s="757"/>
+      <c r="EJ33" s="757"/>
+      <c r="EK33" s="757"/>
+      <c r="EL33" s="757"/>
+      <c r="EM33" s="757"/>
+      <c r="EN33" s="757"/>
+      <c r="EO33" s="757"/>
+      <c r="EP33" s="757"/>
+      <c r="EQ33" s="757"/>
+      <c r="ER33" s="757"/>
+      <c r="ES33" s="757"/>
+      <c r="ET33" s="757"/>
+      <c r="EU33" s="757"/>
+      <c r="EV33" s="757"/>
+      <c r="EW33" s="757"/>
+      <c r="EX33" s="757"/>
+      <c r="EY33" s="757"/>
+      <c r="EZ33" s="757"/>
+      <c r="FA33" s="757"/>
+      <c r="FB33" s="757"/>
+      <c r="FC33" s="757"/>
+      <c r="FD33" s="757"/>
+      <c r="FE33" s="757"/>
+      <c r="FF33" s="757"/>
+      <c r="FG33" s="757"/>
+      <c r="FH33" s="757"/>
+      <c r="FI33" s="757"/>
+      <c r="FJ33" s="757"/>
+      <c r="FK33" s="757"/>
+      <c r="FL33" s="757"/>
+      <c r="FM33" s="757"/>
+      <c r="FN33" s="757"/>
+      <c r="FO33" s="757"/>
+      <c r="FP33" s="757"/>
+      <c r="FQ33" s="757"/>
+      <c r="FR33" s="757"/>
+      <c r="FS33" s="757"/>
+      <c r="FT33" s="757"/>
+      <c r="FU33" s="757"/>
+      <c r="FV33" s="757"/>
+      <c r="FW33" s="757"/>
+      <c r="FX33" s="757"/>
+      <c r="FY33" s="757"/>
+      <c r="FZ33" s="757"/>
+      <c r="GA33" s="757"/>
+      <c r="GB33" s="757"/>
+      <c r="GC33" s="757"/>
+      <c r="GD33" s="757"/>
+      <c r="GE33" s="757"/>
+      <c r="GF33" s="757"/>
+      <c r="GG33" s="757"/>
+      <c r="GH33" s="757"/>
+      <c r="GI33" s="757"/>
+      <c r="GJ33" s="757"/>
+      <c r="GK33" s="757"/>
+      <c r="GL33" s="757"/>
+      <c r="GM33" s="757"/>
+      <c r="GN33" s="757"/>
+      <c r="GO33" s="757"/>
+      <c r="GP33" s="757"/>
+      <c r="GQ33" s="757"/>
+      <c r="GR33" s="757"/>
+      <c r="GS33" s="757"/>
+      <c r="GT33" s="757"/>
+      <c r="GU33" s="757"/>
+      <c r="GV33" s="757"/>
+      <c r="GW33" s="757"/>
+      <c r="GX33" s="757"/>
+      <c r="GY33" s="757"/>
+      <c r="GZ33" s="757"/>
+      <c r="HA33" s="757"/>
+      <c r="HB33" s="757"/>
+      <c r="HC33" s="757"/>
+      <c r="HD33" s="757"/>
+      <c r="HE33" s="757"/>
+      <c r="HF33" s="757"/>
+      <c r="HG33" s="757"/>
+      <c r="HH33" s="757"/>
+      <c r="HI33" s="757"/>
+      <c r="HJ33" s="757"/>
+      <c r="HK33" s="757"/>
+      <c r="HL33" s="757"/>
+      <c r="HM33" s="757"/>
+      <c r="HN33" s="757"/>
+      <c r="HO33" s="757"/>
+      <c r="HP33" s="757"/>
+      <c r="HQ33" s="757"/>
+      <c r="HR33" s="757"/>
+      <c r="HS33" s="757"/>
+      <c r="HT33" s="757"/>
+      <c r="HU33" s="757"/>
+      <c r="HV33" s="757"/>
+      <c r="HW33" s="757"/>
+      <c r="HX33" s="757"/>
+      <c r="HY33" s="757"/>
+      <c r="HZ33" s="757"/>
+      <c r="IA33" s="757"/>
+      <c r="IB33" s="757"/>
+      <c r="IC33" s="757"/>
+      <c r="ID33" s="757"/>
+      <c r="IE33" s="757"/>
+      <c r="IF33" s="757"/>
+      <c r="IG33" s="757"/>
+      <c r="IH33" s="757"/>
+      <c r="II33" s="757"/>
+      <c r="IJ33" s="757"/>
+      <c r="IK33" s="757"/>
+      <c r="IL33" s="757"/>
+      <c r="IM33" s="757"/>
+      <c r="IN33" s="757"/>
+      <c r="IO33" s="757"/>
+      <c r="IP33" s="757"/>
+      <c r="IQ33" s="757"/>
+      <c r="IR33" s="757"/>
+      <c r="IS33" s="757"/>
+      <c r="IT33" s="757"/>
+      <c r="IU33" s="757"/>
+      <c r="IV33" s="757"/>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="524" t="n">
@@ -42671,7 +42921,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="46" spans="1:256" s="757" customFormat="1">
+    <row r="46" spans="2:6" s="757" customFormat="1">
       <c r="B46" s="757" t="n">
         <v>42</v>
       </c>
@@ -42685,7 +42935,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="47" spans="1:256" s="757" customFormat="1">
+    <row r="47" spans="2:6" s="757" customFormat="1">
       <c r="B47" s="757" t="n">
         <v>43</v>
       </c>
@@ -43497,7 +43747,7 @@
       <c r="IU50" s="757"/>
       <c r="IV50" s="757"/>
     </row>
-    <row r="51" spans="1:256" s="758" customFormat="1">
+    <row r="51" spans="1:256" s="522" customFormat="1">
       <c r="A51" s="757"/>
       <c r="B51" s="757" t="n">
         <v>47</v>

</xml_diff>

<commit_message>
new skill, new price
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -21,14 +21,14 @@
   </definedNames>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="pm" day="1491977578" val="694"/>
+      <pm:revision xmlns:pm="pm" day="1496519572" val="694"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="487">
   <si>
     <t>武器等级</t>
   </si>
@@ -1327,19 +1327,19 @@
     <t>坚守I</t>
   </si>
   <si>
-    <t>防御提升百分比为失去生命百分比的40%</t>
+    <t>防御提升百分比为失去生命百分比的100%</t>
   </si>
   <si>
     <t>坚守II</t>
   </si>
   <si>
-    <t>防御提升百分比为失去生命百分比的80%</t>
+    <t>防御提升百分比为失去生命百分比的200%</t>
   </si>
   <si>
     <t>坚守III</t>
   </si>
   <si>
-    <t>防御提升百分比为失去生命百分比的160%</t>
+    <t>防御提升百分比为失去生命百分比的400%</t>
   </si>
   <si>
     <t>嗜血</t>
@@ -1476,6 +1476,24 @@
   </si>
   <si>
     <t>攻速+100%，防御-50%</t>
+  </si>
+  <si>
+    <t>勇猛I</t>
+  </si>
+  <si>
+    <t>被暴击后，攻击+50%，物理伤害+50%，持续5秒</t>
+  </si>
+  <si>
+    <t>勇猛II</t>
+  </si>
+  <si>
+    <t>被暴击后，攻击+100%，物理伤害+100%，持续10秒</t>
+  </si>
+  <si>
+    <t>勇猛III</t>
+  </si>
+  <si>
+    <t>被暴击后，攻击+200%，物理伤害+200%，持续20秒</t>
   </si>
 </sst>
 </file>
@@ -39937,10 +39955,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:IV55"/>
+  <dimension ref="A4:IV57"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A25" zoomScale="115" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.50"/>
@@ -44025,9 +44043,46 @@
         <v>480</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
+    <row r="55" spans="2:6">
       <c r="B55" s="521" t="n">
         <v>51</v>
+      </c>
+      <c r="C55" s="521" t="s">
+        <v>481</v>
+      </c>
+      <c r="E55" s="521" t="s">
+        <v>379</v>
+      </c>
+      <c r="F55" s="521" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="521" t="n">
+        <v>52</v>
+      </c>
+      <c r="C56" s="521" t="s">
+        <v>483</v>
+      </c>
+      <c r="E56" s="521" t="s">
+        <v>379</v>
+      </c>
+      <c r="F56" s="521" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="521" t="n">
+        <v>53</v>
+      </c>
+      <c r="C57" s="521" t="s">
+        <v>485</v>
+      </c>
+      <c r="E57" s="521" t="s">
+        <v>379</v>
+      </c>
+      <c r="F57" s="521" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix equips and consults
</commit_message>
<xml_diff>
--- a/装备列表.xlsx
+++ b/装备列表.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="524">
   <si>
     <t>武器等级</t>
   </si>
@@ -1412,15 +1412,6 @@
     <t>铜头</t>
   </si>
   <si>
-    <t>角色不会受到暴击伤害</t>
-  </si>
-  <si>
-    <t>铁壁</t>
-  </si>
-  <si>
-    <t>角色每次攻击必定造成暴击</t>
-  </si>
-  <si>
     <t>降龙</t>
   </si>
   <si>
@@ -1439,19 +1430,10 @@
     <t>巨化I</t>
   </si>
   <si>
-    <t>每次攻击必暴击，攻速减慢10%</t>
-  </si>
-  <si>
     <t>巨化II</t>
   </si>
   <si>
-    <t>每次攻击必暴击，生命恢复+100%，攻速减慢15%</t>
-  </si>
-  <si>
     <t>巨化III</t>
-  </si>
-  <si>
-    <t>每次攻击必暴击，生命恢复+100%，生命最大值+100%，攻速减慢20%</t>
   </si>
   <si>
     <t>必中</t>
@@ -1539,6 +1521,126 @@
   </si>
   <si>
     <t>汲血III</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血I</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血II</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血III</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发技</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击造成伤害后将30%转化为自己生命</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击造成伤害后将50%转化为自己生命</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击造成伤害后将70%转化为自己生命</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴戾I</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴戾II</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴戾III</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>锁定技</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>33%几率造成3倍伤害</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>33%几率造成5倍伤害</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>33%几率造成7被伤害</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>狙击II</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>狙击I</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>狙击III</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴击时造成的伤害X1.5</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴击时造成的伤害X2.5</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴击时造成的伤害X4</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>回光</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>返照</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命小于25%时将生命值翻转，180秒冷却时间</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命大于25%时恢复速度X300%</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁臂</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色受到暴击时与普通攻击伤害相同</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次攻击若命中必暴击，攻速减慢20%</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次攻击若命中必暴击，生命恢复+200%，攻速减慢40%</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次攻击若命中必暴击，生命恢复+400%，生命最大值+200%，攻速减慢60%</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>当攻击和物理伤害均高于对手时，每次攻击若命中必定造成暴击</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
@@ -1547,14 +1649,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="184" formatCode="0_ "/>
-    <numFmt numFmtId="185" formatCode="0.0_ "/>
-    <numFmt numFmtId="186" formatCode="#,##0_ "/>
-    <numFmt numFmtId="187" formatCode="#,##0.0_ "/>
-    <numFmt numFmtId="188" formatCode="0.000_ "/>
-    <numFmt numFmtId="189" formatCode="#,##0;[Red]#,##0"/>
-    <numFmt numFmtId="190" formatCode="#,##0_);[Red]\(#,##0\)"/>
-    <numFmt numFmtId="191" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="0.0_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0_ "/>
+    <numFmt numFmtId="179" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="180" formatCode="0.000_ "/>
+    <numFmt numFmtId="181" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="182" formatCode="#,##0_);[Red]\(#,##0\)"/>
+    <numFmt numFmtId="183" formatCode="0.0"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -7007,14 +7109,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="103" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="184" fontId="4" fillId="22" borderId="21" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="184" fontId="3" fillId="35" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="184" fontId="3" fillId="16" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="184" fontId="4" fillId="37" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="184" fontId="3" fillId="40" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="184" fontId="4" fillId="19" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="184" fontId="4" fillId="103" borderId="104" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="184" fontId="1" fillId="0" borderId="105" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="4" fillId="22" borderId="21" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="3" fillId="35" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="3" fillId="16" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="4" fillId="37" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="3" fillId="40" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="4" fillId="19" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="4" fillId="103" borderId="104" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="105" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="104" borderId="106" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -7071,11 +7173,11 @@
     <xf numFmtId="0" fontId="4" fillId="130" borderId="136" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="131" borderId="137" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="132" borderId="138" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="185" fontId="4" fillId="122" borderId="128" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="185" fontId="4" fillId="124" borderId="130" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="185" fontId="4" fillId="129" borderId="135" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="185" fontId="3" fillId="131" borderId="137" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="127" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="4" fillId="122" borderId="128" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="4" fillId="124" borderId="130" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="4" fillId="129" borderId="135" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="3" fillId="131" borderId="137" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="127" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="133" borderId="139" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="134" borderId="140" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="135" borderId="141" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -7090,75 +7192,75 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="150" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="151" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="143" borderId="152" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="144" borderId="153" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="35" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="26" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="16" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="40" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="2" fillId="13" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="144" borderId="153" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="35" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="26" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="16" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="40" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="2" fillId="13" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="145" borderId="154" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="146" borderId="155" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="156" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="21" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="157" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="25" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="15" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="68" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="36" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="43" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="39" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="77" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="147" borderId="158" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="18" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="148" borderId="159" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="85" borderId="84" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="156" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="20" borderId="19" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="33" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="24" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="14" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="67" borderId="66" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="38" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="28" borderId="27" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="41" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="76" borderId="75" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="143" borderId="152" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="17" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="149" borderId="160" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="84" borderId="83" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="2" fillId="23" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="7" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="8" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="11" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="10" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="75" borderId="74" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="81" borderId="80" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="150" borderId="161" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="151" borderId="162" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="89" borderId="88" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="163" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="109" borderId="112" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="111" borderId="114" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="152" borderId="165" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="113" borderId="116" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="153" borderId="166" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="120" borderId="125" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="154" borderId="167" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="116" borderId="119" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="155" borderId="168" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="156" borderId="169" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="117" borderId="120" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="157" borderId="170" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="158" borderId="171" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="2" fillId="159" borderId="172" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="21" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="157" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="25" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="15" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="68" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="36" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="43" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="39" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="77" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="147" borderId="158" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="18" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="148" borderId="159" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="85" borderId="84" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="156" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="20" borderId="19" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="33" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="24" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="14" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="67" borderId="66" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="38" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="28" borderId="27" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="41" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="76" borderId="75" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="143" borderId="152" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="17" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="149" borderId="160" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="84" borderId="83" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="2" fillId="23" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="7" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="11" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="10" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="75" borderId="74" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="81" borderId="80" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="150" borderId="161" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="151" borderId="162" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="89" borderId="88" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="163" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="109" borderId="112" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="111" borderId="114" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="152" borderId="165" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="113" borderId="116" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="153" borderId="166" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="120" borderId="125" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="154" borderId="167" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="116" borderId="119" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="155" borderId="168" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="156" borderId="169" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="117" borderId="120" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="157" borderId="170" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="158" borderId="171" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="2" fillId="159" borderId="172" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="160" borderId="173" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="161" borderId="174" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="162" borderId="175" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -7177,88 +7279,88 @@
     <xf numFmtId="0" fontId="4" fillId="174" borderId="187" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="175" borderId="188" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="176" borderId="189" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="177" borderId="190" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="174" borderId="187" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="178" borderId="191" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="177" borderId="190" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="174" borderId="187" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="178" borderId="191" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="179" borderId="192" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="180" borderId="193" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="180" borderId="193" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="194" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="181" borderId="195" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="182" borderId="196" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="182" borderId="196" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="181" borderId="195" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="183" borderId="197" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="184" borderId="198" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="182" borderId="196" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="181" borderId="195" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="183" borderId="197" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="184" borderId="198" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="185" borderId="199" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="186" borderId="200" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="185" borderId="199" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="187" borderId="201" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="188" borderId="202" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="189" borderId="203" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="29" borderId="28" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="33" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="41" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="2" fillId="23" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="145" borderId="154" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="30" borderId="29" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="190" borderId="204" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="21" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="48" borderId="47" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="31" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="47" borderId="46" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="46" borderId="45" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="119" borderId="122" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="60" borderId="59" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="191" borderId="205" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="4" fillId="7" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="192" borderId="206" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="193" borderId="207" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="194" borderId="208" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="195" borderId="209" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="196" borderId="210" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="197" borderId="211" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="198" borderId="212" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="199" borderId="213" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="200" borderId="214" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="50" borderId="49" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="35" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="49" borderId="48" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="111" borderId="114" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="8" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="201" borderId="215" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="202" borderId="216" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="203" borderId="217" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="204" borderId="218" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="205" borderId="219" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="206" borderId="220" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="207" borderId="221" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="208" borderId="222" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="209" borderId="223" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="210" borderId="224" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="211" borderId="225" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="212" borderId="226" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="213" borderId="227" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="138" borderId="144" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="39" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="56" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="40" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="55" borderId="54" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="116" borderId="119" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="214" borderId="228" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="215" borderId="229" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="216" borderId="230" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="217" borderId="231" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="3" fillId="218" borderId="232" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="2" fillId="219" borderId="233" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="2" fillId="62" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="2" fillId="13" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="2" fillId="61" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="187" fontId="2" fillId="159" borderId="172" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="186" borderId="200" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="185" borderId="199" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="187" borderId="201" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="188" borderId="202" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="189" borderId="203" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="29" borderId="28" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="33" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="41" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="2" fillId="23" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="145" borderId="154" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="30" borderId="29" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="190" borderId="204" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="21" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="48" borderId="47" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="31" borderId="30" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="47" borderId="46" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="46" borderId="45" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="119" borderId="122" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="60" borderId="59" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="191" borderId="205" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="4" fillId="7" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="192" borderId="206" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="193" borderId="207" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="194" borderId="208" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="195" borderId="209" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="196" borderId="210" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="197" borderId="211" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="198" borderId="212" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="199" borderId="213" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="200" borderId="214" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="50" borderId="49" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="35" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="49" borderId="48" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="111" borderId="114" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="8" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="201" borderId="215" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="202" borderId="216" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="203" borderId="217" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="204" borderId="218" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="205" borderId="219" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="206" borderId="220" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="207" borderId="221" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="208" borderId="222" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="209" borderId="223" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="210" borderId="224" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="211" borderId="225" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="212" borderId="226" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="213" borderId="227" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="138" borderId="144" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="39" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="56" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="40" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="55" borderId="54" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="116" borderId="119" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="214" borderId="228" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="215" borderId="229" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="216" borderId="230" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="217" borderId="231" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="3" fillId="218" borderId="232" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="2" fillId="219" borderId="233" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="2" fillId="62" borderId="61" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="2" fillId="13" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="2" fillId="61" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="2" fillId="159" borderId="172" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="103" borderId="104" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="120" borderId="125" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="121" borderId="126" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -7278,65 +7380,65 @@
     <xf numFmtId="0" fontId="3" fillId="224" borderId="238" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="225" borderId="239" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="226" borderId="240" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="188" fontId="4" fillId="221" borderId="235" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="188" fontId="3" fillId="226" borderId="240" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="188" fontId="4" fillId="227" borderId="241" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="180" fontId="4" fillId="221" borderId="235" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="180" fontId="3" fillId="226" borderId="240" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="180" fontId="4" fillId="227" borderId="241" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="228" borderId="242" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="229" borderId="243" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="144" borderId="153" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="230" borderId="244" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="35" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="231" borderId="245" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="26" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="232" borderId="246" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="16" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="231" borderId="245" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="69" borderId="68" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="233" borderId="247" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="37" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="231" borderId="245" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="234" borderId="248" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="235" borderId="249" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="72" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="232" borderId="246" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="40" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="231" borderId="245" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="236" borderId="250" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="235" borderId="249" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="78" borderId="77" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="233" borderId="247" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="237" borderId="251" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="232" borderId="246" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="19" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="231" borderId="245" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="238" borderId="252" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="235" borderId="249" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="22" borderId="21" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="231" borderId="245" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="239" borderId="253" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="240" borderId="254" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="4" fillId="86" borderId="85" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="2" fillId="13" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="189" fontId="2" fillId="231" borderId="245" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="145" borderId="154" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="200" borderId="214" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="241" borderId="255" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="242" borderId="256" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="243" borderId="257" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="137" borderId="143" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="221" borderId="235" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="244" borderId="258" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="138" borderId="144" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="245" borderId="259" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="246" borderId="260" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="247" borderId="261" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="248" borderId="262" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="227" borderId="241" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="249" borderId="263" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="250" borderId="264" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="251" borderId="265" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="2" fillId="219" borderId="233" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="144" borderId="153" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="230" borderId="244" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="35" borderId="34" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="231" borderId="245" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="26" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="232" borderId="246" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="16" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="231" borderId="245" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="69" borderId="68" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="233" borderId="247" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="37" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="231" borderId="245" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="234" borderId="248" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="235" borderId="249" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="72" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="232" borderId="246" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="40" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="231" borderId="245" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="236" borderId="250" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="235" borderId="249" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="78" borderId="77" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="233" borderId="247" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="237" borderId="251" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="232" borderId="246" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="19" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="231" borderId="245" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="238" borderId="252" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="235" borderId="249" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="22" borderId="21" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="231" borderId="245" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="239" borderId="253" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="240" borderId="254" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="4" fillId="86" borderId="85" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="2" fillId="13" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="181" fontId="2" fillId="231" borderId="245" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="145" borderId="154" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="200" borderId="214" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="241" borderId="255" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="242" borderId="256" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="243" borderId="257" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="137" borderId="143" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="221" borderId="235" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="244" borderId="258" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="138" borderId="144" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="245" borderId="259" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="246" borderId="260" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="247" borderId="261" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="248" borderId="262" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="227" borderId="241" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="249" borderId="263" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="250" borderId="264" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="251" borderId="265" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="2" fillId="219" borderId="233" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="252" borderId="266" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="170" borderId="183" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="253" borderId="267" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -7347,58 +7449,58 @@
     <xf numFmtId="0" fontId="3" fillId="200" borderId="214" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="256" borderId="270" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="257" borderId="271" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="97" borderId="96" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="37" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="236" borderId="250" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="103" borderId="104" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="234" borderId="248" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="78" borderId="77" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="72" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="258" borderId="272" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="97" borderId="96" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="37" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="236" borderId="250" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="103" borderId="104" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="234" borderId="248" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="78" borderId="77" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="72" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="258" borderId="272" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="259" borderId="273" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="260" borderId="274" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="261" borderId="275" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="262" borderId="276" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="263" borderId="277" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="105" borderId="108" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="106" borderId="109" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="264" borderId="278" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="265" borderId="279" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="266" borderId="280" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="101" borderId="100" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="107" borderId="110" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="252" borderId="266" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="222" borderId="236" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="160" borderId="173" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="102" borderId="102" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="220" borderId="234" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="267" borderId="281" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="268" borderId="282" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="176" borderId="189" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="223" borderId="237" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="2" fillId="140" borderId="146" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="4" fillId="269" borderId="283" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="270" borderId="284" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="3" fillId="226" borderId="240" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="186" fontId="2" fillId="271" borderId="285" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="4" fillId="21" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="1" fillId="0" borderId="157" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="3" fillId="25" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="3" fillId="15" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="3" fillId="68" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="4" fillId="36" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="4" fillId="177" borderId="190" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="3" fillId="43" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="3" fillId="39" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="3" fillId="182" borderId="196" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="3" fillId="77" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="4" fillId="147" borderId="158" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="4" fillId="18" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="4" fillId="186" borderId="200" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="4" fillId="148" borderId="159" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="4" fillId="85" borderId="84" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="260" borderId="274" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="261" borderId="275" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="262" borderId="276" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="263" borderId="277" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="105" borderId="108" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="106" borderId="109" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="264" borderId="278" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="265" borderId="279" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="266" borderId="280" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="101" borderId="100" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="107" borderId="110" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="252" borderId="266" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="222" borderId="236" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="160" borderId="173" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="102" borderId="102" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="220" borderId="234" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="267" borderId="281" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="268" borderId="282" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="176" borderId="189" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="223" borderId="237" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="2" fillId="140" borderId="146" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="4" fillId="269" borderId="283" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="270" borderId="284" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="3" fillId="226" borderId="240" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="2" fillId="271" borderId="285" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="4" fillId="21" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="157" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="3" fillId="25" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="3" fillId="15" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="3" fillId="68" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="4" fillId="36" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="4" fillId="177" borderId="190" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="3" fillId="43" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="3" fillId="39" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="3" fillId="182" borderId="196" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="3" fillId="77" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="4" fillId="147" borderId="158" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="4" fillId="18" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="4" fillId="186" borderId="200" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="4" fillId="148" borderId="159" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="4" fillId="85" borderId="84" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7549,38 +7651,38 @@
     <xf numFmtId="1" fontId="4" fillId="109" borderId="112" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="4" fillId="285" borderId="299" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="4" fillId="158" borderId="171" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="2" fillId="23" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="29" borderId="28" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="44" borderId="43" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="33" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="24" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="14" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="67" borderId="66" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="27" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="38" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="96" borderId="95" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="28" borderId="27" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="41" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="76" borderId="75" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="17" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="20" borderId="19" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="84" borderId="83" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="30" borderId="29" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="42" borderId="41" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="25" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="15" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="68" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="45" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="36" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="101" borderId="100" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="43" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="39" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="77" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="18" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="21" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="85" borderId="84" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="2" fillId="23" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="29" borderId="28" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="44" borderId="43" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="33" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="24" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="14" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="67" borderId="66" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="27" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="38" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="96" borderId="95" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="28" borderId="27" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="41" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="76" borderId="75" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="17" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="20" borderId="19" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="84" borderId="83" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="30" borderId="29" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="42" borderId="41" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="34" borderId="33" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="25" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="15" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="68" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="45" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="36" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="101" borderId="100" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="43" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="39" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="77" borderId="76" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="18" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="21" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="85" borderId="84" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="2" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="4" fillId="30" borderId="29" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="3" fillId="42" borderId="41" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -7614,24 +7716,24 @@
     <xf numFmtId="1" fontId="4" fillId="82" borderId="81" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="4" fillId="59" borderId="58" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="4" fillId="87" borderId="86" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="9" borderId="8" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="66" borderId="65" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="8" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="11" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="10" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="93" borderId="92" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="98" borderId="97" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="75" borderId="74" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="3" fillId="81" borderId="80" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="32" borderId="31" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="7" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="89" borderId="88" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="191" fontId="4" fillId="46" borderId="45" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="9" borderId="8" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="66" borderId="65" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="8" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="11" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="10" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="93" borderId="92" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="98" borderId="97" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="75" borderId="74" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="5" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="3" fillId="81" borderId="80" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="32" borderId="31" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="7" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="89" borderId="88" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="4" fillId="46" borderId="45" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -17264,7 +17366,7 @@
         <v>117200</v>
       </c>
       <c r="E66" s="152">
-        <f t="shared" ref="E66:E97" si="32">D66+I66*14</f>
+        <f t="shared" ref="E66:E68" si="32">D66+I66*14</f>
         <v>146684</v>
       </c>
       <c r="F66" s="162">
@@ -17276,7 +17378,7 @@
         <v>33</v>
       </c>
       <c r="H66" s="157">
-        <f t="shared" ref="H66:H97" si="33">G66+16</f>
+        <f t="shared" ref="H66:H68" si="33">G66+16</f>
         <v>49</v>
       </c>
       <c r="I66" s="157">
@@ -17292,7 +17394,7 @@
         <v>129</v>
       </c>
       <c r="L66" s="157">
-        <f t="shared" ref="L66:L97" si="34">K66+15</f>
+        <f t="shared" ref="L66:L68" si="34">K66+15</f>
         <v>144</v>
       </c>
       <c r="M66" s="157">
@@ -17326,7 +17428,7 @@
         <v>3450</v>
       </c>
       <c r="D67" s="153">
-        <f t="shared" ref="D67:D98" si="35">D66+C67</f>
+        <f t="shared" ref="D67:D68" si="35">D66+C67</f>
         <v>120650</v>
       </c>
       <c r="E67" s="152">
@@ -17366,7 +17468,7 @@
         <v>5200</v>
       </c>
       <c r="N67" s="157">
-        <f t="shared" ref="N67:N98" si="36">M67/2</f>
+        <f t="shared" ref="N67:N68" si="36">M67/2</f>
         <v>2600</v>
       </c>
       <c r="O67" s="157">
@@ -24313,7 +24415,7 @@
         <v>1516729.1400142098</v>
       </c>
       <c r="O37" s="100">
-        <f t="shared" ref="O37:O68" si="52">O35+1</f>
+        <f t="shared" ref="O37:O66" si="52">O35+1</f>
         <v>18</v>
       </c>
       <c r="P37" s="433">
@@ -27916,7 +28018,7 @@
         <v>70</v>
       </c>
       <c r="I66" s="408">
-        <f t="shared" ref="I66:I97" si="54">G66*H66</f>
+        <f t="shared" ref="I66" si="54">G66*H66</f>
         <v>114688000</v>
       </c>
       <c r="J66" s="449">
@@ -37168,7 +37270,7 @@
         <v>1</v>
       </c>
       <c r="E260" s="363">
-        <f t="shared" ref="E260:E323" si="24">MAX(3*(C260-D260)/C260,-0.5)</f>
+        <f t="shared" ref="E260:E278" si="24">MAX(3*(C260-D260)/C260,-0.5)</f>
         <v>2.4163424124513591</v>
       </c>
       <c r="H260" s="356">
@@ -37179,7 +37281,7 @@
         <v>1</v>
       </c>
       <c r="J260" s="362">
-        <f t="shared" ref="J260:J323" si="25">MAX((H260-I260)/H260,-1)</f>
+        <f t="shared" ref="J260:J278" si="25">MAX((H260-I260)/H260,-1)</f>
         <v>0.80544747081711976</v>
       </c>
       <c r="M260" s="356">
@@ -37190,7 +37292,7 @@
         <v>1</v>
       </c>
       <c r="O260" s="362">
-        <f t="shared" ref="O260:O323" si="26">MAX(0.4*(M260-N260)/M260,-0.4)</f>
+        <f t="shared" ref="O260:O278" si="26">MAX(0.4*(M260-N260)/M260,-0.4)</f>
         <v>0.32217898832684794</v>
       </c>
     </row>
@@ -39347,10 +39449,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:IV63"/>
+  <dimension ref="A4:IV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -42034,7 +42136,7 @@
         <v>399</v>
       </c>
       <c r="F44" s="707" t="s">
-        <v>459</v>
+        <v>519</v>
       </c>
       <c r="G44" s="707"/>
       <c r="H44" s="707"/>
@@ -42292,13 +42394,13 @@
         <v>41</v>
       </c>
       <c r="C45" s="483" t="s">
-        <v>460</v>
+        <v>518</v>
       </c>
       <c r="E45" s="483" t="s">
         <v>399</v>
       </c>
       <c r="F45" s="483" t="s">
-        <v>461</v>
+        <v>523</v>
       </c>
     </row>
     <row r="46" spans="1:256" s="707" customFormat="1">
@@ -42306,13 +42408,13 @@
         <v>42</v>
       </c>
       <c r="C46" s="707" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E46" s="707" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F46" s="707" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="47" spans="1:256" s="707" customFormat="1">
@@ -42320,13 +42422,13 @@
         <v>43</v>
       </c>
       <c r="C47" s="707" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="E47" s="707" t="s">
+        <v>460</v>
+      </c>
+      <c r="F47" s="707" t="s">
         <v>463</v>
-      </c>
-      <c r="F47" s="707" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="48" spans="1:256" s="484" customFormat="1">
@@ -42335,14 +42437,14 @@
         <v>44</v>
       </c>
       <c r="C48" s="707" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D48" s="707"/>
       <c r="E48" s="707" t="s">
         <v>399</v>
       </c>
       <c r="F48" s="707" t="s">
-        <v>468</v>
+        <v>520</v>
       </c>
       <c r="G48" s="707"/>
       <c r="H48" s="707"/>
@@ -42601,14 +42703,14 @@
         <v>45</v>
       </c>
       <c r="C49" s="707" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D49" s="707"/>
       <c r="E49" s="707" t="s">
         <v>399</v>
       </c>
       <c r="F49" s="707" t="s">
-        <v>470</v>
+        <v>521</v>
       </c>
       <c r="G49" s="707"/>
       <c r="H49" s="707"/>
@@ -42867,14 +42969,14 @@
         <v>46</v>
       </c>
       <c r="C50" s="707" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D50" s="707"/>
       <c r="E50" s="707" t="s">
         <v>399</v>
       </c>
       <c r="F50" s="707" t="s">
-        <v>472</v>
+        <v>522</v>
       </c>
       <c r="G50" s="707"/>
       <c r="H50" s="707"/>
@@ -43133,14 +43235,14 @@
         <v>47</v>
       </c>
       <c r="C51" s="707" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="D51" s="707"/>
       <c r="E51" s="707" t="s">
         <v>399</v>
       </c>
       <c r="F51" s="707" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="G51" s="707"/>
       <c r="H51" s="707"/>
@@ -43398,13 +43500,13 @@
         <v>48</v>
       </c>
       <c r="C52" s="483" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="E52" s="483" t="s">
         <v>399</v>
       </c>
       <c r="F52" s="483" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="53" spans="1:256">
@@ -43412,13 +43514,13 @@
         <v>49</v>
       </c>
       <c r="C53" s="483" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="E53" s="483" t="s">
         <v>399</v>
       </c>
       <c r="F53" s="483" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="54" spans="1:256">
@@ -43426,13 +43528,13 @@
         <v>50</v>
       </c>
       <c r="C54" s="483" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="E54" s="483" t="s">
         <v>399</v>
       </c>
       <c r="F54" s="483" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="55" spans="1:256">
@@ -43440,14 +43542,14 @@
         <v>51</v>
       </c>
       <c r="C55" s="708" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="D55" s="708"/>
       <c r="E55" s="708" t="s">
         <v>379</v>
       </c>
       <c r="F55" s="708" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="56" spans="1:256">
@@ -43455,14 +43557,14 @@
         <v>52</v>
       </c>
       <c r="C56" s="708" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="D56" s="708"/>
       <c r="E56" s="708" t="s">
         <v>379</v>
       </c>
       <c r="F56" s="708" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="57" spans="1:256">
@@ -43470,14 +43572,14 @@
         <v>53</v>
       </c>
       <c r="C57" s="708" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="D57" s="708"/>
       <c r="E57" s="708" t="s">
         <v>379</v>
       </c>
       <c r="F57" s="708" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="58" spans="1:256">
@@ -43485,13 +43587,13 @@
         <v>54</v>
       </c>
       <c r="C58" s="483" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="E58" s="483" t="s">
         <v>379</v>
       </c>
       <c r="F58" s="483" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="59" spans="1:256">
@@ -43499,13 +43601,13 @@
         <v>55</v>
       </c>
       <c r="C59" s="483" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="E59" s="483" t="s">
         <v>379</v>
       </c>
       <c r="F59" s="483" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="60" spans="1:256">
@@ -43513,13 +43615,13 @@
         <v>56</v>
       </c>
       <c r="C60" s="483" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="E60" s="483" t="s">
         <v>379</v>
       </c>
       <c r="F60" s="483" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="61" spans="1:256">
@@ -43527,14 +43629,14 @@
         <v>57</v>
       </c>
       <c r="C61" s="708" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="D61" s="708"/>
       <c r="E61" s="708" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="F61" s="708" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="62" spans="1:256">
@@ -43542,14 +43644,14 @@
         <v>58</v>
       </c>
       <c r="C62" s="708" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="D62" s="708"/>
       <c r="E62" s="708" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="F62" s="708" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="63" spans="1:256">
@@ -43557,14 +43659,168 @@
         <v>59</v>
       </c>
       <c r="C63" s="708" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D63" s="708"/>
       <c r="E63" s="708" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="F63" s="708" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="64" spans="1:256">
+      <c r="B64" s="483">
+        <v>60</v>
+      </c>
+      <c r="C64" s="483" t="s">
+        <v>494</v>
+      </c>
+      <c r="E64" s="483" t="s">
+        <v>497</v>
+      </c>
+      <c r="F64" s="483" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="483">
+        <v>61</v>
+      </c>
+      <c r="C65" s="483" t="s">
         <v>495</v>
+      </c>
+      <c r="E65" s="483" t="s">
+        <v>497</v>
+      </c>
+      <c r="F65" s="483" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" s="483">
+        <v>62</v>
+      </c>
+      <c r="C66" s="483" t="s">
+        <v>496</v>
+      </c>
+      <c r="E66" s="483" t="s">
+        <v>497</v>
+      </c>
+      <c r="F66" s="483" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="483">
+        <v>63</v>
+      </c>
+      <c r="C67" s="483" t="s">
+        <v>501</v>
+      </c>
+      <c r="E67" s="483" t="s">
+        <v>504</v>
+      </c>
+      <c r="F67" s="483" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="483">
+        <v>64</v>
+      </c>
+      <c r="C68" s="483" t="s">
+        <v>502</v>
+      </c>
+      <c r="E68" s="483" t="s">
+        <v>504</v>
+      </c>
+      <c r="F68" s="483" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" s="483">
+        <v>65</v>
+      </c>
+      <c r="C69" s="483" t="s">
+        <v>503</v>
+      </c>
+      <c r="E69" s="483" t="s">
+        <v>504</v>
+      </c>
+      <c r="F69" s="483" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="483">
+        <v>66</v>
+      </c>
+      <c r="C70" s="483" t="s">
+        <v>509</v>
+      </c>
+      <c r="E70" s="483" t="s">
+        <v>497</v>
+      </c>
+      <c r="F70" s="483" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="483">
+        <v>67</v>
+      </c>
+      <c r="C71" s="483" t="s">
+        <v>508</v>
+      </c>
+      <c r="E71" s="483" t="s">
+        <v>497</v>
+      </c>
+      <c r="F71" s="483" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" s="483">
+        <v>68</v>
+      </c>
+      <c r="C72" s="483" t="s">
+        <v>510</v>
+      </c>
+      <c r="E72" s="483" t="s">
+        <v>497</v>
+      </c>
+      <c r="F72" s="483" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="483">
+        <v>69</v>
+      </c>
+      <c r="C73" s="483" t="s">
+        <v>514</v>
+      </c>
+      <c r="E73" s="483" t="s">
+        <v>504</v>
+      </c>
+      <c r="F73" s="483" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="483">
+        <v>70</v>
+      </c>
+      <c r="C74" s="483" t="s">
+        <v>515</v>
+      </c>
+      <c r="E74" s="483" t="s">
+        <v>497</v>
+      </c>
+      <c r="F74" s="483" t="s">
+        <v>516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>